<commit_message>
update wos exports to 450
</commit_message>
<xml_diff>
--- a/derived/science_geo/prep_wos_exports/output/wos_scijrnls_queries.xlsx
+++ b/derived/science_geo/prep_wos_exports/output/wos_scijrnls_queries.xlsx
@@ -13,15 +13,93 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>PMID=(1281416 OR 1281417 OR 1281418 OR 1281419 OR 1281420 OR 1309646 OR 1309647 OR 1309648 OR 1309649 OR 1309650 OR 1309651 OR 1309652 OR 1310861 OR 1310862 OR 1310863 OR 1310864 OR 1310865 OR 1312848 OR 1312849 OR 1314616 OR 1314617 OR 1314618 OR 1314619 OR 1314621 OR 1314622 OR 1314623 OR 1314624 OR 1316763 OR 1316764 OR 1316765 OR 1316767 OR 1319183 OR 1319184 OR 1319185 OR 1319186 OR 1321644 OR 1321645 OR 1321646 OR 1321647 OR 1321648 OR 1323309 OR 1323310 OR 1323312 OR 1323313 OR 1323314 OR 1326294 OR 1326295 OR 1326296 OR 1326297 OR 1327011 OR 1329864 OR 1334418 OR 1334419 OR 1334420 OR 1334421 OR 1334422 OR 1345671 OR 1346089 OR 1346090 OR 1346742 OR 1347996 OR 1347997 OR 1348949 OR 1348950 OR 1348951 OR 1350203 OR 1351731 OR 1351732 OR 1351733 OR 1352982 OR 1352983 OR 1352984 OR 1352985 OR 1352986 OR 1352987 OR 1355977 OR 1356370 OR 1356372 OR 1356373 OR 1361128 OR 1361129 OR 1370371 OR 1370372 OR 1370374 OR 1371216 OR 1371217 OR 1371218 OR 1371219 OR 1371220 OR 1372510 OR 1375036 OR 1375038 OR 1375039 OR 1376999 OR 1379820 OR 1379821 OR 1381926 OR 1382471 OR 1382472 OR 1382473 OR 1382474 OR 1382475 OR 1384575 OR 1384576 OR 1384577 OR 1384578 OR 1385966 OR 1388031 OR 1389179 OR 1389180 OR 1389181 OR 1389182 OR 1389183 OR 1389184 OR 1389185 OR 1418995 OR 1418996 OR 1418997 OR 1418998 OR 1418999 OR 1419000 OR 1419001 OR 1419002 OR 1419003 OR 1419004 OR 1463605 OR 1463606 OR 1463607 OR 1463608 OR 1463609 OR 1463610 OR 1497890 OR 1497891 OR 1497892 OR 1497893 OR 1497894 OR 1497895 OR 1497896 OR 1497897 OR 1497898 OR 1524823 OR 1524824 OR 1524825 OR 1524826 OR 1524827 OR 1524828 OR 1524829 OR 1524830 OR 1524831 OR 1530909 OR 1531415 OR 1532320 OR 1534012 OR 1550669 OR 1550670 OR 1550671 OR 1550672 OR 1550673 OR 1550674 OR 1550675 OR 1550677 OR 1550678 OR 1550679 OR 1567620 OR 1567621 OR 1567622 OR 1586486 OR 1586488 OR 1610562 OR 1610563 OR 1610564 OR 1610565 OR 1610566 OR 1610567 OR 1610568 OR 1610569 OR 1610570 OR 1632965 OR 1632966 OR 1632967 OR 1632968 OR 1632969 OR 1647174 OR 1647175 OR 1647176 OR 1648935 OR 1648937 OR 1648938 OR 1648939 OR 1648940 OR 1648941 OR 1654946 OR 1654948 OR 1654949 OR 1654950 OR 1654951 OR 1657055 OR 1657056 OR 1657057 OR 1657058 OR 1660283 OR 1660284 OR 1660285 OR 1660286 OR 1662517 OR 1662518 OR 1662519 OR 1662520 OR 1670919 OR 1670920 OR 1670921 OR 1670922 OR 1672071 OR 1672072 OR 1673055 OR 1673849 OR 1673850 OR 1673851 OR 1675862 OR 1675863 OR 1675864 OR 1676893 OR 1676894 OR 1676895 OR 1678612 OR 1678613 OR 1678615 OR 1681831 OR 1681832 OR 1681833 OR 1684900 OR 1684902 OR 1684903 OR 1689586 OR 1690014 OR 1690015 OR 1690016 OR 1690017 OR 1690562 OR 1690563 OR 1690564 OR 1690566 OR 1690567 OR 1690568 OR 1691005 OR 1691006 OR 1693086 OR 1694444 OR 1694445 OR 1694446 OR 1698395 OR 1698396 OR 1698397 OR 1699567 OR 1699568 OR 1699569 OR 1702643 OR 1702645 OR 1702647 OR 1702648 OR 1702650 OR 1702651 OR 1704243 OR 1704244 OR 1705807 OR 1705808 OR 1709023 OR 1709024 OR 1709025 OR 1711347 OR 1711348 OR 1711349 OR 1712602 OR 1712603 OR 1712604 OR 1714745 OR 1716928 OR 1716929 OR 1716930 OR 1718333 OR 1718334 OR 1718335 OR 1720625 OR 1722411 OR 1722412 OR 1722413 OR 1730003 OR 1730004 OR 1730005 OR 1739459 OR 1739460 OR 1739461 OR 1739462 OR 1739463 OR 1742020 OR 1742021 OR 1742022 OR 1742023 OR 1742024 OR 1742025 OR 1742026 OR 1742027 OR 1742028 OR 1764241 OR 1764242 OR 1764243 OR 1764244 OR 1764245 OR 1764246 OR 1764247 OR 1824753 OR 1825171 OR 1825782 OR 1826603 OR 1827266 OR 1829904 OR 1832879 OR 1840649 OR 1846075 OR 1846076 OR 1847064 OR 1847065 OR 1848078 OR 1848081 OR 1848082 OR 1848083 OR 1849721 OR 1849722 OR 1849723 OR 1849724 OR 1849725 OR 1851019 OR 1873027 OR 1873028 OR 1873029 OR 1873030 OR 1873031 OR 1873032 OR 1873033 OR 1898850 OR 1899580 OR 1899581 OR 1901716 OR 1901717 OR 1901718 OR 1902699 OR 1905146 OR 1908251 OR 1908252 OR 1908253 OR 1910787 OR 1910788 OR 1910790 OR 1931049 OR 1931050 OR 1931051 OR 1931052 OR 1931053 OR 1931054 OR 1968344 OR 1968345 OR 1971515 OR 1972886 OR 1976015 OR 1976320 OR 1976321 OR 1977421 OR 1977422 OR 1980068 OR 1980069 OR 1980070 OR 1986772 OR 1986773 OR 1986774 OR 1993122 OR 1993123 OR 1993124 OR 2001285 OR 2001286 OR 2001287 OR 2015091 OR 2015092 OR 2015093 OR 2015094 OR 2015095 OR 2025425 OR 2025426 OR 2025427 OR 2025428 OR 2025429 OR 2025430 OR 2054187 OR 2069816 OR 2106330 OR 2106331 OR 2106905 OR 2106906 OR 2108708 OR 2111712 OR 2114884 OR 2114885 OR 2116813 OR 2116814 OR 2119630 OR 2119631 OR 2138470 OR 2140514 OR 2145879 OR 2148487 OR 2148489 OR 2155007 OR 2155008 OR 2155009 OR 2155010 OR 2155011 OR 2155629 OR 2155630 OR 2156539 OR 2156540 OR 2156541 OR 2156542 OR 2157470 OR 2157471 OR 2160836 OR 2160837 OR 2160838 OR 2163262 OR 2163263 OR 2164403 OR 2164404 OR 2164405 OR 2166544 OR 2166545 OR 2169265 OR 2169266 OR 2169267 OR 2169268 OR 2169269 OR 2169270 OR 2169271 OR 2169272 OR 2169771 OR 2171589 OR 2171590 OR 2171591 OR 2171592 OR 2176509 OR 2176510 OR 2182078 OR 2182079 OR 2196069 OR 2200448 OR 2200449 OR 2200450 OR 2205251 OR 2206530 OR 2206531 OR 2206532 OR 2206533 OR 2206534 OR 2206535 OR 2223090 OR 2223091 OR 2223092 OR 2223093 OR 2223094 OR 2223095 OR 2268433 OR 2306365 OR 2306366 OR 2310570 OR 2310571 OR 2310572 OR 2310573 OR 2310574 OR 2310575 OR 2317379 OR 2322458 OR 2322459 OR 2322460 OR 2322461 OR 2322462 OR 2322463 OR 2322464 OR 2322465 OR 2344404 OR 2344405 OR 2344406 OR 2344407 OR 2344408 OR 2344409 OR 2344410 OR 2344411 OR 2344412 OR 2361010 OR 2361011 OR 2361012 OR 2361013 OR 2361014 OR 2361016 OR 2369518 OR 2369519 OR 2369520 OR 2369521 OR 2369522 OR 2383398 OR 2383399 OR 2383400 OR 2400604 OR 2400605 OR 2400606 OR 2482777 OR 2482778 OR 2483091 OR 2483092 OR 2483093 OR 2483094 OR 2483095 OR 2483096 OR 2483098 OR 2483099 OR 2483100 OR 2483102 OR 2483103 OR 2483104 OR 2483105 OR 2483106 OR 2483107 OR 2483108 OR 2483111 OR 2483112 OR 2483113 OR 2483323 OR 2483324 OR 2483325 OR 2483327 OR 2484339 OR 2484340 OR 2484341 OR 2484342 OR 2484343 OR 2484345 OR 2484346 OR 2484347 OR 2515889 OR 2516449 OR 2516726 OR 2516728 OR 2518369 OR 2518370 OR 2518371 OR 2518372 OR 2534964 OR 2559758 OR 2559759 OR 2559760 OR 2560386 OR 2560387 OR 2560389 OR 2560390 OR 2560391 OR 2560392 OR 2560393 OR 2560638 OR 2560642 OR 2560645 OR 2560647 OR 2560649 OR 2561968 OR 2561969 OR 2561970 OR 2561971 OR 2561973 OR 2561974 OR 2561975 OR 2561976 OR 2561978 OR 2562784 OR 2576209 OR 2576210 OR 2576211 OR 2576212 OR 2576213 OR 2576215 OR 2576372 OR 2576373 OR 2576374 OR 2576375 OR 2576376 OR 2577128 OR 2577129 OR 2577130 OR 2619993 OR 2619994 OR 2619995 OR 2619996 OR 2619997 OR 2624739 OR 2624741 OR 2624742 OR 2624743 OR 2624744 OR 2624745 OR 2624746 OR 2624747 OR 2624748 OR 2627372 OR 2627375 OR 2627376 OR 2627377 OR 2627378 OR 2627379 OR 2627380 OR 2627381 OR 2641999 OR 2642000 OR 2642001 OR 2642002 OR 2642003 OR 2642004 OR 2642005 OR 2642006 OR 2642007 OR 2642008 OR 2642009 OR 2642010 OR 2642011 OR 2642012 OR 2642013 OR 2642014 OR 2642015 OR 2642016 OR 2642017 OR 2695147 OR 2696501 OR 2696503 OR 2696504 OR 2701844 OR 2701845 OR 2856086 OR 2856087 OR 2856088 OR 2856089 OR 2856090 OR 2856091 OR 2856094 OR 2856095 OR 2856096 OR 2856097 OR 2856098 OR 2856099 OR 2856100 OR 2856101 OR 2856102 OR 2856103 OR 2856104 OR 2856162 OR 2908443 OR 2908444 OR 2908447 OR 2908448 OR 2908449 OR 2908450 OR 2978786 OR 3078411 OR 3078412 OR 3078519 OR 3078520 OR 3152287 OR 3152288 OR 3152289 OR 3152290 OR 3152420 OR 3272153 OR 3272154 OR 3272155 OR 3272156 OR 3272157 OR 3272158 OR 3272159 OR 3272160 OR 3272161 OR 3272163 OR 3272164 OR 3272165 OR 3272166 OR 3272167 OR 3272168 OR 3272169 OR 3272170 OR 3272171 OR 3272172 OR 3272173 OR 3272177 OR 3272178 OR 3272179 OR 3272180 OR 3272181 OR 3272182 OR 3272183 OR 3272184 OR 3272185 OR 3272186 OR 3272187 OR 3272188 OR 3272190 OR 3272191 OR 3272738 OR 3272739 OR 7506045 OR 7506046 OR 7507335 OR 7507336 OR 7507337 OR 7507338 OR 7507339 OR 7507340 OR 7507341 OR 7509160 OR 7509161 OR 7512348 OR 7512349 OR 7512350 OR 7512351 OR 7512352 OR 7512353 OR 7512816 OR 7512817 OR 7514425 OR 7514427 OR 7514428 OR 7516686 OR 7516687 OR 7516688 OR 7516689 OR 7519023 OR 7519024 OR 7519025 OR 7519026 OR 7520251 OR 7520252 OR 7520253 OR 7520255 OR 7520256 OR 7522481 OR 7522482 OR 7522483 OR 7522484 OR 7524558 OR 7524560 OR 7524561 OR 7524562 OR 7524563 OR 7524564 OR 7530017 OR 7530018 OR 7530019 OR 7531985 OR 7531987 OR 7536426 OR 7536427 OR 7538309 OR 7538311 OR 7541630 OR 7541631 OR 7541632 OR 7541633 OR 7541634 OR 7541635 OR 7541636 OR 7542461 OR 7542462 OR 7544139 OR 7544140 OR 7544141 OR 7544142 OR 7546733 OR 7546734 OR 7546735 OR 7546737 OR 7546738 OR 7546740 OR 7546741 OR 7546744 OR 7546745 OR 7546746 OR 7546747 OR 7546748 OR 7546750 OR 7546751 OR 7576625 OR 7576627 OR 7576628 OR 7576629 OR 7576630 OR 7576631 OR 7576632 OR 7576633 OR 7576634 OR 7576635 OR 7576636 OR 7576637 OR 7576638 OR 7576639 OR 7576640 OR 7576641 OR 7576643 OR 7576644 OR 7576646 OR 7576647 OR 7576648 OR 7576649 OR 7576650 OR 7576651 OR 7576652 OR 7576653 OR 7576654 OR 7576655 OR 7576656 OR 7576657 OR 7576658 OR 7576659 OR 7576660 OR 7576661 OR 7576662 OR 7605627 OR 7605629 OR 7605630 OR 7605631 OR 7605632 OR 7605633 OR 7605634 OR 7605635 OR 7605636 OR 7605637 OR 7605638 OR 7605639 OR 7619514 OR 7619516 OR 7619517 OR 7619518 OR 7619519 OR 7619520 OR 7619522 OR 7619523 OR 7619524 OR 7619525 OR 7619526 OR 7619527 OR 7619528 OR 7619529 OR 7619530 OR 7619531 OR 7619532 OR 7619533 OR 7646884 OR 7646885 OR 7646886 OR 7646887 OR 7646888 OR 7646889 OR 7646891 OR 7646892 OR 7646893 OR 7646894 OR 7646895 OR 7646896 OR 7646898 OR 7678964 OR 7678965 OR 7678966 OR 7678967 OR 7679913 OR 7679914 OR 7679915 OR 7681676 OR 7682820 OR 7682821 OR 7684232 OR 7684233 OR 7684234 OR 7684235 OR 7684236 OR 7684237 OR 7686378 OR 7686379 OR 7686380 OR 7686381 OR 7686382 OR 7687849 OR 7688973 OR 7691102 OR 7691103 OR 7691104 OR 7691105 OR 7691106 OR 7694601 OR 7695895 OR 7695897 OR 7695899 OR 7695900 OR 7695901 OR 7695902 OR 7695903 OR 7695904 OR 7695905 OR 7695906 OR 7695907 OR 7695908 OR 7695910 OR 7695911 OR 7695912 OR 7695913 OR 7718230 OR 7718231 OR 7718233 OR 7718234 OR 7718235 OR 7718236 OR 7718237 OR 7718238 OR 7718239 OR 7718241 OR 7718242 OR 7718243 OR 7718244 OR 7718245 OR 7718246 OR 7718248 OR 7718249 OR 7748549 OR 7748550 OR 7748552 OR 7748553 OR 7748554 OR 7748555 OR 7748556 OR 7748558 OR 7748559 OR 7748560 OR 7748561 OR 7748563 OR 7748564 OR 7748565 OR 7748566 OR 7794412 OR 7826629 OR 7826630 OR 7826631 OR 7826632 OR 7826633 OR 7826634 OR 7826635 OR 7826636 OR 7826637 OR 7826638 OR 7826639 OR 7826640 OR 7826641 OR 7826642 OR 7826644 OR 7826645 OR 7857635 OR 7857636 OR 7857640 OR 7857642 OR 7857644 OR 7857645 OR 7857646 OR 7857647 OR 7857648 OR 7857652 OR 7902109 OR 7902110 OR 7903858 OR 7903859 OR 7906528 OR 7906529 OR 7906530 OR 7906531 OR 7909234 OR 7910467 OR 7912090 OR 7912091 OR 7912093 OR 7913820 OR 7917287 OR 7917288 OR 7917289 OR 7917290 OR 7917291 OR 7917292 OR 7917293 OR 7917294 OR 7917295 OR 7917296 OR 7917297 OR 7917298 OR 7917299 OR 7917300 OR 7917301 OR 7917302 OR 7917303 OR 7917304 OR 7946325 OR 7946326 OR 7946329 OR 7946330 OR 7946331 OR 7946332 OR 7946333 OR 7946334 OR 7946335 OR 7946336 OR 7946338 OR 7946339 OR 7946340 OR 7946341 OR 7946344 OR 7946345 OR 7946346 OR 7946347 OR 7946348 OR 7946349 OR 7946350 OR 7946351 OR 7946352 OR 7946355 OR 7946356 OR 7946357 OR 7946358 OR 7946359 OR 7946360 OR 7946361 OR 7993619 OR 7993621 OR 7993622 OR 7993623 OR 7993624 OR 7993626 OR 7993627 OR 7993628 OR 7993629 OR 7993631 OR 7993632 OR 7993633 OR 7993634 OR 7993635 OR 7993636 OR 7993637 OR 7993638 OR 8011334 OR 8011335 OR 8011336 OR 8011340 OR 8043271 OR 8043272 OR 8043274 OR 8043276 OR 8043277 OR 8043278 OR 8043279 OR 8043280 OR 8043281 OR 8043282 OR 8060613 OR 8060614 OR 8060615 OR 8060616 OR 8060617 OR 8060618 OR 8060620 OR 8060621 OR 8060622 OR 8060623 OR 8068082 OR 8080464 OR 8094963 OR 8096385 OR 8097399 OR 8098608 OR 8098609 OR 8098610 OR 8098611 OR 8100427 OR 8101711 OR 8101712 OR 8102532 OR 8102533 OR 8102534 OR 8104431 OR 8104432 OR 8104433 OR 8110456 OR 8110457 OR 8110458 OR 8110459 OR 8110460 OR 8110461 OR 8110462 OR 8110463 OR 8110464 OR 8110465 OR 8110466 OR 8155316 OR 8155317 OR 8155318 OR 8155319 OR 8155320 OR 8155321 OR 8155322 OR 8155323 OR 8155324 OR 8155325 OR 8155326 OR 8161448 OR 8161449 OR 8161450 OR 8161451 OR 8161452 OR 8161453 OR 8161454 OR 8161455 OR 8161456 OR 8161457 OR 8161458 OR 8161459 OR 8161460 OR 8185941 OR 8185942 OR 8185943 OR 8185944 OR 8185947 OR 8185948 OR 8185949 OR 8185950 OR 8185953 OR 8240805 OR 8240806 OR 8240807 OR 8240808 OR 8240809 OR 8240810 OR 8240811 OR 8240812 OR 8240813 OR 8240814 OR 8240815 OR 8240816 OR 8240817 OR 8240818 OR 8240819 OR 8274272 OR 8274274 OR 8274275 OR 8274277 OR 8274278 OR 8274279 OR 8274280 OR 8274281 OR 8274283 OR 8292355 OR 8292356 OR 8292358 OR 8292359 OR 8292360 OR 8292361 OR 8292362 OR 8292363 OR 8318226 OR 8318227 OR 8318228 OR 8318229 OR 8318230 OR 8318231 OR 8318232 OR 8318234 OR 8338662 OR 8338663 OR 8338664 OR 8338665 OR 8338666 OR 8338667 OR 8338668 OR 8338669 OR 8338670 OR 8352940 OR 8352941 OR 8352942 OR 8352943 OR 8352944 OR 8352945 OR 8352946 OR 8381289 OR 8381290 OR 8382496 OR 8382497 OR 8382498 OR 8382499 OR 8382500 OR 8382501 OR 8384857 OR 8384858 OR 8384859 OR 8386524 OR 8386525 OR 8386526 OR 8386527 OR 8386528 OR 8386529 OR 8386530 OR 8386531 OR 8386532 OR 8388224 OR 8388225 OR 8388226 OR 8391279 OR 8391280 OR 8391281 OR 8393322 OR 8393323 OR 8393324 OR 8394719 OR 8394720 OR 8394721 OR 8394722 OR 8394723 OR 8398136 OR 8398137 OR 8398139 OR 8398140 OR 8398141 OR 8398142 OR 8398143 OR 8398144 OR 8398145 OR 8398147 OR 8398149 OR 8398150 OR 8398151 OR 8398152 OR 8398156 OR 8398157 OR 8398158 OR 8427698 OR 8427699 OR 8427700 OR 8427701 OR 8427702 OR 8439408 OR 8439409 OR 8439410 OR 8439411 OR 8439412 OR 8439413 OR 8439414 OR 8461131 OR 8461132 OR 8461133 OR 8461134 OR 8461135 OR 8461136 OR 8461137 OR 8461138 OR 8461139 OR 8461140 OR 8461141 OR 8461142 OR 8476609 OR 8476610 OR 8476611 OR 8476612 OR 8476613 OR 8476614 OR 8494644 OR 8494645 OR 8494646 OR 8494648 OR 8562074 OR 8562075 OR 8562078 OR 8562079 OR 8562080 OR 8562082 OR 8562084 OR 8562085 OR 8562086 OR 8562088 OR 8562089 OR 8562091 OR 8562092 OR 8562093 OR 8562094 OR 8607986 OR 8607991 OR 8607992 OR 8607993 OR 8607995 OR 8607996 OR 8607997 OR 8607998 OR 8607999 OR 8608000 OR 8608001 OR 8608002 OR 8608003 OR 8608004 OR 8608006 OR 8630240 OR 8630241 OR 8630242 OR 8630243 OR 8630246 OR 8630251 OR 8630252 OR 8630253 OR 8630254 OR 8630255 OR 8630256 OR 8630257 OR 8630258 OR 8663985 OR 8663986 OR 8663987 OR 8663988 OR 8663989 OR 8663990 OR 8663991 OR 8663992 OR 8663993 OR 8663994 OR 8663995 OR 8663996 OR 8663997 OR 8663998 OR 8663999 OR 8755474 OR 8755475 OR 8755476 OR 8755477 OR 8755478 OR 8755479 OR 8755480 OR 8755481 OR 8755482 OR 8755483 OR 8755484 OR 8755485 OR 8755486 OR 8755487 OR 8755488 OR 8755489 OR 8780645 OR 8780646 OR 8780647 OR 8780648 OR 8780649 OR 8780651 OR 8780652 OR 8780653 OR 8780654 OR 8780655 OR 8780656 OR 8780657 OR 8780658 OR 8785047 OR 8785048 OR 8785049 OR 8785050 OR 8785051 OR 8785052 OR 8785053 OR 8785054 OR 8785055 OR 8785056 OR 8785057 OR 8785058 OR 8785059 OR 8785060 OR 8785061 OR 8785062 OR 8785063 OR 8785064 OR 8789941 OR 8789943 OR 8789944 OR 8789945 OR 8789946 OR 8789947 OR 8789948 OR 8789949 OR 8789950 OR 8789952 OR 8789953 OR 8789954 OR 8789955 OR 8789956 OR 8789957 OR 8789958 OR 8789959 OR 8789960 OR 8816703 OR 8816704 OR 8816705 OR 8816706 OR 8816707 OR 8816708 OR 8816709 OR 8816710 OR 8816711 OR 8816712 OR 8816713 OR 8816714 OR 8816715 OR 8816716 OR 8816717 OR 8816718 OR 8845150 OR 8845151 OR 8845152 OR 8845153 OR 8845154 OR 8845155 OR 8845156 OR 8845157 OR 8845158 OR 8845159 OR 8845160 OR 8845161 OR 8845162 OR 8845163 OR 8845164 OR 8845165 OR 8845166 OR 8845167 OR 8845168 OR 8845169 OR 8893018 OR 8893019 OR 8893020 OR 8893021 OR 8893022 OR 8893023 OR 8893024 OR 8893025 OR 8893026 OR 8893028 OR 8893029 OR 8893030 OR 8893031 OR 8893032 OR 8893033 OR 8893034 OR 8893035 OR 8938116 OR 8938117 OR 8938118 OR 8938119 OR 8938120 OR 8938121 OR 8938122 OR 8938123 OR 8938124 OR 8938125 OR 8938126 OR 8938127 OR 8938128 OR 8938129 OR 8938131 OR 8938132 OR 8938133 OR 8982155 OR 8982156 OR 8982157 OR 8982158 OR 8982159 OR 8982160 OR 8982161 OR 8982162 OR 8982163 OR 8982164 OR 8982165 OR 8982166 OR 8982167 OR 8982168 OR 8982169 OR 8982170 OR 8982171 OR 9010203 OR 9010204 OR 9010205 OR 9010206 OR 9010207 OR 9010208 OR 9010210 OR 9010211 OR 9010212 OR 9010214 OR 9052791 OR 9052792 OR 9052793 OR 9052794 OR 9052795 OR 9052796 OR 9052797 OR 9052798 OR 9052799 OR 9052800 OR 9052801 OR 9052802 OR 9115732 OR 9115733 OR 9115734 OR 9115735 OR 9115737 OR 9115740 OR 9115741 OR 9115743 OR 9136763 OR 9136764 OR 9136765 OR 9136766 OR 9136767 OR 9136768 OR 9136769 OR 9136770 OR 9136771 OR 9136772 OR 9136773 OR 9136774 OR 9136775 OR 9182797 OR 9182798 OR 9182799 OR 9182800 OR 9182801 OR 9182802 OR 9182803 OR 9182804 OR 9182805 OR 9182806 OR 9208853 OR 9208855 OR 9208856 OR 9208857 OR 9208858 OR 9208859 OR 9208860 OR 9208861 OR 9208862 OR 9208863 OR 9208864 OR 9208865 OR 9208866 OR 9208867 OR 9208868 OR 9247259 OR 9247260 OR 9247261 OR 9247262 OR 9247263 OR 9247264 OR 9247265 OR 9247266 OR 9247267 OR 9247268 OR 9247269 OR 9247270 OR 9247271 OR 9247272 OR 9247273 OR 9247274 OR 9247275 OR 9247276 OR 9292716 OR 9292717 OR 9292718 OR 9292719 OR 9292720 OR 9292721 OR 9292722 OR 9292723 OR 9292724 OR 9292725 OR 9292726 OR 9292727 OR 9292728 OR 9292729 OR 9292730 OR 9292731 OR 9292732 OR 9292733 OR 9331338 OR 9331343 OR 9331344 OR 9331345 OR 9331346 OR 9331347 OR 9331348 OR 9331349 OR 9331350 OR 9331352 OR 9331353 OR 9331354 OR 9331355 OR 9331356 OR 9331357 OR 9331358 OR 9331359 OR 9331360 OR 9331361 OR 9354320 OR 9354321 OR 9354324 OR 9354325 OR 9354326 OR 9354327 OR 9354328 OR 9354329 OR 9354330 OR 9354331 OR 9354332 OR 9354334 OR 9354335 OR 9354336 OR 9354338 OR 9354339 OR 9390513 OR 9390514 OR 9390515 OR 9390516 OR 9390517 OR 9390518 OR 9390519 OR 9390520 OR 9390521 OR 9390522 OR 9390523 OR 9390524 OR 9390525 OR 9390526 OR 9427242 OR 9427243 OR 9427244 OR 9427245 OR 9427246 OR 9427247 OR 9427248 OR 9427249 OR 9427250 OR 9427251 OR 9427252 OR 9427253 OR 9427254 OR 9427255 OR 9427256 OR 9459439 OR 9459440 OR 9459441 OR 9459442 OR 9459443 OR 9459444 OR 9459445 OR 9459446 OR 9459447 OR 9459448 OR 9459449 OR 9459450 OR 9459451 OR 9491979 OR 9491982 OR 9491983 OR 9491984 OR 9491985 OR 9491986 OR 9491987 OR 9491988 OR 9491990 OR 9491991 OR 9491992 OR 9491993 OR 9491994 OR 9539122 OR 9539123 OR 9539124 OR 9539125 OR 9539126 OR 9539127 OR 9539128 OR 9539129 OR 9539130 OR 9539131 OR 9539132 OR 9539133 OR 9581754 OR 9581759 OR 9581760 OR 9581761 OR 9581762 OR 9581763 OR 9581764 OR 9581765 OR 9581766 OR 9581767 OR 9581768 OR 9581769 OR 9581770 OR 9581771 OR 9620689 OR 9620690 OR 9620691 OR 9620692 OR 9620693 OR 9620694 OR 9620695 OR 9620696 OR 9620697 OR 9620698 OR 9620699 OR 9620700 OR 9620701 OR 9620702 OR 9620703 OR 9620704 OR 9620705 OR 9620706 OR 9620707 OR 9655492 OR 9655497 OR 9655498 OR 9655499 OR 9655500 OR 9655501 OR 9655502 OR 9655503 OR 9655504 OR 9655505 OR 9655507 OR 9655508 OR 9655509 OR 9655510 OR 9655511 OR 9655512 OR 9655513 OR 9655514 OR 9697850 OR 9697851 OR 9697852 OR 9697853 OR 9697854 OR 9697855 OR 9697856 OR 9697857 OR 9697858 OR 9697859 OR 9697860 OR 9697861 OR 9697862 OR 9697863 OR 9697864 OR 9697865 OR 9697866 OR 9697867 OR 9697868 OR 9728905 OR 9728911 OR 9728912 OR 9728913 OR 9728914 OR 9728915 OR 9728916 OR 9728917 OR 9728919 OR 9728920 OR 9728921 OR 9728922 OR 9728923 OR 9728924 OR 9728925 OR 9768836 OR 9768837 OR 9768838 OR 9768839 OR 9768840 OR 9768841 OR 9768842 OR 9768843 OR 9768844 OR 9768845 OR 9768846 OR 9768847 OR 9768848 OR 9768849 OR 9808444 OR 9808455 OR 9808456 OR 9808457 OR 9808458 OR 9808459 OR 9808460 OR 9808461 OR 9808462 OR 9808463 OR 9808464 OR 9808465 OR 9808466 OR 9808467 OR 9808468 OR 9808469 OR 9808470 OR 9808471 OR 9808472 OR 9808473 OR 9808474 OR 9808475 OR 9808476 OR 9856456 OR 9856457 OR 9856458 OR 9856459 OR 9856460 OR 9856461 OR 9856462 OR 9856463 OR 9856464 OR 9856465 OR 9856466 OR 9856467 OR 9856468 OR 9856469 OR 9856470 OR 9856471 OR 9856472 OR 9856473 OR 9856474 OR 9856475 OR 9883720 OR 9883721 OR 9883722 OR 9883723 OR 9883724 OR 9883725 OR 9883726 OR 9883727 OR 9883728 OR 9883729 OR 9883730 OR 9883731 OR 9883732 OR 9883733 OR 9883734 OR 9883735 OR 9883736 OR 9883737 OR 9883738 OR 9883739 OR 9883740 OR 10027287 OR 10027288 OR 10027289 OR 10027290 OR 10027291 OR 10027292 OR 10027293 OR 10027294 OR 10027295 OR 10027296 OR 10027297 OR 10027298 OR 10027299 OR 10027300 OR 10027301 OR 10069331 OR 10069332 OR 10069333 OR 10069334 OR 10069335 OR 10069336 OR 10069337 OR 10069338 OR 10069339 OR 10069340 OR 10069341 OR 10069342 OR 10069343 OR 10069344 OR 10195101 OR 10195102 OR 10195104 OR 10195105 OR 10195106 OR 10195107 OR 10195108 OR 10195109 OR 10195110 OR 10195111 OR 10195112 OR 10195113 OR 10195114 OR 10195122 OR 10195123 OR 10195124 OR 10195125 OR 10195126 OR 10195127 OR 10195128 OR 10195129 OR 10195130 OR 10195131 OR 10195132 OR 10195133 OR 10195141 OR 10195142 OR 10195143 OR 10195144 OR 10195145 OR 10195146 OR 10195147 OR 10195148 OR 10195151 OR 10195152 OR 10195157 OR 10195158 OR 10195160 OR 10195161 OR 10195162 OR 10195163 OR 10195164 OR 10195165 OR 10195166 OR 10195173 OR 10195174 OR 10195175 OR 10195176 OR 10195177 OR 10195178 OR 10195179 OR 10195180 OR 10195181 OR 10195182 OR 10195183 OR 10195184 OR 10195185 OR 10195193 OR 10195194 OR 10195195 OR 10195196 OR 10195197 OR 10195198 OR 10195199 OR 10195200 OR 10195201 OR 10195202 OR 10195203 OR 10195204 OR 10195205 OR 10195211 OR 10195213 OR 10195215 OR 10195216 OR 10195217 OR 10195218 OR 10195219 OR 10195220 OR 10195221 OR 10195222 OR 10195223 OR 10195224 OR 10196521 OR 10196522 OR 10196524 OR 10196525 OR 10196526 OR 10196527 OR 10196528 OR 10196529 OR 10196530 OR 10196531 OR 10196532 OR 10196533 OR 10196534 OR 10196542 OR 10196543 OR 10196544 OR 10196545 OR 10196546 OR 10196547 OR 10196548 OR 10196549 OR 10196550 OR 10196551 OR 10196560 OR 10196561 OR 10196562 OR 10196563 OR 10196564 OR 10196565 OR 10196566 OR 10196567 OR 10196568 OR 10196569 OR 10196570 OR 10196571 OR 10196572 OR 10196573 OR 10196578 OR 10196579 OR 10196581 OR 10196582 OR 10196583 OR 10196584 OR 10196585 OR 10196586 OR 10196587 OR 10196588 OR 10196589 OR 10196590 OR 10196591 OR 10196592 OR 10197518 OR 10197526 OR 10197527 OR 10197528 OR 10197529 OR 10197530 OR 10197531 OR 10197532 OR 10197533 OR 10197534 OR 10197535 OR 10197536 OR 10197537 OR 10197538 OR 10197539 OR 10197541 OR 10204538 OR 10204539 OR 10204540 OR 10204541 OR 10204543 OR 10204544 OR 10204545 OR 10204546 OR 10204547 OR 10230778 OR 10230780 OR 10230781 OR 10230788 OR 10230789 OR 10230790 OR 10230791 OR 10230792 OR 10230793 OR 10230794 OR 10230796 OR 10230797 OR 10230798 OR 10230799 OR 10230800 OR 10230801 OR 10230802 OR 10321241 OR 10321243 OR 10321244 OR 10321245 OR 10321246 OR 10321247 OR 10321248 OR 10321249 OR 10321250 OR 10321251 OR 10321252 OR 10321253 OR 10399931 OR 10399932 OR 10399933 OR 10399934 OR 10399935 OR 10399936 OR 10399937 OR 10399938 OR 10399939 OR 10399940 OR 10399941 OR 10399942 OR 10399943 OR 10399944 OR 10402191 OR 10402192 OR 10402193 OR 10402194 OR 10402195 OR 10402196 OR 10402197 OR 10402198 OR 10402199 OR 10402200 OR 10402201 OR 10402202 OR 10402203 OR 10402204 OR 10404179 OR 10404183 OR 10404192 OR 10404196 OR 10404197 OR 10404198 OR 10404199 OR 10404200 OR 10404201 OR 10404202 OR 10404203 OR 10409387 OR 10412055 OR 10412057 OR 10412058 OR 10412059 OR 10412060 OR 10412061 OR 10412062 OR 10412063 OR 10412064 OR 10412065 OR 10412066 OR 10433258 OR 10433259 OR 10433260 OR 10433261 OR 10433262 OR 10433263 OR 10433264 OR 10433265 OR 10433266 OR 10433267 OR 10433268 OR 10433269 OR 10433270 OR 10433271 OR 10433272 OR 10448211 OR 10448212 OR 10448213 OR 10448214 OR 10448215 OR 10448216 OR 10448217 OR 10448218 OR 10448219 OR 10448220 OR 10448221 OR 10448222 OR 10448223 OR 10448224 OR 10461216 OR 10461217 OR 10461218 OR 10461219 OR 10461220 OR 10461221 OR 10461223 OR 10461225 OR 10482224 OR 10482234 OR 10482235 OR 10482236 OR 10482237 OR 10482238 OR 10482239 OR 10482240 OR 10482242 OR 10482243 OR 10482244 OR 10482245 OR 10482246 OR 10482247 OR 10491597 OR 10491598 OR 10491599 OR 10491600 OR 10491605 OR 10491606 OR 10491607 OR 10491608 OR 10491609 OR 10491610 OR 10491612 OR 10526323 OR 10526324 OR 10526325 OR 10526326 OR 10526329 OR 10526330 OR 10526331 OR 10526333 OR 10526334 OR 10526335 OR 10526336 OR 10526337 OR 10526338 OR 10526339 OR 10526340 OR 10526343 OR 10570481 OR 10570482 OR 10570483 OR 10570485 OR 10570486 OR 10570487 OR 10570488 OR 10570489 OR 10570490 OR 10570491 OR 10570492 OR 10571227 OR 10571229 OR 10571231 OR 10571233 OR 10571234 OR 10571235 OR 10571236 OR 10571237 OR 10571238 OR 10571239 OR 10571240 OR 10571241 OR 10595507 OR 10595508 OR 10595509 OR 10595510 OR 10595511 OR 10595512 OR 10595513 OR 10595514 OR 10595515 OR 10595516 OR 10595517 OR 10595518 OR 10595519 OR 10595520 OR 10595521 OR 10595522 OR 10595523 OR 10595524 OR 10607390 OR 10607391 OR 10607392 OR 10607393 OR 10607394 OR 10607395 OR 10607398 OR 10624936 OR 10624937 OR 10624938 OR 10624939 OR 10624943 OR 10624944 OR 10624945 OR 10624946 OR 10624947 OR 10624948 OR 10624949 OR 10624950 OR 10624951 OR 10624954 OR 10624957 OR 10624958 OR 10624959 OR 10624960 OR 10624961 OR 10624962 OR 10624963 OR 10624964 OR 10624965 OR 10649564 OR 10649565 OR 10649566 OR 10649567 OR 10649568 OR 10649569 OR 10649570 OR 10649571 OR 10649572 OR 10649574 OR 10677022 OR 10677031 OR 10677032 OR 10677033 OR 10677034 OR 10677035 OR 10677036 OR 10677037 OR 10677038 OR 10677039 OR 10677040 OR 10677041 OR 10677042 OR 10677043 OR 10677044 OR 10700250 OR 10700251 OR 10700252 OR 10700253 OR 10700254 OR 10700255 OR 10700256 OR 10700257 OR 10700258 OR 10700260 OR 10700261 OR 10700262 OR 10700263 OR 10707970 OR 10707971 OR 10707972 OR 10707973 OR 10707974 OR 10707975 OR 10707976 OR 10707977 OR 10707978 OR 10707979 OR 10707980 OR 10707981 OR 10707982 OR 10707983 OR 10707984 OR 10707985 OR 10707986 OR 10707987 OR 10719885 OR 10719886 OR 10719887 OR 10719888 OR 10719889 OR 10719890 OR 10719891 OR 10719893 OR 10719894 OR 10719895 OR 10719896 OR 10719897 OR 10719898 OR 10719899 OR 10719900 OR 10719901 OR 10725917 OR 10725919 OR 10725920 OR 10725921 OR 10725922 OR 10725923 OR 10725924 OR 10725925 OR 10725926 OR 10725927 OR 10725928 OR 10725929 OR 10725930 OR 10725931 OR 10769379 OR 10769380 OR 10769382 OR 10769383 OR 10769384 OR 10769385 OR 10769386 OR 10769387 OR 10769388 OR 10769389 OR 10769390 OR 10769391 OR 10769392 OR 10769393 OR 10769394 OR 10774723 OR 10774724 OR 10774726 OR 10774727 OR 10774728 OR 10774729 OR 10774730 OR 10774731 OR 10774732 OR 10774733 OR 10774734 OR 10774735 OR 10774736 OR 10774737 OR 10774738 OR 10798390 OR 10798391 OR 10798392 OR 10798393 OR 10798394 OR 10798395 OR 10798396 OR 10798397 OR 10798398 OR 10798399 OR 10798400 OR 10798401 OR 10798402 OR 10798403 OR 10798404 OR 10798405 OR 10798406 OR 10798407 OR 10798408 OR 10798409 OR 10798410 OR 10816306 OR 10816307 OR 10816310 OR 10816311 OR 10816312 OR 10816313 OR 10816314 OR 10816315 OR 10816316 OR 10816318 OR 10816319 OR 10839350 OR 10839352 OR 10839353 OR 10839354 OR 10839355 OR 10839356 OR 10839357 OR 10839358 OR 10839359 OR 10839360 OR 10839361 OR 10839362 OR 10839363 OR 10839364 OR 10839365 OR 10839366 OR 10839367 OR 10839368 OR 10839369 OR 10839370 OR 10839371 OR 10862694 OR 10862695 OR 10862696 OR 10862698 OR 10862699 OR 10862700 OR 10862701 OR 10862702 OR 10862703 OR 10862704 OR 10862706 OR 10862708 OR 10896155 OR 10896156 OR 10896157 OR 10896158 OR 10896159 OR 10896160 OR 10896161 OR 10896162 OR 10896163 OR 10896164 OR 10896165 OR 10896166 OR 10896167 OR 10896168 OR 10896169 OR 10903565 OR 10903566 OR 10903569 OR 10903570 OR 10903571 OR 10903572 OR 10903573 OR 10903574 OR 10903575 OR 10903576 OR 10903577 OR 10903578 OR 10939323 OR 10939328 OR 10939329 OR 10939330 OR 10939331 OR 10939332 OR 10939333 OR 10939334 OR 10939335 OR 10939336 OR 10939337 OR 10939338 OR 10939339 OR 10939340 OR 10939341 OR 10966613 OR 10966614 OR 10966616 OR 10966617 OR 10966618 OR 10966619 OR 10966620 OR 10966621 OR 10966622 OR 10966623 OR 10966624 OR 10966625 OR 10966626 OR 10966627 OR 10966628 OR 10985339 OR 10985343 OR 10985345 OR 10985346 OR 10985347 OR 10985348 OR 10985349 OR 10985350 OR 10985351 OR 10985352 OR 10985353 OR 10985354 OR 10985355 OR 10985356 OR 10985357 OR 10985358 OR 11017168 OR 11017169 OR 11017170 OR 11017171 OR 11017172 OR 11017173 OR 11017174 OR 11017175 OR 11017176 OR 11017177 OR 11017178 OR 11017179 OR 11036260 OR 11036261 OR 11036262 OR 11036263 OR 11036264 OR 11036265 OR 11036266 OR 11036267 OR 11036268 OR 11036269 OR 11036270 OR 11036271 OR 11036272 OR 11036273 OR 11036274 OR 11055428 OR 11055429 OR 11055430 OR 11055431 OR 11055432 OR 11055433 OR 11055434 OR 11055435 OR 11055436 OR 11055437 OR 11055438 OR 11055439 OR 11055440 OR 11055441 OR 11055442 OR 11055443 OR 11055444 OR 11055445 OR 11086981 OR 11086982 OR 11086983 OR 11086984 OR 11086985 OR 11086986 OR 11086987 OR 11086988 OR 11086989 OR 11086990 OR 11086991 OR 11086992 OR 11086993 OR 11086994 OR 11086995 OR 11086996 OR 11086997 OR 11086998 OR 11086999 OR 11087000 OR 11087001 OR 11100141 OR 11100144 OR 11100145 OR 11100146 OR 11100147 OR 11100148 OR 11100149 OR 11100150 OR 11100151 OR 11100152 OR 11100153 OR 11100154 OR 11100155 OR 11100156 OR 11100157 OR 11135641 OR 11135642 OR 11135643 OR 11135644 OR 11135645 OR 11135646 OR 11135647 OR 11135652 OR 11144348 OR 11144350 OR 11144351 OR 11144352 OR 11144353 OR 11144354 OR 11144355 OR 11144356 OR 11144357 OR 11144358 OR 11144359 OR 11144360 OR 11144361 OR 11144362 OR 11144363 OR 11144364 OR 11144365 OR 11144366 OR 11144367 OR 11163258 OR 11163259 OR 11163260 OR 11163261 OR 11163262 OR 11163263 OR 11163264 OR 11163265 OR 11163266 OR 11163267 OR 11163268 OR 11163269 OR 11163270 OR 11163271 OR 11163272 OR 11163273 OR 11163274 OR 11163275 OR 11163276 OR 11163277 OR 11163278 OR 11163279 OR 11163280 OR 11175864 OR 11175869 OR 11175870 OR 11175872 OR 11175873 OR 11175874 OR 11175875 OR 11175876 OR 11175877 OR 11175878 OR 11175879 OR 11175880 OR 11175881 OR 11175882 OR 11175883 OR 11175884 OR 11182080 OR 11182081 OR 11182082 OR 11182083 OR 11182084 OR 11182085 OR 11182086 OR 11182087 OR 11182088 OR 11182089 OR 11182090 OR 11182091 OR 11182092 OR 11182093 OR 11182094 OR 11182095 OR 11182096 OR 11182097 OR 11224535 OR 11224536 OR 11224537 OR 11224538 OR 11224539 OR 11224540 OR 11224541 OR 11224542 OR 11224543 OR 11224544 OR 11224545 OR 11224546 OR 11224547 OR 11224548 OR 11224549 OR 11224550 OR 11224551 OR 11239426 OR 11239427 OR 11239428 OR 11239429 OR 11239430 OR 11239431 OR 11239432 OR 11239433 OR 11239434 OR 11239435 OR 11239436 OR 11239437 OR 11239438 OR 11239439 OR 11239440 OR 11239441 OR 11239442 OR 11276221 OR 11276222 OR 11276223 OR 11276224 OR 11276226 OR 11276227 OR 11276228 OR 11276229 OR 11276230 OR 11276231 OR 11276232 OR 11276233 OR 11276234 OR 11276235 OR 11276236 OR 11276237 OR 11301021 OR 11301022 OR 11301023 OR 11301026 OR 11301027 OR 11301028 OR 11301029 OR 11301030 OR 11301031 OR 11301032 OR 11301033 OR 11301034 OR 11301035 OR 11319553 OR 11319555 OR 11319556 OR 11319557 OR 11319558 OR 11319559 OR 11319560 OR 11319561 OR 11319562 OR 11343643 OR 11343644 OR 11343645 OR 11343646 OR 11343647 OR 11343648 OR 11343649 OR 11343650 OR 11343651 OR 11343652 OR 11343653 OR 11343654 OR 11343655 OR 11343656 OR 11343657 OR 11343658 OR 11343659 OR 11343660 OR 11343661 OR 11343662 OR 11369935 OR 11369936 OR 11369938 OR 11369939 OR 11369940 OR 11369942 OR 11369943 OR 11369944 OR 11369945 OR 11369946 OR 11369947 OR 11369948 OR 11369949 OR 11394998 OR 11394999 OR 11395000 OR 11395001 OR 11395002 OR 11395003 OR 11395004 OR 11395005 OR 11395006 OR 11395007 OR 11395008 OR 11395009 OR 11395010 OR 11395011 OR 11395012 OR 11395013 OR 11395014 OR 11395015 OR 11395016 OR 11395017 OR 11395018 OR 11395019 OR 11426219 OR 11426220 OR 11426221 OR 11426222 OR 11426224 OR 11426225 OR 11426226 OR 11426227 OR 11426228 OR 11426229 OR 11426230 OR 11426233 OR 11430800 OR 11430801 OR 11430802 OR 11430803 OR 11430804 OR 11430805 OR 11430806 OR 11430807 OR 11430808 OR 11430809 OR 11430810 OR 11430811 OR 11430812 OR 11430813 OR 11430814 OR 11477421 OR 11477422 OR 11477424 OR 11477425 OR 11477426 OR 11477427 OR 11477428 OR 11477429 OR 11477430 OR 11477431 OR 11477432 OR 11498048 OR 11498049 OR 11498050 OR 11498051 OR 11498052 OR 11498053 OR 11498054 OR 11498055 OR 11498056 OR 11498057 OR 11498058 OR 11502254 OR 11502255 OR 11502256 OR 11502257 OR 11502258 OR 11502259 OR 11502260 OR 11502261 OR 11502262 OR 11516394 OR 11516395 OR 11516396 OR 11516397 OR 11516398 OR 11516399 OR 11516401 OR 11516402 O</t>
-  </si>
-  <si>
-    <t>PMID=(17952068 OR 17952069 OR 17965653 OR 17965710 OR 17965711 OR 17965712 OR 17982449 OR 17982450 OR 17982451 OR 17982452 OR 17982453 OR 17988629 OR 17988630 OR 17988631 OR 17988632 OR 17988633 OR 17988634 OR 17988635 OR 17988636 OR 17988637 OR 17988638 OR 17994013 OR 17994014 OR 17994015 OR 17994016 OR 18026096 OR 18026097 OR 18026098 OR 18026099 OR 18031679 OR 18031680 OR 18031681 OR 18031682 OR 18031683 OR 18031684 OR 18031685 OR 18031686 OR 18031687 OR 18031688 OR 18031689 OR 18037883 OR 18037884 OR 18054856 OR 18054857 OR 18054858 OR 18054859 OR 18054860 OR 18054861 OR 18054862 OR 18054863 OR 18054864 OR 18054865 OR 18054866 OR 18059264 OR 18059265 OR 18066056 OR 18066057 OR 18066058 OR 18066059 OR 18066060 OR 18066061 OR 18084286 OR 18084287 OR 18084288 OR 18084289 OR 18093519 OR 18093520 OR 18093522 OR 18093523 OR 18093524 OR 18093525 OR 18093526 OR 18093527 OR 18093528 OR 18093529 OR 18093530 OR 18093531 OR 18093532 OR 18157125 OR 18157126 OR 18159219 OR 18160954 OR 18160955 OR 18160956 OR 18160957 OR 18176559 OR 18176560 OR 18184560 OR 18184562 OR 18184563 OR 18184564 OR 18184565 OR 18184566 OR 18184567 OR 18184568 OR 18184569 OR 18184570 OR 18184571 OR 18184572 OR 18193039 OR 18193040 OR 18193041 OR 18193042 OR 18204441 OR 18204442 OR 18204443 OR 18204444 OR 18204445 OR 18213359 OR 18215619 OR 18215620 OR 18215621 OR 18215622 OR 18215623 OR 18215624 OR 18215625 OR 18215626 OR 18215627 OR 18223647 OR 18223648 OR 18223649 OR 18246064 OR 18246065 OR 18255029 OR 18255030 OR 18255031 OR 18255032 OR 18255033 OR 18255034 OR 18255035 OR 18255036 OR 18255037 OR 18255038 OR 18264094 OR 18264095 OR 18278039 OR 18278040 OR 18278041 OR 18278042 OR 18278043 OR 18297065 OR 18297066 OR 18297067 OR 18297068 OR 18311133 OR 18311135 OR 18311136 OR 18344990 OR 18344994 OR 18344995 OR 18344997 OR 18345353 OR 18367083 OR 18367084 OR 18367085 OR 18367086 OR 18367087 OR 18367088 OR 18367089 OR 18367090 OR 18367091 OR 18367092 OR 18367093 OR 18371326 OR 18371327 OR 18371330 OR 18371331 OR 18371332 OR 18371335 OR 18371336 OR 18371337 OR 18371338 OR 18371339 OR 18371340 OR 18371342 OR 18371343 OR 18371345 OR 18371348 OR 18371349 OR 18371350 OR 18371351 OR 18371352 OR 18371353 OR 18371359 OR 18371362 OR 18371363 OR 18371364 OR 18371365 OR 18371366 OR 18371367 OR 18371368 OR 18371370 OR 18371373 OR 18371377 OR 18371378 OR 18371379 OR 18371380 OR 18371381 OR 18371382 OR 18371391 OR 18371392 OR 18371393 OR 18371394 OR 18371395 OR 18371405 OR 18371406 OR 18371407 OR 18371408 OR 18371409 OR 18371420 OR 18371421 OR 18371422 OR 18371423 OR 18371424 OR 18371425 OR 18371432 OR 18371435 OR 18371436 OR 18371437 OR 18371438 OR 18371439 OR 18371447 OR 18371448 OR 18371449 OR 18371450 OR 18371451 OR 18371452 OR 18371453 OR 18376400 OR 18382462 OR 18383627 OR 18391942 OR 18391943 OR 18391944 OR 18391945 OR 18391946 OR 18397753 OR 18397754 OR 18397755 OR 18397756 OR 18397757 OR 18397758 OR 18408715 OR 18408716 OR 18408717 OR 18425121 OR 18425122 OR 18425123 OR 18425124 OR 18432196 OR 18432197 OR 18432198 OR 18439401 OR 18439403 OR 18439404 OR 18439405 OR 18439406 OR 18439407 OR 18439408 OR 18439409 OR 18439410 OR 18439411 OR 18439412 OR 18454144 OR 18454145 OR 18462688 OR 18462691 OR 18462692 OR 18462694 OR 18462695 OR 18462696 OR 18462697 OR 18462698 OR 18462699 OR 18466743 OR 18466744 OR 18466745 OR 18466746 OR 18466747 OR 18466748 OR 18466749 OR 18466750 OR 18466751 OR 18466752 OR 18466753 OR 18466754 OR 18469810 OR 18469811 OR 18488022 OR 18488023 OR 18488024 OR 18488025 OR 18498732 OR 18498733 OR 18498734 OR 18498735 OR 18498736 OR 18498737 OR 18498738 OR 18498739 OR 18498740 OR 18498741 OR 18498742 OR 18500338 OR 18516033 OR 18516034 OR 18516035 OR 18516036 OR 18522848 OR 18522849 OR 18522850 OR 18522851 OR 18522852 OR 18522853 OR 18536709 OR 18536710 OR 18536711 OR 18536712 OR 18549778 OR 18549780 OR 18549781 OR 18549782 OR 18549783 OR 18549784 OR 18549785 OR 18549786 OR 18549787 OR 18549788 OR 18549789 OR 18549790 OR 18549791 OR 18552840 OR 18552841 OR 18552842 OR 18552843 OR 18552844 OR 18568020 OR 18568021 OR 18568022 OR 18587389 OR 18587390 OR 18587391 OR 18587392 OR 18587393 OR 18593551 OR 18593552 OR 18593554 OR 18593557 OR 18593558 OR 18593559 OR 18593560 OR 18593561 OR 18593562 OR 18593563 OR 18604203 OR 18604204 OR 18604205 OR 18614027 OR 18614028 OR 18614029 OR 18614030 OR 18614031 OR 18614032 OR 18614033 OR 18614034 OR 18614035 OR 18614036 OR 18614037 OR 18614038 OR 18622399 OR 18622400 OR 18622401 OR 18622402 OR 18641642 OR 18641643 OR 18641644 OR 18641645 OR 18660806 OR 18660807 OR 18660808 OR 18682239 OR 18682240 OR 18682241 OR 18682242 OR 18682243 OR 18701062 OR 18701064 OR 18701065 OR 18701066 OR 18701067 OR 18701068 OR 18701069 OR 18701070 OR 18701071 OR 18701072 OR 18701073 OR 18701074 OR 18701075 OR 18711393 OR 18758458 OR 18758459 OR 18758460 OR 18760692 OR 18760693 OR 18760696 OR 18760697 OR 18760698 OR 18760699 OR 18776892 OR 18776893 OR 18776894 OR 18776895 OR 18776896 OR 18776897 OR 18786354 OR 18786355 OR 18786356 OR 18786357 OR 18786358 OR 18786359 OR 18786360 OR 18786361 OR 18786362 OR 18786363 OR 18786364 OR 18786365 OR 18786407 OR 18786408 OR 18786410 OR 18786413 OR 18786414 OR 18786415 OR 18786416 OR 18786417 OR 18786418 OR 18786419 OR 18786421 OR 18794839 OR 18794840 OR 18804426 OR 18806784 OR 18806785 OR 18806786 OR 18817733 OR 18817734 OR 18817735 OR 18817736 OR 18817737 OR 18817738 OR 18817739 OR 18818591 OR 18820690 OR 18820691 OR 18820692 OR 18820693 OR 18820694 OR 18820695 OR 18836441 OR 18836442 OR 18836443 OR 18849983 OR 18849984 OR 18849985 OR 18849986 OR 18931664 OR 18931665 OR 18931666 OR 18938742 OR 18938746 OR 18940731 OR 18940732 OR 18940733 OR 18940734 OR 18940735 OR 18940736 OR 18953346 OR 18953347 OR 18953348 OR 18956012 OR 18957216 OR 18957217 OR 18957218 OR 18957219 OR 18957220 OR 18957221 OR 18957222 OR 18957223 OR 18957224 OR 18957225 OR 18957226 OR 18957227 OR 18957228 OR 18978778 OR 18978779 OR 18978780 OR 18978781 OR 18983965 OR 18983966 OR 18983967 OR 18983968 OR 18983969 OR 18983970 OR 18995816 OR 18995818 OR 18995819 OR 18995820 OR 18995821 OR 18995827 OR 18997789 OR 18997790 OR 18997791 OR 19011624 OR 19011625 OR 19029885 OR 19029887 OR 19029888 OR 19029889 OR 19029890 OR 19038214 OR 19038215 OR 19038216 OR 19038217 OR 19038218 OR 19038219 OR 19038220 OR 19038221 OR 19038222 OR 19038223 OR 19038224 OR 19038225 OR 19038226 OR 19038227 OR 19041778 OR 19041779 OR 19041780 OR 19041781 OR 19041782 OR 19041783 OR 19043409 OR 19043410 OR 19060895 OR 19079249 OR 19079250 OR 19079251 OR 19081373 OR 19081374 OR 19081375 OR 19081376 OR 19081377 OR 19081378 OR 19081379 OR 19081380 OR 19081381 OR 19081382 OR 19081384 OR 19081385 OR 19098904 OR 19098905 OR 19109905 OR 19109906 OR 19109907 OR 19109908 OR 19109909 OR 19109910 OR 19109911 OR 19109912 OR 19109913 OR 19109914 OR 19109915 OR 19109917 OR 19109918 OR 19109919 OR 19119091 OR 19122665 OR 19122666 OR 19128787 OR 19128789 OR 19128791 OR 19128792 OR 19128793 OR 19128794 OR 19128795 OR 19136969 OR 19136970 OR 19136971 OR 19136972 OR 19136973 OR 19136974 OR 19146810 OR 19146811 OR 19146812 OR 19146813 OR 19146814 OR 19146815 OR 19146816 OR 19146817 OR 19146818 OR 19151709 OR 19151710 OR 19151711 OR 19151712 OR 19160494 OR 19160495 OR 19160496 OR 19160497 OR 19160498 OR 19160499 OR 19160500 OR 19160501 OR 19160502 OR 19160503 OR 19160504 OR 19160505 OR 19160506 OR 19160507 OR 19160508 OR 19160509 OR 19160510 OR 19169249 OR 19169250 OR 19169251 OR 19169252 OR 19186162 OR 19186163 OR 19186164 OR 19186165 OR 19186166 OR 19186167 OR 19186168 OR 19186169 OR 19186170 OR 19186171 OR 19186172 OR 19200796 OR 19200800 OR 19200802 OR 19200803 OR 19200804 OR 19200805 OR 19209466 OR 19217371 OR 19217373 OR 19217374 OR 19217375 OR 19217376 OR 19217377 OR 19217378 OR 19217379 OR 19217380 OR 19217381 OR 19217382 OR 19217383 OR 19249272 OR 19249273 OR 19249274 OR 19249275 OR 19249276 OR 19249277 OR 19249278 OR 19249279 OR 19249280 OR 19249281 OR 19249282 OR 19252494 OR 19252495 OR 19252496 OR 19252497 OR 19252498 OR 19265651 OR 19265653 OR 19265655 OR 19265659 OR 19265661 OR 19265662 OR 19265663 OR 19265664 OR 19265665 OR 19270686 OR 19270687 OR 19270688 OR 19270689 OR 19270690 OR 19285465 OR 19285466 OR 19285468 OR 19285469 OR 19285470 OR 19285471 OR 19285472 OR 19285473 OR 19285474 OR 19285475 OR 19287386 OR 19287387 OR 19287388 OR 19287389 OR 19305400 OR 19305401 OR 19305402 OR 19322241 OR 19323994 OR 19323995 OR 19323996 OR 19323997 OR 19323998 OR 19323999 OR 19324000 OR 19324001 OR 19324002 OR 19324003 OR 19330001 OR 19330002 OR 19330003 OR 19330004 OR 19341616 OR 19341618 OR 19341619 OR 19341621 OR 19341622 OR 19341623 OR 19341624 OR 19341625 OR 19345177 OR 19349974 OR 19349975 OR 19349976 OR 19349977 OR 19363489 OR 19363490 OR 19363491 OR 19363492 OR 19376064 OR 19376065 OR 19376067 OR 19376068 OR 19376069 OR 19376070 OR 19376071 OR 19376072 OR 19376073 OR 19376074 OR 19377470 OR 19377471 OR 19377472 OR 19377473 OR 19396165 OR 19398399 OR 19409264 OR 19409265 OR 19409266 OR 19409267 OR 19409268 OR 19409269 OR 19409270 OR 19409271 OR 19409272 OR 19409273 OR 19412165 OR 19412166 OR 19412167 OR 19412168 OR 19427283 OR 19427286 OR 19427288 OR 19427290 OR 19427291 OR 19427292 OR 19427293 OR 19427294 OR 19430469 OR 19430470 OR 19430471 OR 19430472 OR 19430473 OR 19430474 OR 19447089 OR 19447090 OR 19447092 OR 19447093 OR 19447094 OR 19447095 OR 19447098 OR 19448628 OR 19448629 OR 19477150 OR 19477151 OR 19477152 OR 19477153 OR 19477154 OR 19477155 OR 19477156 OR 19477157 OR 19477158 OR 19477159 OR 19481515 OR 19483686 OR 19483687 OR 19483688 OR 19483689 OR 19497280 OR 19497281 OR 19497282 OR 19497283 OR 19497284 OR 19497285 OR 19503082 OR 19503083 OR 19503084 OR 19503085 OR 19503086 OR 19503087 OR 19524523 OR 19524524 OR 19524525 OR 19524526 OR 19524527 OR 19524528 OR 19524529 OR 19524530 OR 19524531 OR 19525941 OR 19525942 OR 19525943 OR 19525944 OR 19525945 OR 19525946 OR 19540188 OR 19543280 OR 19543281 OR 19555646 OR 19555647 OR 19555648 OR 19555649 OR 19555650 OR 19555651 OR 19555652 OR 19555653 OR 19555654 OR 19561601 OR 19561602 OR 19561603 OR 19570509 OR 19570512 OR 19570513 OR 19570514 OR 19570515 OR 19570516 OR 19570517 OR 19570518 OR 19578379 OR 19578380 OR 19578381 OR 19578382 OR 19597494 OR 19597495 OR 19607788 OR 19607789 OR 19607790 OR 19607791 OR 19607792 OR 19607793 OR 19607794 OR 19607795 OR 19607796 OR 19607797 OR 19607798 OR 19620975 OR 19620976 OR 19620977 OR 19620978 OR 19631602 OR 19633665 OR 19633666 OR 19633667 OR 19640477 OR 19640478 OR 19640479 OR 19640480 OR 19640481 OR 19640482 OR 19640483 OR 19640484 OR 19648911 OR 19648912 OR 19648913 OR 19648914 OR 19648915 OR 19657336 OR 19664980 OR 19664984 OR 19664985 OR 19664988 OR 19664990 OR 19664991 OR 19664992 OR 19664993 OR 19664994 OR 19664995 OR 19668198 OR 19668199 OR 19668200 OR 19668201 OR 19679071 OR 19679072 OR 19679073 OR 19679074 OR 19679075 OR 19679076 OR 19679077 OR 19679078 OR 19679079 OR 19684588 OR 19684589 OR 19684590 OR 19684591 OR 19684592 OR 19684593 OR 19699165 OR 19701197 OR 19701198 OR 19716359 OR 19718034 OR 19718035 OR 19718036 OR 19733528 OR 19733531 OR 19733533 OR 19733540 OR 19733541 OR 19733542 OR 19733543 OR 19733544 OR 19734891 OR 19734892 OR 19734893 OR 19734894 OR 19734895 OR 19734896 OR 19734897 OR 19749747 OR 19749748 OR 19749749 OR 19749750 OR 19749751 OR 19755100 OR 19755102 OR 19755103 OR 19755104 OR 19755105 OR 19755106 OR 19755107 OR 19755108 OR 19755109 OR 19755110 OR 19755111 OR 19759538 OR 19767747 OR 19778502 OR 19778505 OR 19778506 OR 19778507 OR 19778508 OR 19778509 OR 19778510 OR 19778511 OR 19778512 OR 19778513 OR 19778514 OR 19778515 OR 19778516 OR 19778517 OR 19783975 OR 19783978 OR 19783979 OR 19783992 OR 19783993 OR 19783994 OR 19796610 OR 19796612 OR 19796616 OR 19796619 OR 19796620 OR 19796621 OR 19796622 OR 19796623 OR 19796624 OR 19801986 OR 19801987 OR 19801988 OR 19801989 OR 19818703 OR 19820704 OR 19820705 OR 19820706 OR 19820707 OR 19838177 OR 19838178 OR 19838179 OR 19838180 OR 19840541 OR 19840542 OR 19840543 OR 19840544 OR 19840547 OR 19855389 OR 19855390 OR 19874785 OR 19874786 OR 19874787 OR 19874788 OR 19874789 OR 19874790 OR 19874791 OR 19874792 OR 19874793 OR 19874794 OR 19881502 OR 19881503 OR 19881504 OR 19881505 OR 19881506 OR 19896441 OR 19896442 OR 19896443 OR 19896444 OR 19896445 OR 19898467 OR 19898468 OR 19898469 OR 19898470 OR 19904261 OR 19914180 OR 19914181 OR 19914182 OR 19914183 OR 19914184 OR 19914185 OR 19914186 OR 19914187 OR 19914188 OR 19914189 OR 19914190 OR 19915562 OR 19915563 OR 19915564 OR 19915565 OR 19915566 OR 19915567 OR 19935653 OR 19935654 OR 19935655 OR 19946318 OR 19946319 OR 19951688 OR 19951689 OR 19951690 OR 19951691 OR 19951692 OR 19951693 OR 19966837 OR 19966838 OR 19966839 OR 19966840 OR 19966842 OR 20005817 OR 20005819 OR 20005821 OR 20005822 OR 20005823 OR 20005824 OR 20005825 OR 20005826 OR 20005827 OR 20005828 OR 20005829 OR 20005830 OR 20010818 OR 20010819 OR 20010820 OR 20010821 OR 20010822 OR 20010823 OR 20010824 OR 20023650 OR 20023651 OR 20023652 OR 20023653 OR 20023654 OR 20023655 OR 20023656 OR 20036631 OR 20037574 OR 20037575 OR 20037576 OR 20037577 OR 20037578 OR 20037579 OR 20062052 OR 20062053 OR 20064381 OR 20064385 OR 20064387 OR 20064388 OR 20064389 OR 20064390 OR 20064391 OR 20064392 OR 20064393 OR 20064394 OR 20064395 OR 20064397 OR 20064398 OR 20064399 OR 20074533 OR 20074534 OR 20074535 OR 20074536 OR 20081850 OR 20081851 OR 20081852 OR 20085737 OR 20085738 OR 20085739 OR 20085740 OR 20085741 OR 20096661 OR 20098418 OR 20098419 OR 20098420 OR 20118924 OR 20118925 OR 20118926 OR 20118927 OR 20139973 OR 20139974 OR 20139976 OR 20144783 OR 20144785 OR 20144786 OR 20144787 OR 20144788 OR 20144789 OR 20152111 OR 20152112 OR 20152113 OR 20152114 OR 20152115 OR 20152116 OR 20152117 OR 20152118 OR 20152119 OR 20154682 OR 20154683 OR 20154684 OR 20159445 OR 20159446 OR 20159447 OR 20159448 OR 20159449 OR 20159450 OR 20159451 OR 20159452 OR 20159453 OR 20159454 OR 20173744 OR 20173745 OR 20173746 OR 20188651 OR 20188652 OR 20188653 OR 20188654 OR 20188655 OR 20188656 OR 20188657 OR 20188658 OR 20188659 OR 20188660 OR 20207221 OR 20207222 OR 20207225 OR 20207226 OR 20207227 OR 20207228 OR 20207229 OR 20207230 OR 20223197 OR 20223198 OR 20223199 OR 20223200 OR 20223201 OR 20223202 OR 20223203 OR 20223204 OR 20223205 OR 20223206 OR 20348915 OR 20348916 OR 20348917 OR 20348918 OR 20348919 OR 20348920 OR 20362535 OR 20362536 OR 20362537 OR 20362538 OR 20362539 OR 20362540 OR 20362541 OR 20362542 OR 20364143 OR 20364144 OR 20364145 OR 20383135 OR 20383136 OR 20383137 OR 20383138 OR 20399725 OR 20399727 OR 20399728 OR 20399730 OR 20399732 OR 20399733 OR 20399734 OR 20399735 OR 20399736 OR 20400959 OR 20400960 OR 20414199 OR 20418874 OR 20418875 OR 20434996 OR 20434997 OR 20434998 OR 20434999 OR 20435000 OR 20435001 OR 20435002 OR 20435003 OR 20435004 OR 20435005 OR 20435006 OR 20436478 OR 20436479 OR 20436480 OR 20436481 OR 20436482 OR 20452313 OR 20452314 OR 20452315 OR 20452317 OR 20452318 OR 20452319 OR 20452320 OR 20452321 OR 20452322 OR 20453850 OR 20453851 OR 20453852 OR 20453853 OR 20471349 OR 20471350 OR 20471351 OR 20471352 OR 20471353 OR 20471354 OR 20471355 OR 20471356 OR 20471357 OR 20471358 OR 20473290 OR 20473291 OR 20473292 OR 20473293 OR 20495557 OR 20495558 OR 20495559 OR 20510855 OR 20512132 OR 20512133 OR 20512134 OR 20512135 OR 20512136 OR 20512137 OR 20526331 OR 20526332 OR 20526333 OR 20526334 OR 20543841 OR 20543842 OR 20543843 OR 20562869 OR 20569687 OR 20569688 OR 20569689 OR 20569691 OR 20569693 OR 20569694 OR 20569695 OR 20569697 OR 20578343 OR 20581814 OR 20581815 OR 20581816 OR 20581840 OR 20581841 OR 20581842 OR 20581843 OR 20601946 OR 20601947 OR 20601948 OR 20619762 OR 20619763 OR 20620868 OR 20620869 OR 20620870 OR 20620871 OR 20620872 OR 20620873 OR 20620874 OR 20620875 OR 20620876 OR 20620877 OR 20620878 OR 20620879 OR 20621043 OR 20621044 OR 20621045 OR 20621046 OR 20621049 OR 20621050 OR 20621051 OR 20621052 OR 20621053 OR 20621054 OR 20621055 OR 20621056 OR 20622871 OR 20622872 OR 20622873 OR 20624589 OR 20624590 OR 20624591 OR 20624592 OR 20624593 OR 20624594 OR 20624595 OR 20624596 OR 20624597 OR 20624598 OR 20624599 OR 20639873 OR 20639874 OR 20639875 OR 20657591 OR 20657592 OR 20670829 OR 20670830 OR 20670831 OR 20670832 OR 20670833 OR 20670834 OR 20670835 OR 20670836 OR 20670837 OR 20670838 OR 20670839 OR 20676103 OR 20676104 OR 20676105 OR 20680010 OR 20682443 OR 20682445 OR 20682446 OR 20682447 OR 20682448 OR 20682449 OR 20682450 OR 20682451 OR 20694001 OR 20694002 OR 20694003 OR 20694004 OR 20711183 OR 20711184 OR 20711185 OR 20711186 OR 20727844 OR 20729843 OR 20729844 OR 20729845 OR 20729846 OR 20797533 OR 20797535 OR 20797536 OR 20797537 OR 20797538 OR 20797540 OR 20797541 OR 20797542 OR 20802489 OR 20802490 OR 20804965 OR 20804969 OR 20804970 OR 20804971 OR 20804972 OR 20804973 OR 20804974 OR 20804975 OR 20818384 OR 20818385 OR 20818386 OR 20826301 OR 20826302 OR 20826303 OR 20826308 OR 20826309 OR 20826310 OR 20826311 OR 20826312 OR 20826313 OR 20826314 OR 20826315 OR 20826316 OR 20826317 OR 20826318 OR 20835249 OR 20835250 OR 20835251 OR 20835252 OR 20835253 OR 20852623 OR 20852624 OR 20852625 OR 20852626 OR 20869591 OR 20869592 OR 20869593 OR 20869594 OR 20869595 OR 20869596 OR 20869597 OR 20869598 OR 20869599 OR 20869600 OR 20869601 OR 20871602 OR 20871603 OR 20887947 OR 20887952 OR 20887953 OR 20887954 OR 20887955 OR 20887956 OR 20887957 OR 20887958 OR 20888316 OR 20890293 OR 20890294 OR 20890295 OR 20890296 OR 20920788 OR 20920789 OR 20920790 OR 20920791 OR 20920792 OR 20920793 OR 20920794 OR 20920795 OR 20920796 OR 20920797 OR 20935640 OR 20935641 OR 20935642 OR 20935643 OR 20935644 OR 20935645 OR 20953193 OR 20953194 OR 20953195 OR 20953196 OR 20953197 OR 20955921 OR 20955922 OR 20955923 OR 20955925 OR 20955927 OR 20955931 OR 20975754 OR 20975755 OR 20975756 OR 21040839 OR 21040842 OR 21040843 OR 21040844 OR 21040845 OR 21040846 OR 21040847 OR 21040848 OR 21040849 OR 21040850 OR 21040851 OR 21040852 OR 21040853 OR 21040854 OR 21040855 OR 21040856 OR 21040895 OR 21040897 OR 21040898 OR 21040899 OR 21040900 OR 21040901 OR 21040902 OR 21040903 OR 21076425 OR 21076426 OR 21102449 OR 21102451 OR 21112562 OR 21112563 OR 21112564 OR 21112565 OR 21112566 OR 21112567 OR 21112568 OR 21113162 OR 21131950 OR 21131951 OR 21131952 OR 21131953 OR 21131954 OR 21131955 OR 21144998 OR 21145001 OR 21145003 OR 21145004 OR 21145005 OR 21145006 OR 21145008 OR 21145009 OR 21145010 OR 21145011 OR 21150916 OR 21151119 OR 21151120 OR 21151121 OR 21167805 OR 21170052 OR 21170053 OR 21170054 OR 21170055 OR 21170056 OR 21185252 OR 21186355 OR 21186356 OR 21186357 OR 21186358 OR 21186359 OR 21186360 OR 21187849 OR 21209617 OR 21211781 OR 21211782 OR 21211783 OR 21211784 OR 21211785 OR 21217762 OR 21217763 OR 21217764 OR 21217765 OR 21220097 OR 21220098 OR 21220099 OR 21220100 OR 21220101 OR 21220102 OR 21220103 OR 21220104 OR 21220105 OR 21220106 OR 21220107 OR 21240273 OR 21258326 OR 21258327 OR 21258328 OR 21262461 OR 21262462 OR 21262463 OR 21262464 OR 21262465 OR 21262466 OR 21262467 OR 21262468 OR 21262469 OR 21262470 OR 21262471 OR 21262472 OR 21262473 OR 21262474 OR 21270780 OR 21270781 OR 21270782 OR 21278728 OR 21278729 OR 21278730 OR 21278732 OR 21278733 OR 21295269 OR 21295271 OR 21295272 OR 21295273 OR 21295274 OR 21295275 OR 21295276 OR 21295277 OR 21295278 OR 21297628 OR 21297629 OR 21297630 OR 21297631 OR 21317905 OR 21317906 OR 21336270 OR 21336271 OR 21336272 OR 21338871 OR 21338872 OR 21338873 OR 21338881 OR 21338882 OR 21338883 OR 21338884 OR 21338885 OR 21338886 OR 21338887 OR 21338888 OR 21358640 OR 21358641 OR 21358642 OR 21358643 OR 21358644 OR 21358645 OR 21362566 OR 21362567 OR 21362568 OR 21362569 OR 21362570 OR 21362571 OR 21362572 OR 21362573 OR 21378970 OR 21378972 OR 21378973 OR 21378974 OR 21382548 OR 21382549 OR 21382550 OR 21382551 OR 21382552 OR 21382553 OR 21382554 OR 21382555 OR 21382556 OR 21382557 OR 21382558 OR 21382559 OR 21382560 OR 21399631 OR 21399632 OR 21419747 OR 21423190 OR 21423191 OR 21435553 OR 21435554 OR 21435556 OR 21435557 OR 21435558 OR 21435559 OR 21435560 OR 21435561 OR 21435562 OR 21435563 OR 21441919 OR 21441920 OR 21441921 OR 21441922 OR 21441923 OR 21441924 OR 21441925 OR 21458401 OR 21460831 OR 21460832 OR 21460833 OR 21460834 OR 21474098 OR 21474100 OR 21474101 OR 21474102 OR 21474103 OR 21474104 OR 21474105 OR 21474106 OR 21474107 OR 21478884 OR 21478885 OR 21478886 OR 21478887 OR 21499253 OR 21499254 OR 21499255 OR 21516098 OR 21516099 OR 21516100 OR 21516101 OR 21516102 OR 21521610 OR 21521611 OR 21521612 OR 21521614 OR 21521615 OR 21521618 OR 21521619 OR 21521620 OR 21532576 OR 21532577 OR 21532578 OR 21532579 OR 21532580 OR 21549321 OR 21549325 OR 21549326 OR 21549327 OR 21549328 OR 21549329 OR 21549330 OR 21549331 OR 21552273 OR 21552274 OR 21552275 OR 21555070 OR 21555071 OR 21555072 OR 21555073 OR 21555074 OR 21555075 OR 21555076 OR 21555077 OR 21555078 OR 21555079 OR 21572432 OR 21572433 OR 21572434 OR 21596650 OR 21602821 OR 21602822 OR 21620789 OR 21623361 OR 21623362 OR 21623363 OR 21623364 OR 21623365 OR 21624809 OR 21624810 OR 21624811 OR 21624812 OR 21624813 OR 21642972 OR 21642973 OR 21642974 OR 21642975 OR 21642976 OR 21658579 OR 21658580 OR 21658581 OR 21658583 OR 21658584 OR 21658585 OR 21658586 OR 21658587 OR 21658590 OR 21658591 OR 21666671 OR 21666672 OR 21666673 OR 21666674 OR 21683670 OR 21685916 OR 21685917 OR 21685918 OR 21685919 OR 21689595 OR 21689596 OR 21689598 OR 21689599 OR 21689600 OR 21689601 OR 21689602 OR 21689603 OR 21689604 OR 21689605 OR 21706017 OR 21706018 OR 21706020 OR 21706021 OR 21725311 OR 21725312 OR 21725313 OR 21725314 OR 21725315 OR 21726828 OR 21726829 OR 21726830 OR 21726831 OR 21726832 OR 21726833 OR 21726834 OR 21743470 OR 21743471 OR 21743472 OR 21743473 OR 21745635 OR 21745638 OR 21745639 OR 21745640 OR 21745641 OR 21745642 OR 21745643 OR 21745644 OR 21745645 OR 21745646 OR 21745647 OR 21750548 OR 21765421 OR 21765422 OR 21765423 OR 21765424 OR 21765425 OR 21765426 OR 21785434 OR 21785435 OR 21785436 OR 21791283 OR 21791284 OR 21791285 OR 21791286 OR 21791288 OR 21791289 OR 21791290 OR 21791291 OR 21791292 OR 21791294 OR 21792192 OR 21802386 OR 21804537 OR 21804538 OR 21816361 OR 21816363 OR 21816364 OR 21816365 OR 21816366 OR 21816367 OR 21822269 OR 21822270 OR 21822271 OR 21835340 OR 21835341 OR 21835342 OR 21835343 OR 21835344 OR 21835345 OR 21835346 OR 21835347 OR 21835348 OR 21835349 OR 21841774 OR 21841775 OR 21841776 OR 21841777 OR 21852222 OR 21857656 OR 21857657 OR 21857658 OR 21857659 OR 21867878 OR 21867879 OR 21867880 OR 21867881 OR 21867882 OR 21867883 OR 21867884 OR 21867885 OR 21867886 OR 21867887 OR 21867888 OR 21867889 OR 21874013 OR 21874014 OR 21874015 OR 21874016 OR 21874017 OR 21878933 OR 21885013 OR 21885015 OR 21885018 OR 21885019 OR 21885020 OR 21885021 OR 21885022 OR 21892154 OR 21892155 OR 21892156 OR 21892157 OR 21903074 OR 21903075 OR 21903077 OR 21903078 OR 21903079 OR 21903080 OR 21903082 OR 21903083 OR 21903084 OR 21903085 OR 21909085 OR 21909086 OR 21909087 OR 21909088 OR 21909089 OR 21909090 OR 21926982 OR 21926983 OR 21926984 OR 21926985 OR 21943598 OR 21943599 OR 21943600 OR 21943601 OR 21943602 OR 21943603 OR 21943604 OR 21943605 OR 21943606 OR 21943607 OR 21943608 OR 21943609 OR 21944778 OR 21944779 OR 21946326 OR 21946327 OR 21946328 OR 21962918 OR 21964488 OR 21964489 OR 21964490 OR 21982232 OR 21982233 OR 21982234 OR 21982235 OR 21982236 OR 21982367 OR 21982368 OR 21982369 OR 21982370 OR 21982371 OR 21982372 OR 21982373 OR 21982374 OR 21982375 OR 21982376 OR 21982377 OR 21982378 OR 21983681 OR 21983682 OR 21983683 OR 21983684 OR 22002768 OR 22017985 OR 22017987 OR 22017988 OR 22017989 OR 22017990 OR 22017991 OR 22017992 OR 22017993 OR 22017994 OR 22017995 OR 22017996 OR 22017997 OR 22019014 OR 22019730 OR 22019731 OR 22019732 OR 22030546 OR 22030547 OR 22030551 OR 22037496 OR 22037498 OR 22037499 OR 22037500 OR 22037501 OR 22056139 OR 22056140 OR 22056141 OR 22056142 OR 22056143 OR 22057188 OR 22057189 OR 22057190 OR 22057191 OR 22057192 OR 22057193 OR 22078507 OR 22081156 OR 22081157 OR 22081158 OR 22081159 OR 22081160 OR 22081161 OR 22100412 OR 22101640 OR 22101641 OR 22101642 OR 22101643 OR 22101644 OR 22101645 OR 22119902 OR 22119903 OR 22136926 OR 22136928 OR 22136929 OR 22136930 OR 22136931 OR 22136932 OR 22138642 OR 22138643 OR 22138644 OR 22138645 OR 22138646 OR 22138647 OR 22153366 OR 22153367 OR 22153369 OR 22153370 OR 22153371 OR 22153372 OR 22153373 OR 22153374 OR 22153375 OR 22153376 OR 22153377 OR 22153378 OR 22153379 OR 22153380 OR 22153381 OR 22158510 OR 22158511 OR 22158512 OR 22158513 OR 22158514 OR 22179109 OR 22179110 OR 22179111 OR 22179112 OR 22179113 OR 22197828 OR 22197830 OR 22197831 OR 22197832 OR 22197833 OR 22226352 OR 22226354 OR 22226355 OR 22226356 OR 22226357 OR 22226358 OR 22226359 OR 22231425 OR 22231426 OR 22231427 OR 22231428 OR 22243744 OR 22243745 OR 22243746 OR 22243747 OR 22243748 OR 22243750 OR 22243751 OR 22243752 OR 22243753 OR 22243754 OR 22243755 OR 22243756 OR 22243757 OR 22246433 OR 22246434 OR 22246435 OR 22246436 OR 22246437 OR 22246438 OR 22267160 OR 22267161 OR 22267162 OR 22267163 OR 22281715 OR 22284180 OR 22284181 OR 22284182 OR 22284183 OR 22284184 OR 22284185 OR 22284186 OR 22284187 OR 22284188 OR 22284189 OR 22284190 OR 22284191 OR 22286174 OR 22286175 OR 22305565 OR 22305566 OR 22305567 OR 22305568 OR 22305569 OR 22305570 OR 22305571 OR 22306606 OR 22306607 OR 22306608 OR 22325196 OR 22325198 OR 22325199 OR 22325200 OR 22325201 OR 22325202 OR 22325203 OR 22325204 OR 22325205 OR 22325206 OR 22325207 OR 22325208 OR 22325209 OR 22325210 OR 22327473 OR 22365540 OR 22365542 OR 22365543 OR 22365544 OR 22365545 OR 22365546 OR 22365547 OR 22365548 OR 22365549 OR 22365550 OR 22365552 OR 22365553 OR 22365554 OR 22385654 OR 22385655 OR 22385656 OR 22385657 OR 22385658 OR 22385659 OR 22385660 OR 22405201 OR 22405202 OR 22405203 OR 22405206 OR 22405207 OR 22405208 OR 22405209 OR 22405210 OR 22405211 OR 22405212 OR 22406547 OR 22406549 OR 22406551 OR 22424902 OR 22426252 OR 22426253 OR 22426255 OR 22445337 OR 22445338 OR 22445339 OR 22445341 OR 22445342 OR 22445343 OR 22445344 OR 22445345 OR 22445346 OR 22445347 OR 22445348 OR 22445349 OR 22445517 OR 22445518 OR 22446878 OR 22446880 OR 22446881 OR 22446882 OR 22449960 OR 22466505 OR 22466506 OR 22482503 OR 22482504 OR 22482505 OR 22482506 OR 22482507 OR 22482508 OR 22484571 OR 22486005 OR 22500627 OR 22500628 OR 22500629 OR 22500630 OR 22500631 OR 22500632 OR 22500633 OR 22500634 OR 22500635 OR 22500636 OR 22500637 OR 22500638 OR 22500639 OR 22500640 OR 22504346 OR 22522400 OR 22522401 OR 22522402 OR 22542159 OR 22542160 OR 22542177 OR 22542180 OR 22542181 OR 22542182 OR 22542183 OR 22542184 OR 22542185 OR 22542186 OR 22542189 OR 22542190 OR 22542191 OR 22542192 OR 22544310 OR 22544311 OR 22544312 OR 22544313 OR 22560075 OR 22560076 OR 22560077 OR 22560078 OR 22560079 OR 22560080 OR 22560081 OR 22560082 OR 22561452 OR 22561453 OR 22561454 OR 22561455 OR 22578499 OR 22578500 OR 22578501 OR 22578502 OR 22578503 OR 22578504 OR 22578505 OR 22578506 OR 22578507 OR 22578508 OR 22581183 OR 22581184 OR 22581185 OR 22608532 OR 22610068 OR 22610069 OR 22632720 OR 22632721 OR 22632722 OR 22632723 OR 22632724 OR 22632725 OR 22632726 OR 22632727 OR 22632728 OR 22632729 OR 22632730 OR 22632731 OR 22632732 OR 22634728 OR 22634729 OR 22634730 OR 22634731 OR 22660477 OR 22660478 OR 22660479 OR 22660480 OR 22681682 OR 22681684 OR 22681685 OR 22681686 OR 22681687 OR 22681688 OR 22681689 OR 22681690 OR 22681691 OR 22681692 OR 22681693 OR 22681694 OR 22681695 OR 22681696 OR 22681697 OR 22683203 OR 22683204 OR 22683681 OR 22683682 OR 22683683 OR 22704497 OR 22704498 OR 22704499 OR 22704500 OR 22704501 OR 22704502 OR 22704503 OR 22704504 OR 22704505 OR 22704507 OR 22704510 OR 22704516 OR 22704518 OR 22706266 OR 22706267 OR 22706268 OR 22706269 OR 22706270 OR 22726828 OR 22726831 OR 22726832 OR 22726833 OR 22726834 OR 22726835 OR 22726836 OR 22726837 OR 22726838 OR 22726839 OR 22726840 OR 22726841 OR 22729174 OR 22729175 OR 22729176 OR 22729177 OR 22748967 OR 22748968 OR 22751036 OR 22770236 OR 22770237 OR 22770240 OR 22770241 OR 22770242 OR 22770243 OR 22770244 OR 22770245 OR 22770246 OR 22770845 OR 22772332 OR 22772333 OR 22794259 OR 22794260 OR 22794261 OR 22794262 OR 22794263 OR 22794264 OR 22794265 OR 22794266 OR 22794267 OR 22794268 OR 22797695 OR 22820465 OR 22820466 OR 22837034 OR 22837035 OR 22837036 OR 22837037 OR 22841310 OR 22841311 OR 22841312 OR 22841313 OR 22841314 OR 22841315 OR 22841316 OR 22841317 OR 22841318 OR 22842144 OR 22842145 OR 22842146 OR 22842147 OR 22842148 OR 22862941 OR 22862942 OR 22862943 OR 22862944 OR 22862945 OR 22862946 OR 22862947 OR 22862948 OR 22862949 OR 22863532 OR 22863533 OR 22863534 OR 22864610 OR 22864611 OR 22864612 OR 22864613 OR 22884324 OR 22884325 OR 22884327 OR 22884328 OR 22884329 OR 22884330 OR 22884331 OR 22884332 OR 22884333 OR 22884334 OR 22884335 OR 22885848 OR 22885849 OR 22885850 OR 22885851 OR 22902294 OR 22902295 OR 22902718 OR 22902719 OR 22902720 OR 22920251 OR 22920252 OR 22920253 OR 22920255 OR 22920257 OR 22920258 OR 22920259 OR 22920260 OR 22920262 OR 22922782 OR 22922783 OR 22922784 OR 22922785 OR 22922786 OR 22941107 OR 22941108 OR 22941109 OR 22941110 OR 22941111 OR 22958819 OR 22958820 OR 22958821 OR 22958822 OR 22958823 OR 22958824 OR 22958825 OR 22958828 OR 22958829 OR 22958830 OR 22958930 OR 22958931 OR 22958932 OR 22958933 OR 22958934 OR 22960931 OR 22960932 OR 22960933 OR 22960934 OR 22981823 OR 22983208 OR 22983209 OR 22983211 OR 22998867 OR 22998869 OR 22998870 OR 22998871 OR 22998872 OR 22998873 OR 22998875 OR 22998876 OR 22998877 OR 22998878 OR 22998879 OR 23001059 OR 23001060 OR 23001061 OR 23001062 OR 23023292 OR 23023293 OR 23023294 OR 23040474 OR 23040476 OR 23040477 OR 23040478 OR 23040479 OR 23040480 OR 23040481 OR 23040482 OR 23042081 OR 23042082 OR 23064101 OR 23064379 OR 23064381 OR 23064382 OR 23083732 OR 23083733 OR 23083734 OR 23083736 OR 23083737 OR 23083738 OR 23083739 OR 23083740 OR 23083741 OR 23083742 OR 23083743 OR 23083744 OR 23083745 OR 23084023 OR 23086334 OR 23086335 OR 23086336 OR 23103054 OR 23103964 OR 23103965 OR 23122285 OR 23122286 OR 23122287 OR 23122289 OR 23122290 OR 23122291 OR 23122292 OR 23122293 OR 23122294 OR 23141062 OR 23141063 OR 23141064 OR 23141065 OR 23141066 OR 23141067 OR 23141068 OR 23141069 OR 23141071 OR 23141072 OR 23141075 OR 23142520 OR 23142521 OR 23143511 OR 23143512 OR 23143513 OR 23143514 OR 23143515 OR 23143516 OR 23143517 OR 23143518 OR 23143519 OR 23143520 OR 23143521 OR 23143522 OR 23160043 OR 23160044 OR 23160045 OR 23168163 OR 23168164 OR 23177958 OR 23177959 OR 23177960 OR 23177961 OR 23177962 OR 23177963 OR 23177965 OR 23177966 OR 23177967 OR 23178974 OR 23178975 OR 23201972 OR 23217418 OR 23217419 OR 23217420 OR 23217423 OR 23217424 OR 23217425 OR 23217739 OR 23217740 OR 23217741 OR 23217742 OR 23217743 OR 23217744 OR 23217745 OR 23217746 OR 23217747 OR 23217748 OR 23217749 OR 23217750 OR 23222911 OR 23222912 OR 23222913 OR 23222914 OR 23242309 OR 23242310 OR 23242311 OR 23242312 OR 23246482 OR 23246483 OR 23259944 OR 23259945 OR 23259946 OR 23259947 OR 23259948 OR 23259949 OR 23259950 OR 23259951 OR 23259952 OR 23259953 OR 23259954 OR 23259955 OR 23259956 OR 23260487 OR 23260488 OR 23263442 OR 23263443 OR 23290135 OR 23290136 OR 23290137 OR 23290138 OR 23290139 OR 23290140 OR 23292679 OR 23292680 OR 23292681 OR 23292682 OR 23292683 OR 23312514 OR 23312515 OR 23312516 OR 23312517 OR 23312518 OR 23312519 OR 23312520 OR 23312521 OR 23312522 OR 23312523 OR 23312524 OR 23312525 OR 23312526 OR 23313908 OR 23313909 OR 23313910 OR 23313911 OR 23313912 OR 23318055 OR 23318056 OR 23333148 OR 23333149 OR 23333150 OR 23334578 OR 23334579 OR 23334580 OR 23334581 OR 23352160 OR 23352161 OR 23352162 OR 23352164 OR 23352165 OR 23352166 OR 23352167 OR 23352168 OR 23352169 OR 23352170 OR 23352171 OR 23352605 OR 23354328 OR 23354329 OR 23354330 OR 23354331 OR 23354332 OR 23354333 OR 23354385 OR 23377126 OR 23377127 OR 23377128 OR 23395371 OR 23395373 OR 23395374 OR 23395375 OR 23395376 OR 23395377 OR 23395378 OR 23395380 OR 23395381 OR 23395382 OR 23395444 OR 23395445 OR 23395446 OR 23395447 OR 23396101 OR 23396102 OR 23415312 OR 23415913 OR 23415914 OR 23415915 OR 23416448 OR 23416450 OR 23416452 OR 23434393 OR 23434911 OR 23434912 OR 23434913 OR 23434914 OR 23434978 OR 23439118 OR 23439119 OR 23439120 OR 23439121 OR 23439122 OR 23439123 OR 23439124 OR 23439125 OR 23439126 OR 23439127 OR 23439128 OR 23439129 OR 23455607 OR 23455608 OR 23455609 OR 23455610 OR 23472870 OR 23472872 OR 23472873 OR 23472874 OR 23473315 OR 2</t>
-  </si>
-  <si>
-    <t>PMID=(27989770 OR 27991897 OR 27991898 OR 27991899 OR 27991900 OR 27991901 OR 28009267 OR 28009268 OR 28009269 OR 28009270 OR 28009271 OR 28009272 OR 28009274 OR 28009276 OR 28009277 OR 28009278 OR 28017470 OR 28017471 OR 28017472 OR 28017794 OR 28017795 OR 28017796 OR 28024158 OR 28024159 OR 28025983 OR 28025984 OR 28041881 OR 28041882 OR 28041883 OR 28041884 OR 28041894 OR 28041895 OR 28041896 OR 28056340 OR 28056342 OR 28056344 OR 28056345 OR 28056346 OR 28056347 OR 28061350 OR 28065650 OR 28067902 OR 28067903 OR 28067904 OR 28067905 OR 28089908 OR 28089909 OR 28089910 OR 28092659 OR 28094016 OR 28094017 OR 28094018 OR 28103471 OR 28103472 OR 28103473 OR 28103474 OR 28103478 OR 28103479 OR 28103480 OR 28103481 OR 28103482 OR 28103483 OR 28111077 OR 28111080 OR 28111081 OR 28111082 OR 28111199 OR 28111200 OR 28111201 OR 28114293 OR 28114294 OR 28114295 OR 28114296 OR 28132824 OR 28132825 OR 28132826 OR 28132827 OR 28132828 OR 28132829 OR 28132830 OR 28132833 OR 28132834 OR 28132835 OR 28135239 OR 28135240 OR 28135241 OR 28135242 OR 28135243 OR 28157497 OR 28162806 OR 28162807 OR 28162808 OR 28162809 OR 28166219 OR 28166220 OR 28166221 OR 28182899 OR 28182900 OR 28182901 OR 28182902 OR 28182903 OR 28182906 OR 28190640 OR 28190641 OR 28190642 OR 28190643 OR 28192394 OR 28192395 OR 28192396 OR 28196600 OR 28196601 OR 28215557 OR 28215558 OR 28215559 OR 28215825 OR 28218914 OR 28218915 OR 28218916 OR 28218917 OR 28231464 OR 28231465 OR 28231466 OR 28231467 OR 28231468 OR 28231469 OR 28231470 OR 28238546 OR 28238547 OR 28238549 OR 28238551 OR 28250408 OR 28250409 OR 28253233 OR 28262416 OR 28262417 OR 28263300 OR 28263301 OR 28263302 OR 28279351 OR 28279352 OR 28279353 OR 28279354 OR 28279355 OR 28279356 OR 28285819 OR 28285820 OR 28285821 OR 28285822 OR 28285823 OR 28285824 OR 28285903 OR 28285904 OR 28285905 OR 28288124 OR 28288125 OR 28288126 OR 28288127 OR 28288128 OR 28318784 OR 28319608 OR 28319609 OR 28319610 OR 28330582 OR 28334598 OR 28334599 OR 28334600 OR 28334601 OR 28334602 OR 28334606 OR 28334607 OR 28334608 OR 28334609 OR 28334610 OR 28334611 OR 28334612 OR 28343864 OR 28343865 OR 28343867 OR 28343868 OR 28343869 OR 28343982 OR 28343983 OR 28343984 OR 28346452 OR 28346453 OR 28366587 OR 28366588 OR 28366589 OR 28368384 OR 28368385 OR 28384467 OR 28384468 OR 28384469 OR 28384470 OR 28384472 OR 28384475 OR 28384476 OR 28384479 OR 28388428 OR 28388429 OR 28388430 OR 28388431 OR 28388432 OR 28392070 OR 28392071 OR 28392072 OR 28394322 OR 28394323 OR 28394324 OR 28414331 OR 28414332 OR 28414333 OR 28416077 OR 28426960 OR 28426961 OR 28426962 OR 28426963 OR 28426964 OR 28426965 OR 28426966 OR 28426967 OR 28426968 OR 28426969 OR 28426970 OR 28426971 OR 28434800 OR 28434801 OR 28434802 OR 28436980 OR 28436981 OR 28436982 OR 28457596 OR 28457748 OR 28457749 OR 28457750 OR 28459441 OR 28459442 OR 28472644 OR 28472645 OR 28472646 OR 28472647 OR 28472651 OR 28472653 OR 28472654 OR 28472656 OR 28472659 OR 28472660 OR 28472661 OR 28475884 OR 28481348 OR 28481349 OR 28481350 OR 28504117 OR 28504671 OR 28504672 OR 28504673 OR 28506464 OR 28506465 OR 28521119 OR 28521120 OR 28521121 OR 28521122 OR 28521123 OR 28521124 OR 28521125 OR 28521129 OR 28521130 OR 28521131 OR 28521132 OR 28521133 OR 28521134 OR 28521135 OR 28521138 OR 28521139 OR 28521140 OR 28521141 OR 28526555 OR 28530661 OR 28530662 OR 28530663 OR 28530664 OR 28552314 OR 28553943 OR 28553944 OR 28581479 OR 28581480 OR 28602620 OR 28602689 OR 28604683 OR 28604684 OR 28604685 OR 28625485 OR 28625486 OR 28625487 OR 28625488 OR 28628100 OR 28628101 OR 28628102 OR 28628103 OR 28628104 OR 28641101 OR 28641102 OR 28641103 OR 28641104 OR 28641105 OR 28641109 OR 28641110 OR 28641111 OR 28641112 OR 28641113 OR 28641114 OR 28641115 OR 28641116 OR 28648363 OR 28648364 OR 28648365 OR 28648497 OR 28648498 OR 28648499 OR 28648500 OR 28669543 OR 28669544 OR 28669545 OR 28669546 OR 28671691 OR 28671692 OR 28671693 OR 28671694 OR 28671695 OR 28671696 OR 28683262 OR 28683263 OR 28683264 OR 28683266 OR 28683267 OR 28683269 OR 28683270 OR 28683271 OR 28683272 OR 28683273 OR 28686860 OR 28686865 OR 28686870 OR 28689980 OR 28689981 OR 28689982 OR 28689983 OR 28689984 OR 28692061 OR 28692062 OR 28712652 OR 28712653 OR 28712654 OR 28712938 OR 28714951 OR 28714952 OR 28714953 OR 28714954 OR 28728018 OR 28728022 OR 28728023 OR 28728024 OR 28728025 OR 28728026 OR 28735746 OR 28735747 OR 28735748 OR 28735749 OR 28735750 OR 28736215 OR 28736216 OR 28736217 OR 28757304 OR 28757305 OR 28757306 OR 28757360 OR 28758994 OR 28758995 OR 28758996 OR 28758997 OR 28758998 OR 28758999 OR 28772121 OR 28772122 OR 28772123 OR 28772124 OR 28772125 OR 28777942 OR 28777944 OR 28777945 OR 28777946 OR 28781167 OR 28781168 OR 28781169 OR 28783139 OR 28783140 OR 28803732 OR 28803918 OR 28803919 OR 28803920 OR 28805814 OR 28805815 OR 28805816 OR 28817792 OR 28817793 OR 28817794 OR 28817795 OR 28817796 OR 28817799 OR 28817800 OR 28817801 OR 28817802 OR 28817804 OR 28817805 OR 28823726 OR 28823728 OR 28823729 OR 28823730 OR 28825718 OR 28825719 OR 28826723 OR 28844526 OR 28844837 OR 28846081 OR 28846083 OR 28858611 OR 28858614 OR 28858616 OR 28858617 OR 28858618 OR 28858619 OR 28858621 OR 28858624 OR 28858625 OR 28858626 OR 28858627 OR 28867551 OR 28867552 OR 28869581 OR 28869582 OR 28869583 OR 28869584 OR 28886366 OR 28886367 OR 28890345 OR 28892057 OR 28892058 OR 28910611 OR 28910612 OR 28910613 OR 28910614 OR 28910615 OR 28910619 OR 28910620 OR 28910621 OR 28910622 OR 28910623 OR 28910624 OR 28919175 OR 28919367 OR 28920932 OR 28920933 OR 28920934 OR 28920935 OR 28920936 OR 28943028 OR 28943029 OR 28943231 OR 28945220 OR 28945221 OR 28945222 OR 28957662 OR 28957663 OR 28957664 OR 28957665 OR 28957667 OR 28957668 OR 28957669 OR 28957670 OR 28957671 OR 28957674 OR 28957677 OR 28957678 OR 28957679 OR 28957680 OR 28957681 OR 28965765 OR 28965766 OR 28965767 OR 28965997 OR 28967909 OR 28967910 OR 28985523 OR 28985524 OR 28985526 OR 28985527 OR 28985528 OR 28985529 OR 29024648 OR 29024650 OR 29024651 OR 29024657 OR 29024658 OR 29024659 OR 29024660 OR 29024661 OR 29024662 OR 29024663 OR 29024664 OR 29024665 OR 29024666 OR 29024667 OR 29024668 OR 29024669 OR 29033205 OR 29033351 OR 29033352 OR 29033353 OR 29056294 OR 29056295 OR 29056296 OR 29056297 OR 29056298 OR 29056299 OR 29100010 OR 29100012 OR 29100013 OR 29100014 OR 29100015 OR 29103804 OR 29103805 OR 29103806 OR 29103807 OR 29103808 OR 29107517 OR 29107518 OR 29107519 OR 29107520 OR 29107521 OR 29107522 OR 29107523 OR 29129523 OR 29144974 OR 29154125 OR 29154126 OR 29154127 OR 29154128 OR 29154129 OR 29154130 OR 29174331 OR 29174332 OR 29174333 OR 29180747 OR 29180748 OR 29184197 OR 29184198 OR 29184199 OR 29184200 OR 29184201 OR 29184202 OR 29184203 OR 29184204 OR 29184206 OR 29184207 OR 29184208 OR 29184209 OR 29184212 OR 29198754 OR 29198756 OR 29198757 OR 29198940 OR 29198941 OR 29198942 OR 29203896 OR 29203897 OR 29216448 OR 29216449 OR 29216450 OR 29216451 OR 29220665 OR 29220666 OR 29220667 OR 29224721 OR 29224722 OR 29224723 OR 29224724 OR 29224725 OR 29224726 OR 29224727 OR 29230051 OR 29230052 OR 29230053 OR 29230054 OR 29230055 OR 29230056 OR 29230057 OR 29230058 OR 29230059 OR 29249282 OR 29249283 OR 29249284 OR 29249285 OR 29249286 OR 29249287 OR 29249288 OR 29249289 OR 29249462 OR 29249463 OR 29249464 OR 29268095 OR 29268096 OR 29268097 OR 29268098 OR 29268099 OR 29273772 OR 29276054 OR 29276055 OR 29276056 OR 29276141 OR 29276142 OR 29276143 OR 29290548 OR 29290549 OR 29290550 OR 29290552 OR 29290553 OR 29290554 OR 29290616 OR 29290617 OR 29292378 OR 29301098 OR 29301100 OR 29301106 OR 29304339 OR 29304344 OR 29307709 OR 29307710 OR 29307712 OR 29311741 OR 29311742 OR 29311743 OR 29311744 OR 29311745 OR 29311746 OR 29335603 OR 29335604 OR 29335605 OR 29335606 OR 29335607 OR 29335608 OR 29337181 OR 29337182 OR 29337183 OR 29346752 OR 29346754 OR 29358017 OR 29358044 OR 29358666 OR 29379116 OR 29379117 OR 29395054 OR 29395055 OR 29395056 OR 29395906 OR 29395907 OR 29395908 OR 29395909 OR 29395910 OR 29395911 OR 29395912 OR 29395913 OR 29395914 OR 29395915 OR 29395916 OR 29397273 OR 29398355 OR 29398356 OR 29398357 OR 29398358 OR 29398359 OR 29398360 OR 29398361 OR 29398362 OR 29398363 OR 29398364 OR 29398365 OR 29398366 OR 29403029 OR 29403030 OR 29403032 OR 29403033 OR 29403034 OR 29420933 OR 29420934 OR 29420935 OR 29429933 OR 29429934 OR 29429935 OR 29429936 OR 29429937 OR 29429938 OR 29429939 OR 29429943 OR 29434375 OR 29434377 OR 29451855 OR 29456026 OR 29456158 OR 29456159 OR 29459763 OR 29459764 OR 29463850 OR 29470967 OR 29472620 OR 29478844 OR 29478915 OR 29478916 OR 29478917 OR 29483663 OR 29483664 OR 29499147 OR 29499153 OR 29499154 OR 29499155 OR 29503184 OR 29503185 OR 29503186 OR 29503187 OR 29503188 OR 29503189 OR 29503190 OR 29503191 OR 29503192 OR 29507408 OR 29507409 OR 29507410 OR 29507411 OR 29507412 OR 29507413 OR 29507414 OR 29518356 OR 29518357 OR 29518358 OR 29518359 OR 29526553 OR 29526554 OR 29531361 OR 29531362 OR 29531364 OR 29551301 OR 29551489 OR 29551490 OR 29551491 OR 29551492 OR 29551493 OR 29556025 OR 29556028 OR 29556029 OR 29556030 OR 29566793 OR 29566794 OR 29576387 OR 29576388 OR 29576389 OR 29576390 OR 29606579 OR 29606580 OR 29606581 OR 29606582 OR 29621484 OR 29621485 OR 29621487 OR 29621490 OR 29625067 OR 29625068 OR 29625069 OR 29625070 OR 29625071 OR 29625072 OR 29628186 OR 29628187 OR 29628188 OR 29632359 OR 29632360 OR 29632361 OR 29656871 OR 29656872 OR 29656873 OR 29656874 OR 29656875 OR 29656876 OR 29656941 OR 29656943 OR 29662213 OR 29662214 OR 29662216 OR 29662217 OR 29673481 OR 29673482 OR 29673483 OR 29673484 OR 29673485 OR 29681515 OR 29681516 OR 29681530 OR 29681531 OR 29681532 OR 29681533 OR 29681534 OR 29686260 OR 29686261 OR 29686262 OR 29706577 OR 29706582 OR 29706583 OR 29706584 OR 29706585 OR 29713079 OR 29713080 OR 29727680 OR 29727681 OR 29727682 OR 29727683 OR 29731251 OR 29731252 OR 29731253 OR 29754750 OR 29754752 OR 29754754 OR 29754779 OR 29760525 OR 29760527 OR 29772202 OR 29772203 OR 29779889 OR 29779890 OR 29779891 OR 29779941 OR 29779943 OR 29786081 OR 29786082 OR 29786083 OR 29786085 OR 29802388 OR 29802390 OR 29802391 OR 29804889 OR 29804890 OR 29804891 OR 29804919 OR 29804920 OR 29859170 OR 29859171 OR 29861281 OR 29861282 OR 29861283 OR 29861284 OR 29861285 OR 29861286 OR 29867081 OR 29879384 OR 29879392 OR 29887317 OR 29887318 OR 29887338 OR 29887339 OR 29887340 OR 29892048 OR 29909995 OR 29909996 OR 29909997 OR 29909998 OR 29909999 OR 29910000 OR 29910149 OR 29910151 OR 29915192 OR 29915193 OR 29915194 OR 29915195 OR 29937200 OR 29937201 OR 29937202 OR 29937203 OR 29937275 OR 29937276 OR 29937277 OR 29937279 OR 29937281 OR 29942037 OR 29950668 OR 29950669 OR 29950670 OR 29953872 OR 29979986 OR 29979988 OR 29979993 OR 29983322 OR 29983323 OR 29983324 OR 29983325 OR 29983327 OR 29988069 OR 30001507 OR 30001512 OR 30008297 OR 30008298 OR 30013171 OR 30017392 OR 30017393 OR 30017394 OR 30017395 OR 30017396 OR 30017589 OR 30017590 OR 30017591 OR 30033119 OR 30033120 OR 30033151 OR 30033152 OR 30033153 OR 30033154 OR 30038273 OR 30038275 OR 30038276 OR 30038277 OR 30038279 OR 30038280 OR 30038282 OR 30048615 OR 30049452 OR 30050107 OR 30056831 OR 30056832 OR 30057201 OR 30057202 OR 30057203 OR 30057204 OR 30057205 OR 30057206 OR 30075129 OR 30075130 OR 30077356 OR 30078576 OR 30078577 OR 30078578 OR 30078579 OR 30078580 OR 30082067 OR 30082068 OR 30082915 OR 30092214 OR 30092215 OR 30100166 OR 30100167 OR 30100168 OR 30100254 OR 30100255 OR 30100256 OR 30104731 OR 30104732 OR 30104733 OR 30104734 OR 30122373 OR 30122374 OR 30122375 OR 30122377 OR 30122378 OR 30122379 OR 30122380 OR 30122381 OR 30122475 OR 30122476 OR 30127424 OR 30127427 OR 30127430 OR 30138589 OR 30138590 OR 30138591 OR 30146299 OR 30146300 OR 30146301 OR 30146302 OR 30146303 OR 30146304 OR 30146305 OR 30146306 OR 30146307 OR 30146308 OR 30146410 OR 30146411 OR 30146412 OR 30150661 OR 30150662 OR 30150663 OR 30154505 OR 30154506 OR 30174114 OR 30174115 OR 30174116 OR 30174117 OR 30174118 OR 30174119 OR 30174295 OR 30174296 OR 30174297 OR 30177795 OR 30189202 OR 30189209 OR 30197236 OR 30197237 OR 30220509 OR 30220510 OR 30220511 OR 30220512 OR 30220521 OR 30224803 OR 30224804 OR 30224805 OR 30224807 OR 30224808 OR 30224809 OR 30224810 OR 30236284 OR 30236285 OR 30244867 OR 30244869 OR 30244870 OR 30244883 OR 30244884 OR 30244885 OR 30244886 OR 30250263 OR 30258238 OR 30258239 OR 30269902 OR 30269903 OR 30269904 OR 30269986 OR 30269987 OR 30269988 OR 30269989 OR 30269990 OR 30269991 OR 30269992 OR 30269993 OR 30290177 OR 30290178 OR 30290179 OR 30290982 OR 30293821 OR 30293822 OR 30293823 OR 30297807 OR 30308165 OR 30308166 OR 30308173 OR 30318302 OR 30318303 OR 30318409 OR 30318410 OR 30318411 OR 30318412 OR 30318413 OR 30318414 OR 30318415 OR 30318416 OR 30323275 OR 30323276 OR 30344040 OR 30344041 OR 30344042 OR 30344043 OR 30344044 OR 30344045 OR 30344046 OR 30344047 OR 30344048 OR 30344100 OR 30349100 OR 30349101 OR 30349103 OR 30349104 OR 30349105 OR 30349106 OR 30349107 OR 30349110 OR 30349111 OR 30361547 OR 30382196 OR 30392793 OR 30392794 OR 30392795 OR 30392796 OR 30392797 OR 30392798 OR 30392799 OR 30392800 OR 30397325 OR 30401455 OR 30408443 OR 30408444 OR 30415993 OR 30415995 OR 30415996 OR 30415998 OR 30416070 OR 30416071 OR 30416072 OR 30420732 OR 30449656 OR 30449657 OR 30449714 OR 30449715 OR 30455454 OR 30455455 OR 30455456 OR 30455457 OR 30455458 OR 30465766 OR 30467079 OR 30467080 OR 30472076 OR 30472077 OR 30472156 OR 30472157 OR 30472158 OR 30473013 OR 30473014 OR 30482688 OR 30482689 OR 30482690 OR 30482691 OR 30482692 OR 30482693 OR 30482694 OR 30482945 OR 30482946 OR 30482947 OR 30482948 OR 30482949 OR 30497771 OR 30497772 OR 30502044 OR 30503141 OR 30503142 OR 30503143 OR 30503172 OR 30503173 OR 30503644 OR 30503645 OR 30521777 OR 30521779 OR 30522820 OR 30526881 OR 30526882 OR 30528064 OR 30528065 OR 30528555 OR 30545599 OR 30551997 OR 30551998 OR 30553546 OR 30554781 OR 30554961 OR 30554962 OR 30554964 OR 30559469 OR 30559470 OR 30559471 OR 30559472 OR 30559475 OR 30559476 OR 30559478 OR 30559479 OR 30559480 OR 30573346 OR 30578106 OR 30581011 OR 30581012 OR 30581079 OR 30581080 OR 30594427 OR 30595332 OR 30595499 OR 30598527 OR 30606613 OR 30606614 OR 30609396 OR 30617257 OR 30617258 OR 30635232 OR 30638744 OR 30638745 OR 30638901 OR 30638902 OR 30639035 OR 30639036 OR 30639037 OR 30643291 OR 30643292 OR 30643294 OR 30643295 OR 30643296 OR 30643297 OR 30643298 OR 30643299 OR 30653935 OR 30654923 OR 30654924 OR 30658859 OR 30658860 OR 30661738 OR 30661739 OR 30661958 OR 30661959 OR 30661960 OR 30664766 OR 30664767 OR 30664768 OR 30664769 OR 30664770 OR 30664771 OR 30664772 OR 30679017 OR 30679018 OR 30683545 OR 30683546 OR 30685224 OR 30686732 OR 30686733 OR 30686763 OR 30686764 OR 30686765 OR 30692687 OR 30692688 OR 30692689 OR 30692690 OR 30692691 OR 30704910 OR 30704911 OR 30709656 OR 30711355 OR 30713093 OR 30713094 OR 30718900 OR 30718902 OR 30718903 OR 30718904 OR 30731062 OR 30733148 OR 30733149 OR 30733150 OR 30737130 OR 30742114 OR 30742115 OR 30742116 OR 30742117 OR 30744986 OR 30744987 OR 30765165 OR 30765166 OR 30770252 OR 30770301 OR 30778148 OR 30778149 OR 30792150 OR 30795900 OR 30795902 OR 30799020 OR 30799021 OR 30799279 OR 30804529 OR 30804530 OR 30819547 OR 30824353 OR 30833699 OR 30833700 OR 30846309 OR 30849366 OR 30849367 OR 30850257 OR 30853298 OR 30853299 OR 30853300 OR 30853556 OR 30853557 OR 30853558 OR 30858601 OR 30858603 OR 30858604 OR 30858605 OR 30871858 OR 30871859 OR 30876848 OR 30876849 OR 30878289 OR 30879785 OR 30880024 OR 30880025 OR 30880026 OR 30886406 OR 30886407 OR 30886408 OR 30902550 OR 30905618 OR 30905619 OR 30905620 OR 30911182 OR 30911183 OR 30911184 OR 30911185 OR 30926280 OR 30928170 OR 30930044 OR 30930145 OR 30930146 OR 30930147 OR 30936555 OR 30936556 OR 30936557 OR 30936558 OR 30951662 OR 30962628 OR 30962630 OR 30962632 OR 30979537 OR 30981533 OR 30982627 OR 30982770 OR 30982771 OR 30988523 OR 30988524 OR 30988525 OR 30988526 OR 30988527 OR 31003725 OR 31005376 OR 31006620 OR 31006621 OR 31006622 OR 31011224 OR 31011226 OR 31011227 OR 31023509 OR 31027966 OR 31029403 OR 31030955 OR 31031137 OR 31031138 OR 31031139 OR 31036941 OR 31036942 OR 31036944 OR 31036945 OR 31036947 OR 31047778 OR 31047779 OR 31051134 OR 31054873 OR 31056352 OR 31056353 OR 31061493 OR 31061494 OR 31072787 OR 31076274 OR 31078368 OR 31079872 OR 31080134 OR 31080135 OR 31080136 OR 31086314 OR 31086315 OR 31086316 OR 31097360 OR 31097361 OR 31101394 OR 31101395 OR 31103358 OR 31104942 OR 31104943 OR 31104950 OR 31104951 OR 31110321 OR 31110323 OR 31110324 OR 31121123 OR 31122676 OR 31122677 OR 31127258 OR 31127260 OR 31130330 OR 31130512 OR 31130513 OR 31130514 OR 31133689 OR 31147152 OR 31147153 OR 31151773 OR 31151774 OR 31153646 OR 31153647 OR 31155482 OR 31155483 OR 31155484 OR 31160741 OR 31171447 OR 31171448 OR 31173711 OR 31173712 OR 31173713 OR 31173715 OR 31173718 OR 31174959 OR 31174960 OR 31178114 OR 31178115 OR 31178255 OR 31182866 OR 31182867 OR 31182869 OR 31196672 OR 31196673 OR 31201122 OR 31201123 OR 31202541 OR 31204082 OR 31204176 OR 31204177 OR 31209376 OR 31209378 OR 31209379 OR 31209380 OR 31209381 OR 31221559 OR 31221560 OR 31227309 OR 31227310 OR 31230761 OR 31230859 OR 31230860 OR 31235906 OR 31235907 OR 31235908 OR 31235930 OR 31235931 OR 31235932 OR 31235933 OR 31248728 OR 31253468 OR 31253469 OR 31255486 OR 31257105 OR 31263205 OR 31271748 OR 31271750 OR 31272828 OR 31272829 OR 31277924 OR 31279774 OR 31280924 OR 31285612 OR 31285613 OR 31285614 OR 31285615 OR 31285616 OR 31296412 OR 31300277 OR 31301936 OR 31303374 OR 31303547 OR 31303548 OR 31303549 OR 31308530 OR 31319048 OR 31324538 OR 31327663 OR 31327664 OR 31332371 OR 31332372 OR 31332373 OR 31332375 OR 31345643 OR 31346295 OR 31346296 OR 31350097 OR 31351757 OR 31353074 OR 31358989 OR 31358990 OR 31358991 OR 31358992 OR 31371111 OR 31374198 OR 31374199 OR 31376984 OR 31384015 OR 31395429 OR 31399280 OR 31406364 OR 31406365 OR 31406366 OR 31416668 OR 31420117 OR 31422912 OR 31422913 OR 31427770 OR 31427771 OR 31439429 OR 31447169 OR 31451801 OR 31451803 OR 31455879 OR 31455884 OR 31455886 OR 31455887 OR 31466734 OR 31471123 OR 31473062 OR 31474560 OR 31477898 OR 31488328 OR 31491396 OR 31492534 OR 31493975 OR 31495645 OR 31495646 OR 31495780 OR 31495781 OR 31495782 OR 31501571 OR 31501572 OR 31501573 OR 31515109 OR 31521441 OR 31522764 OR 31523027 OR 31523028 OR 31527803 OR 31542321 OR 31543297 OR 31543366 OR 31543367 OR 31548723 OR 31551592 OR 31551593 OR 31551596 OR 31551598 OR 31551599 OR 31551601 OR 31551603 OR 31551604 OR 31558350 OR 31561919 OR 31563294 OR 31564548 OR 31564549 OR 31564591 OR 31564592 OR 31570859 OR 31570865 OR 31582313 OR 31585093 OR 31585094 OR 31585809 OR 31586516 OR 31587918 OR 31587919 OR 31588046 OR 31588047 OR 31591558 OR 31591559 OR 31591560 OR 31591561 OR 31601510 OR 31604597 OR 31606247 OR 31606248 OR 31607423 OR 31611705 OR 31611706 OR 31611707 OR 31611708 OR 31623918 OR 31623919 OR 31627985 OR 31629603 OR 31630908 OR 31631012 OR 31631013 OR 31636447 OR 31636448 OR 31636449 OR 31636451 OR 31648898 OR 31648899 OR 31648900 OR 31653463 OR 31659341 OR 31659342 OR 31668484 OR 31668485 OR 31668844 OR 31672263 OR 31676170 OR 31677957 OR 31679900 OR 31686023 OR 31704028 OR 31706697 OR 31708306 OR 31708402 OR 31712775 OR 31719672 OR 31727548 OR 31727549 OR 31732258 OR 31733940 OR 31735403 OR 31740813 OR 31740814 OR 31753579 OR 31753580 OR 31757603 OR 31757604 OR 31759806 OR 31759807 OR 31759808 OR 31761708 OR 31761709 OR 31761710 OR 31761722 OR 31761723 OR 31761724 OR 31768050 OR 31768051 OR 31768052 OR 31768054 OR 31768056 OR 31768057 OR 31780328 OR 31780329 OR 31780330 OR 31784285 OR 31784286 OR 31784287 OR 31784288 OR 31786011 OR 31786012 OR 31786013 OR 31786014 OR 31786016 OR 31792463 OR 31792464 OR 31792465 OR 31792466 OR 31792467 OR 31806491 OR 31806492 OR 31806493 OR 31809737 OR 31809738 OR 31809739 OR 31809740 OR 31810837 OR 31810838 OR 31810839 OR 31812514 OR 31812515 OR 31812516 OR 31813651 OR 31813652 OR 31813653 OR 31831331 OR 31831332 OR 31836321 OR 31836322 OR 31837915 OR 31839569 OR 31839570 OR 31844311 OR 31844313 OR 31844314 OR 31844315 OR 31844317 OR 31859030 OR 31859031 OR 31862210 OR 31864947 OR 31866091 OR 31866222 OR 31866223 OR 31866224 OR 31873194 OR 31873285 OR 31873286 OR 31879163 OR 31883788 OR 31883789 OR 31883834 OR 31883835 OR 31899071 OR 31899072 OR 31901251 OR 31901304 OR 31902528 OR 31907436 OR 31907437 OR 31907438 OR 31907439 OR 31924446 OR 31926610 OR 31928842 OR 31928944 OR 31932764 OR 31932766 OR 31932767 OR 31932769 OR 31932770 OR 31948733 OR 31948734 OR 31952856 OR 31954621 OR 31955944 OR 31956038 OR 31956039 OR 31956040 OR 31959933 OR 31959934 OR 31959935 OR 31959936 OR 31959937 OR 31972144 OR 31974009 OR 31978363 OR 31978364 OR 31978365 OR 31980319 OR 31982322 OR 31983538 OR 31995730 OR 32001108 OR 32004439 OR 32004478 OR 32004479 OR 32015540 OR 32023429 OR 32027824 OR 32027825 OR 32032525 OR 32032526 OR 32042174 OR 32042175 OR 32042176 OR 32048996 OR 32053769 OR 32059759 OR 32059806 OR 32059807 OR 32059808 OR 32066981 OR 32066983 OR 32066984 OR 32066985 OR 32066986 OR 32066987 OR 32070475 OR 32075716 OR 32078800 OR 32084331 OR 32084388 OR 32084389 OR 32084390 OR 32094970 OR 32097629 OR 32097630 OR 32101698 OR 32105611 OR 32109363 OR 32109376 OR 32109377 OR 32109378 OR 32112058 OR 32112061 OR 32123378 OR 32126198 OR 32130872 OR 32135084 OR 32142646 OR 32142647 OR 32142648 OR 32142663 OR 32142681 OR 32142682 OR 32142683 OR 32145183 OR 32145184 OR 32152537 OR 32155441 OR 32155442 OR 32160515 OR 32164873 OR 32164874 OR 32164875 OR 32169166 OR 32169167 OR 32169170 OR 32169171 OR 32171388 OR 32183943 OR 32187528 OR 32191871 OR 32197063 OR 32197066 OR 32199103 OR 32199104 OR 32203495 OR 32203496 OR 32203497 OR 32203499 OR 32208171 OR 32209430 OR 32213321 OR 32220666 OR 32229307 OR 32229310 OR 32229311 OR 32231338 OR 32231340 OR 32240599 OR 32243780 OR 32243781 OR 32243809 OR 32251386 OR 32259476 OR 32259481 OR 32272058 OR 32272064 OR 32275860 OR 32284604 OR 32284605 OR 32284606 OR 32284607 OR 32284608 OR 32289250 OR 32294466 OR 32302522 OR 32302523 OR 32302532 OR 32304628 OR 32313267 OR 32315603 OR 32320644 OR 32320679 OR 32325031 OR 32330411 OR 32333845 OR 32341540 OR 32341541 OR 32341542 OR 32343945 OR 32348717 OR 32348727 OR 32348728 OR 32353253 OR 32359400 OR 32362337 OR 32367065 OR 32369733 OR 32375063 OR 32375064 OR 32380032 OR 32386524 OR 32386552 OR 32386554 OR 32386572 OR 32392471 OR 32392472 OR 32393895 OR 32393896 OR 32396852 OR 32396862 OR 32396863 OR 32396864 OR 32402250 OR 32402251 OR 32407670 OR 32413331 OR 32413332 OR 32416059 OR 32424284 OR 32424285 OR 32424286 OR 32424287 OR 32428433 OR 32433908 OR 32442395 OR 32442399 OR 32445624 OR 32451482 OR 32451483 OR 32451484 OR 32451485 OR 32451487 OR 32459995 OR 32459996 OR 32464095 OR 32464096 OR 32473094 OR 32483349 OR 32485136 OR 32492366 OR 32514135 OR 32514136 OR 32514137 OR 32514138 OR 32514139 OR 32516567 OR 32516573 OR 32521223 OR 32526196 OR 32526197 OR 32531207 OR 32533915 OR 32541962 OR 32541964 OR 32544386 OR 32553204 OR 32559415 OR 32559418 OR 32562661 OR 32562662 OR 32572235 OR 32572236 OR 32572237 OR 32574559 OR 32579880 OR 32589864 OR 32589877 OR 32589878 OR 32592656 OR 32603655 OR 32610039 OR 32610040 OR 32615067 OR 32616470 OR 32619510 OR 32619511 OR 32619517 OR 32619518 OR 32632286 OR 32632287 OR 32640183 OR 32640191 OR 32645299 OR 32649865 OR 32661394 OR 32661395 OR 32661396 OR 32663438 OR 32673563 OR 32673568 OR 32673569 OR 32679036 OR 32681824 OR 32681825 OR 32690967 OR 32690968 OR 32690969 OR 32693086 OR 32693087 OR 32697942 OR 32697949 OR 32702287 OR 32707082 OR 32707083 OR 32710818 OR 32710819 OR 32719561 OR 32719562 OR 32719563 OR 32721381 OR 32730753 OR 32735778 OR 32735781 OR 32747787 OR 32747789 OR 32747790 OR 32750316 OR 32755548 OR 32758424 OR 32758425 OR 32758426 OR 32763144 OR 32763145 OR 32763182 OR 32778789 OR 32778791 OR 32778793 OR 32778794 OR 32783881 OR 32783882 OR 32783885 OR 32783886 OR 32791039 OR 32795399 OR 32795400 OR 32807948 OR 32807949 OR 32807950 OR 32810432 OR 32810433 OR 32810435 OR 32814018 OR 32818433 OR 32822582 OR 32822583 OR 32822613 OR 32839618 OR 32841590 OR 32846139 OR 32846140 OR 32853550 OR 32853551 OR 32868932 OR 32877641 OR 32888408 OR 32888424 OR 32888425 OR 32891188 OR 32891189 OR 32895565 OR 32895566 OR 32895567 OR 32905785 OR 32910893 OR 32910894 OR 32916090 OR 32916091 OR 32929244 OR 32929245 OR 32931729 OR 32931730 OR 32931754 OR 32931755 OR 32937099 OR 32946744 OR 32946745 OR 32946788 OR 32949502 OR 32961128 OR 32961129 OR 32961143 OR 32966764 OR 32966778 OR 32970991 OR 32976770 OR 32979312 OR 32979316 OR 32989293 OR 32989294 OR 32989295 OR 32991831 OR 32991838 OR 32997960 OR 33002411 OR 33007236 OR 33010822 OR 33020652 OR 33020653 OR 33020654 OR 33022226 OR 33022227 OR 33022228 OR 33027639 OR 33027640 OR 33049200 OR 33049201 OR 33049217 OR 33053374 OR 33068531 OR 33068532 OR 33077946 OR 33077947 OR 33077948 OR 33080226 OR 33080227 OR 33080228 OR 33080229 OR 33080230 OR 33086034 OR 33086038 OR 33086039 OR 33091338 OR 33091339 OR 33091368 OR 33096025 OR 33097921 OR 33098762 OR 33098807 OR 33108748 OR 33113347 OR 33113348 OR 33125872 OR 33125873 OR 33128895 OR 33139942 OR 33142113 OR 33142114 OR 33147442 OR 33147489 OR 33152265 OR 33152266 OR 33157003 OR 33159842 OR 33169029 OR 33169031 OR 33171117 OR 33176168 OR 33181065 OR 33181066 OR 33181078 OR 33186546 OR 33188733 OR 33199896 OR 33199898 OR 33202244 OR 33207217 OR 33207218 OR 33212012 OR 33217323 OR 33217328 OR 33220177 OR 33230320 OR 33230321 OR 33230322 OR 33230328 OR 33230329 OR 33232655 OR 33232662 OR 33232663 OR 33238137 OR 33242413 OR 33242421 OR 33242422 OR 33248017 OR 33257875 OR 33257876 OR 33259798 OR 33259804 OR 33264592 OR 33264636 OR 33271069 OR 33271070 OR 33275875 OR 33275898 OR 33278341 OR 33278342 OR 33288907 OR 33288908 OR 33288909 OR 33288910 OR 33290731 OR 33290732 OR 33296670 OR 33301706 OR 33301712 OR 33318667 OR 33321071 OR 33321072 OR 33321074 OR 33326754 OR 33326755 OR 33328624 OR 33333001 OR 33338395 OR 33340448 OR 33340451 OR 33349709 OR 33349710 OR 33349711 OR 33349712 OR 33352111 OR 33352118 OR 33353966 OR 33357383 OR 33357384 OR 33357385 OR 33357405 OR 33357412 OR 33357413 OR 33357417 OR 33361822 OR 33373620 OR 33378647 OR 33406410 OR 33412101 OR 33417867 OR 33417871 OR 33432193 OR 33432194 OR 33432195 OR 33432196 OR 33450185 OR 33450186 OR 33450187 OR 33453151 OR 33462481 OR 33472037 OR 33472038 OR 33476548 OR 33476575 OR 33482086 OR 33482087 OR 33484641 OR 33495635 OR 33495636 OR 33495637 OR 33497602 OR 33503410 OR 33508244 OR 33510480 OR 33513358 OR 33513363 OR 33526922 OR 33526942 OR 33529599 OR 33529646 OR 33535028 OR 33539722 OR 33539723 OR 33539763 OR 33542524 OR 33545077 OR 33545078 OR 33545080 OR 33545081 OR 33548174 OR 33558694 OR 33558695 OR 33561398 OR 33561399 OR 33561425 OR 33567253 OR 33567267 OR 33571444 OR 33571445 OR 33577748 OR 33581058 OR 33589832 OR 33589833 OR 33589834 OR 33600762 OR 33600763 OR 33603228 OR 33603230 OR 33603231 OR 33606969 OR 33609440 OR 33609483 OR 33619403 OR 33619404 OR 33619405 OR 33621485 OR 33621486 OR 33626322 OR 33626327 OR 33631115 OR 33631116 OR 33631117 OR 33651975 OR 33657412 OR 33657413 OR 33667342 OR 33667343 OR 33667356 OR 33667358 OR 33675684 OR 33675685 OR 33675690 OR 33686297 OR 33686298 OR 33686299 OR 33707754 OR 33711258 OR 33711282 OR 33711283 OR 33723433 OR 33723434 OR 33723435 OR 33730554 OR 33730555 OR 33737752 OR 33740416 OR 33740417 OR 33743191 OR 33753944 OR 33753945 OR 33756103 OR 33756104 OR 33765445 OR 33770504 OR 33770505 OR 33782620 OR 33782621 OR 33782622 OR 33782623 OR 33784497 OR 33784498 OR 33789082 OR 33789083 OR 33795883 OR 33795885 OR 33798407 OR 33798421 OR 33820999 OR 33821000 OR 33821001 OR 33823137 OR 33823138 OR 33823144 OR 33826906 OR 33831348 OR 33831349 OR 33831364 OR 33831365 OR 33831366 OR 33838105 OR 33846625 OR 33846626 OR 33848469 OR 33848470 OR 33848471 OR 33848472 OR 33848473 OR 33848474 OR 33852896 OR 33852917 OR 33859437 OR 33859438 OR 33861941 OR 33861942 OR 33875891 OR 33875892 OR 33875893 OR 33878295 OR 33882290 OR 33882291 OR 33887179 OR 33887199 OR 33894142 OR 33903770 OR 33910058 OR 33915078 OR 33915079 OR 33915080 OR 33915081 OR 33915110 OR 33927400 OR 33930307 OR 33945793 OR 33945794 OR 33951478 OR 33951479 OR 33957065 OR 33957072 OR 33957073 OR 33957080 OR 33957081 OR 33958804 OR 33961761 OR 33961762 OR 33961763 OR 33961764 OR 33961765 OR 33961766 OR 33961767 OR 33961768 OR 33961804 OR 33972801 OR 33972802 OR 33974915 OR 33979633 OR 33979634 OR 33979635 OR 33984282 OR 33984283 OR 33986549 OR 33986551 OR 33991504 OR 34002087 OR 34004179 OR 34010627 OR 34010628 OR 34015253 OR 34017129 OR 34017130 OR 34017131 OR 34019810 OR 34022129 OR 34031600 OR 34033742 OR 34038708 OR 34038743 OR 34048697 OR 34051145 OR 34059832 OR 34077741 OR 34077742 OR 34081911 OR 34083786 OR 34083787 OR 34089643 OR 34099922 OR 34102111 OR 34102139 OR 34118190 OR 34129813 OR 34133944 OR 34133945 OR 34139149 OR 34140698 OR 34146468 OR 34146469 OR 34157306 OR 34166604 OR 34168338 OR 34168339 OR 34168340 OR 34171289 OR 34171290 OR 34171291 OR 34183865 OR 34183866 OR 34183867 OR 34183869 OR 34186026 OR 34186027 OR 34197732 OR 34197733 OR 34228959 OR 34228960 OR 34233151 OR 34239128 OR 34239129 OR 34242565 OR 34245686 OR 34253921 OR 34253922 OR 34265252 OR 34265253 OR 34267392 OR 34293291 OR 34293292 OR 34293295 OR 34293334 OR 34294918 OR 34294919 OR 34297916 OR 34314698 OR 34320411 OR 34341584 OR 34341585 OR 34341586 OR 34343491 OR 34343492 OR 34352213 OR 34352214 OR 34354282 OR 34358441 OR 34363751 OR 34363753 OR 34373644 OR 34380016 OR 34381241 OR 34384519 OR 34385700 OR 34388375 OR 34390650 OR 34390651 OR 34390652 OR 34400844 OR 34407389 OR 34407390 OR 34407456 OR 34411513 OR 34411514 OR 34413511 OR 34413512 OR 34413513 OR 34413514 OR 34413515 OR 34416169 OR 34426698 OR 34437845 OR 34450025 OR 34450026 OR 34450065 OR 34465915 OR 34469773 OR 34473944 OR 34473945 OR 34473953 OR 34473954 OR 34478630 OR 34478631 OR 34478642 OR 34480863 OR 34480866 OR 34496297 OR 34496298 OR 34499856 OR 34499868 OR 34506723 OR 34506724 OR 34506725 OR 34508666 OR 34508667 OR 34525346 OR 34525347 OR 34525348 OR 34529935 OR 34534453 OR 34534454 OR 34534455 OR 34534456 OR 34536352 OR 34536353 OR 34536354 OR 34545249 OR 34551362 OR 34555313 OR 34555314 OR 34555316 OR 34559981 OR 34582785 OR 34582804 OR 34592167 OR 34592168 OR 34608335 OR 34614419 OR 34614420 OR 34614421 OR 34619088 OR 34619093 OR 34624205 OR 34624206 OR 34624220 OR 34626537 OR 34637706 OR 34644545 OR 34644546 OR 34648750 OR 34655526 OR 34663956 OR 34663957 OR 34663958 OR 34663959 OR 34665999 OR 34672984 OR 34672985 OR 34675436 OR 34675437 OR 34678146 OR 34678147 OR 34678169 OR 34687663 OR 34687664 OR 34687665 OR 34697455 OR 34699777 OR 34699778 OR 34706218 OR 34706219 OR 34706220 OR 34706221 OR 34706256 OR 34710366 OR 34711960 OR 34711961 OR 34715026 OR 34717794 OR 34727519 OR 34727520 OR 34735779 OR 34737447 OR 34737448 OR 34739817 OR 34741806 OR 34752775 OR 34762860 OR 34764474 OR 34767769 OR 34767770 OR 34776042 OR 34782793 OR 34782794 OR 34788632 OR 34793692 OR 34793693 OR 34793694 OR 34793707 OR 34795450 OR 34795451 OR 34798047 OR 34811521 OR 34847364 OR 34852235 OR 34856120 OR 34856121 OR 34857949 OR 34857950 OR 34861147 OR 34861149 OR 34861150 OR 34863366 OR 34863367 OR 34875233 OR 34879244 OR 34887588 OR 34887590 OR 34890566 OR 34903880 OR 34914919 OR 34916658 OR 34921780 OR 34921781 OR 34921782 OR 34931070 OR 34932940 OR 34932941 OR 34932942 OR 34932943 OR 34936886 OR 34942116 OR 34965381 OR 34980924 OR 34980925 OR 34982958 OR 34986325 OR 34990571 OR 34990576 OR 34990580 OR 34995486 OR 34995493 OR 34998469 OR 35027761 OR 35032430 OR 35041805 OR 35045331 OR 35045337 OR 35045338 OR 35045339 OR 35051374 OR 35051376 OR 35051377 OR 35065706 OR 35065714 OR 35065715 OR 35077667 OR 35085492 OR 35087246 OR 35090595 OR 35093191 OR 35102333 OR 35104442 OR 35104451 OR 35108498 OR 35108519 OR 35114101 OR 35114102 OR 35115729 OR 35115730 OR 35115731 OR 35120626 OR 35120627 OR 35120628 OR 35123654 OR 35123655 OR 35132236 OR 35139362 OR 35139363 OR 35139364 OR 35139365 OR 35143752 OR 35143761 OR 35165460 OR 35176221 OR 35176222 OR 35176223 OR 35180389 OR 35180390 OR 35180391 OR 35180398 OR 35210624 OR 35216662 OR 35216671 OR 35228700 OR 35241802 OR 35241804 OR 35245443 OR 35260862 OR 35260863 OR 35260864 OR 35260865 OR 35263617 OR 35263618 OR 35276083 OR 35276096 OR 35278361 OR 35278369 OR 35278370 OR 35288716 OR 35290791 OR 35290792 OR 35294899 OR 35294900 OR 35294901 OR 35301477 OR 35314823 OR 35325615 OR 35349784 OR 35349785 OR 35354062 OR 35358415 OR 35361972 OR 35361973 OR 35361974 OR 35364013 OR 35364014 OR 3</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+  <si>
+    <t>PMID=(1281416 OR 1281417 OR 1281418 OR 1281419 OR 1281420 OR 1309646 OR 1309647 OR 1309648 OR 1309649 OR 1309650 OR 1309651 OR 1309652 OR 1310861 OR 1310862 OR 1310863 OR 1310864 OR 1310865 OR 1312848 OR 1312849 OR 1314616 OR 1314617 OR 1314618 OR 1314619 OR 1314621 OR 1314622 OR 1314623 OR 1314624 OR 1316763 OR 1316764 OR 1316765 OR 1316767 OR 1319183 OR 1319184 OR 1319185 OR 1319186 OR 1321644 OR 1321645 OR 1321646 OR 1321647 OR 1321648 OR 1323309 OR 1323310 OR 1323312 OR 1323313 OR 1323314 OR 1326294 OR 1326295 OR 1326296 OR 1326297 OR 1327011 OR 1329864 OR 1334418 OR 1334419 OR 1334420 OR 1334421 OR 1334422 OR 1345671 OR 1346089 OR 1346090 OR 1346742 OR 1347996 OR 1347997 OR 1348949 OR 1348950 OR 1348951 OR 1350203 OR 1351731 OR 1351732 OR 1351733 OR 1352982 OR 1352983 OR 1352984 OR 1352985 OR 1352986 OR 1352987 OR 1355977 OR 1356370 OR 1356372 OR 1356373 OR 1361128 OR 1361129 OR 1370371 OR 1370372 OR 1370374 OR 1371216 OR 1371217 OR 1371218 OR 1371219 OR 1371220 OR 1372510 OR 1375036 OR 1375038 OR 1375039 OR 1376999 OR 1379820 OR 1379821 OR 1381926 OR 1382471 OR 1382472 OR 1382473 OR 1382474 OR 1382475 OR 1384575 OR 1384576 OR 1384577 OR 1384578 OR 1385966 OR 1388031 OR 1389179 OR 1389180 OR 1389181 OR 1389182 OR 1389183 OR 1389184 OR 1389185 OR 1418995 OR 1418996 OR 1418997 OR 1418998 OR 1418999 OR 1419000 OR 1419001 OR 1419002 OR 1419003 OR 1419004 OR 1463605 OR 1463606 OR 1463607 OR 1463608 OR 1463609 OR 1463610 OR 1497890 OR 1497891 OR 1497892 OR 1497893 OR 1497894 OR 1497895 OR 1497896 OR 1497897 OR 1497898 OR 1524823 OR 1524824 OR 1524825 OR 1524826 OR 1524827 OR 1524828 OR 1524829 OR 1524830 OR 1524831 OR 1530909 OR 1531415 OR 1532320 OR 1534012 OR 1550669 OR 1550670 OR 1550671 OR 1550672 OR 1550673 OR 1550674 OR 1550675 OR 1550677 OR 1550678 OR 1550679 OR 1567620 OR 1567621 OR 1567622 OR 1586486 OR 1586488 OR 1610562 OR 1610563 OR 1610564 OR 1610565 OR 1610566 OR 1610567 OR 1610568 OR 1610569 OR 1610570 OR 1632965 OR 1632966 OR 1632967 OR 1632968 OR 1632969 OR 1647174 OR 1647175 OR 1647176 OR 1648935 OR 1648937 OR 1648938 OR 1648939 OR 1648940 OR 1648941 OR 1654946 OR 1654948 OR 1654949 OR 1654950 OR 1654951 OR 1657055 OR 1657056 OR 1657057 OR 1657058 OR 1660283 OR 1660284 OR 1660285 OR 1660286 OR 1662517 OR 1662518 OR 1662519 OR 1662520 OR 1670919 OR 1670920 OR 1670921 OR 1670922 OR 1672071 OR 1672072 OR 1673055 OR 1673849 OR 1673850 OR 1673851 OR 1675862 OR 1675863 OR 1675864 OR 1676893 OR 1676894 OR 1676895 OR 1678612 OR 1678613 OR 1678615 OR 1681831 OR 1681832 OR 1681833 OR 1684900 OR 1684902 OR 1684903 OR 1689586 OR 1690014 OR 1690015 OR 1690016 OR 1690017 OR 1690562 OR 1690563 OR 1690564 OR 1690566 OR 1690567 OR 1690568 OR 1691005 OR 1691006 OR 1693086 OR 1694444 OR 1694445 OR 1694446 OR 1698395 OR 1698396 OR 1698397 OR 1699567 OR 1699568 OR 1699569 OR 1702643 OR 1702645 OR 1702647 OR 1702648 OR 1702650 OR 1702651 OR 1704243 OR 1704244 OR 1705807 OR 1705808 OR 1709023 OR 1709024 OR 1709025 OR 1711347 OR 1711348 OR 1711349 OR 1712602 OR 1712603 OR 1712604 OR 1714745 OR 1716928 OR 1716929 OR 1716930 OR 1718333 OR 1718334 OR 1718335 OR 1720625 OR 1722411 OR 1722412 OR 1722413 OR 1730003 OR 1730004 OR 1730005 OR 1739459 OR 1739460 OR 1739461 OR 1739462 OR 1739463 OR 1742020 OR 1742021 OR 1742022 OR 1742023 OR 1742024 OR 1742025 OR 1742026 OR 1742027 OR 1742028 OR 1764241 OR 1764242 OR 1764243 OR 1764244 OR 1764245 OR 1764246 OR 1764247 OR 1824753 OR 1825171 OR 1825782 OR 1826603 OR 1827266 OR 1829904 OR 1832879 OR 1840649 OR 1846075 OR 1846076 OR 1847064 OR 1847065 OR 1848078 OR 1848081 OR 1848082 OR 1848083 OR 1849721 OR 1849722 OR 1849723 OR 1849724 OR 1849725 OR 1851019 OR 1873027 OR 1873028 OR 1873029 OR 1873030 OR 1873031 OR 1873032 OR 1873033 OR 1898850 OR 1899580 OR 1899581 OR 1901716 OR 1901717 OR 1901718 OR 1902699 OR 1905146 OR 1908251 OR 1908252 OR 1908253 OR 1910787 OR 1910788 OR 1910790 OR 1931049 OR 1931050 OR 1931051 OR 1931052 OR 1931053 OR 1931054 OR 1968344 OR 1968345 OR 1971515 OR 1972886 OR 1976015 OR 1976320 OR 1976321 OR 1977421 OR 1977422 OR 1980068 OR 1980069 OR 1980070 OR 1986772 OR 1986773 OR 1986774 OR 1993122 OR 1993123 OR 1993124 OR 2001285 OR 2001286 OR 2001287 OR 2015091 OR 2015092 OR 2015093 OR 2015094 OR 2015095 OR 2025425 OR 2025426 OR 2025427 OR 2025428 OR 2025429 OR 2025430 OR 2054187 OR 2069816 OR 2106330 OR 2106331 OR 2106905 OR 2106906 OR 2108708 OR 2111712 OR 2114884 OR 2114885 OR 2116813 OR 2116814 OR 2119630 OR 2119631 OR 2138470 OR 2140514 OR 2145879 OR 2148487 OR 2148489 OR 2155007 OR 2155008 OR 2155009 OR 2155010 OR 2155011 OR 2155629 OR 2155630 OR 2156539 OR 2156540 OR 2156541 OR 2156542 OR 2157470 OR 2157471 OR 2160836 OR 2160837 OR 2160838 OR 2163262 OR 2163263 OR 2164403 OR 2164404 OR 2164405 OR 2166544 OR 2166545 OR 2169265 OR 2169266 OR 2169267 OR 2169268 OR 2169269 OR 2169270 OR 2169271 OR 2169272 OR 2169771 OR 2171589 OR 2171590 OR 2171591 OR 2171592 OR 2176509 OR 2176510 OR 2182078 OR 2182079)</t>
+  </si>
+  <si>
+    <t>PMID=(2196069 OR 2200448 OR 2200449 OR 2200450 OR 2205251 OR 2206530 OR 2206531 OR 2206532 OR 2206533 OR 2206534 OR 2206535 OR 2223090 OR 2223091 OR 2223092 OR 2223093 OR 2223094 OR 2223095 OR 2268433 OR 2306365 OR 2306366 OR 2310570 OR 2310571 OR 2310572 OR 2310573 OR 2310574 OR 2310575 OR 2317379 OR 2322458 OR 2322459 OR 2322460 OR 2322461 OR 2322462 OR 2322463 OR 2322464 OR 2322465 OR 2344404 OR 2344405 OR 2344406 OR 2344407 OR 2344408 OR 2344409 OR 2344410 OR 2344411 OR 2344412 OR 2361010 OR 2361011 OR 2361012 OR 2361013 OR 2361014 OR 2361016 OR 2369518 OR 2369519 OR 2369520 OR 2369521 OR 2369522 OR 2383398 OR 2383399 OR 2383400 OR 2400604 OR 2400605 OR 2400606 OR 2482777 OR 2482778 OR 2483091 OR 2483092 OR 2483093 OR 2483094 OR 2483095 OR 2483096 OR 2483098 OR 2483099 OR 2483100 OR 2483102 OR 2483103 OR 2483104 OR 2483105 OR 2483106 OR 2483107 OR 2483108 OR 2483111 OR 2483112 OR 2483113 OR 2483323 OR 2483324 OR 2483325 OR 2483327 OR 2484339 OR 2484340 OR 2484341 OR 2484342 OR 2484343 OR 2484345 OR 2484346 OR 2484347 OR 2515889 OR 2516449 OR 2516726 OR 2516728 OR 2518369 OR 2518370 OR 2518371 OR 2518372 OR 2534964 OR 2559758 OR 2559759 OR 2559760 OR 2560386 OR 2560387 OR 2560389 OR 2560390 OR 2560391 OR 2560392 OR 2560393 OR 2560638 OR 2560642 OR 2560645 OR 2560647 OR 2560649 OR 2561968 OR 2561969 OR 2561970 OR 2561971 OR 2561973 OR 2561974 OR 2561975 OR 2561976 OR 2561978 OR 2562784 OR 2576209 OR 2576210 OR 2576211 OR 2576212 OR 2576213 OR 2576215 OR 2576372 OR 2576373 OR 2576374 OR 2576375 OR 2576376 OR 2577128 OR 2577129 OR 2577130 OR 2619993 OR 2619994 OR 2619995 OR 2619996 OR 2619997 OR 2624739 OR 2624741 OR 2624742 OR 2624743 OR 2624744 OR 2624745 OR 2624746 OR 2624747 OR 2624748 OR 2627372 OR 2627375 OR 2627376 OR 2627377 OR 2627378 OR 2627379 OR 2627380 OR 2627381 OR 2641999 OR 2642000 OR 2642001 OR 2642002 OR 2642003 OR 2642004 OR 2642005 OR 2642006 OR 2642007 OR 2642008 OR 2642009 OR 2642010 OR 2642011 OR 2642012 OR 2642013 OR 2642014 OR 2642015 OR 2642016 OR 2642017 OR 2695147 OR 2696501 OR 2696503 OR 2696504 OR 2701844 OR 2701845 OR 2856086 OR 2856087 OR 2856088 OR 2856089 OR 2856090 OR 2856091 OR 2856094 OR 2856095 OR 2856096 OR 2856097 OR 2856098 OR 2856099 OR 2856100 OR 2856101 OR 2856102 OR 2856103 OR 2856104 OR 2856162 OR 2908443 OR 2908444 OR 2908447 OR 2908448 OR 2908449 OR 2908450 OR 2978786 OR 3078411 OR 3078412 OR 3078519 OR 3078520 OR 3152287 OR 3152288 OR 3152289 OR 3152290 OR 3152420 OR 3272153 OR 3272154 OR 3272155 OR 3272156 OR 3272157 OR 3272158 OR 3272159 OR 3272160 OR 3272161 OR 3272163 OR 3272164 OR 3272165 OR 3272166 OR 3272167 OR 3272168 OR 3272169 OR 3272170 OR 3272171 OR 3272172 OR 3272173 OR 3272177 OR 3272178 OR 3272179 OR 3272180 OR 3272181 OR 3272182 OR 3272183 OR 3272184 OR 3272185 OR 3272186 OR 3272187 OR 3272188 OR 3272190 OR 3272191 OR 3272738 OR 3272739 OR 7506045 OR 7506046 OR 7507335 OR 7507336 OR 7507337 OR 7507338 OR 7507339 OR 7507340 OR 7507341 OR 7509160 OR 7509161 OR 7512348 OR 7512349 OR 7512350 OR 7512351 OR 7512352 OR 7512353 OR 7512816 OR 7512817 OR 7514425 OR 7514427 OR 7514428 OR 7516686 OR 7516687 OR 7516688 OR 7516689 OR 7519023 OR 7519024 OR 7519025 OR 7519026 OR 7520251 OR 7520252 OR 7520253 OR 7520255 OR 7520256 OR 7522481 OR 7522482 OR 7522483 OR 7522484 OR 7524558 OR 7524560 OR 7524561 OR 7524562 OR 7524563 OR 7524564 OR 7530017 OR 7530018 OR 7530019 OR 7531985 OR 7531987 OR 7536426 OR 7536427 OR 7538309 OR 7538311 OR 7541630 OR 7541631 OR 7541632 OR 7541633 OR 7541634 OR 7541635 OR 7541636 OR 7542461 OR 7542462 OR 7544139 OR 7544140 OR 7544141 OR 7544142 OR 7546733 OR 7546734 OR 7546735 OR 7546737 OR 7546738 OR 7546740 OR 7546741 OR 7546744 OR 7546745 OR 7546746 OR 7546747 OR 7546748 OR 7546750 OR 7546751 OR 7576625 OR 7576627 OR 7576628 OR 7576629 OR 7576630 OR 7576631 OR 7576632 OR 7576633 OR 7576634 OR 7576635 OR 7576636 OR 7576637 OR 7576638 OR 7576639 OR 7576640 OR 7576641 OR 7576643 OR 7576644 OR 7576646 OR 7576647 OR 7576648 OR 7576649 OR 7576650 OR 7576651 OR 7576652 OR 7576653 OR 7576654 OR 7576655 OR 7576656 OR 7576657 OR 7576658 OR 7576659 OR 7576660 OR 7576661 OR 7576662 OR 7605627 OR 7605629 OR 7605630 OR 7605631 OR 7605632 OR 7605633 OR 7605634 OR 7605635 OR 7605636 OR 7605637 OR 7605638 OR 7605639 OR 7619514 OR 7619516 OR 7619517 OR 7619518 OR 7619519 OR 7619520 OR 7619522 OR 7619523 OR 7619524 OR 7619525 OR 7619526 OR 7619527 OR 7619528 OR 7619529 OR 7619530 OR 7619531 OR 7619532 OR 7619533 OR 7646884 OR 7646885 OR 7646886 OR 7646887 OR 7646888 OR 7646889 OR 7646891 OR 7646892 OR 7646893 OR 7646894 OR 7646895 OR 7646896 OR 7646898 OR 7678964 OR 7678965 OR 7678966 OR 7678967 OR 7679913 OR 7679914 OR 7679915 OR 7681676 OR 7682820 OR 7682821 OR 7684232 OR 7684233 OR 7684234 OR 7684235 OR 7684236 OR 7684237 OR 7686378 OR 7686379 OR 7686380 OR 7686381 OR 7686382 OR 7687849 OR 7688973 OR 7691102 OR 7691103 OR 7691104 OR 7691105 OR 7691106 OR 7694601 OR 7695895 OR 7695897 OR 7695899)</t>
+  </si>
+  <si>
+    <t>PMID=(7695900 OR 7695901 OR 7695902 OR 7695903 OR 7695904 OR 7695905 OR 7695906 OR 7695907 OR 7695908 OR 7695910 OR 7695911 OR 7695912 OR 7695913 OR 7718230 OR 7718231 OR 7718233 OR 7718234 OR 7718235 OR 7718236 OR 7718237 OR 7718238 OR 7718239 OR 7718241 OR 7718242 OR 7718243 OR 7718244 OR 7718245 OR 7718246 OR 7718248 OR 7718249 OR 7748549 OR 7748550 OR 7748552 OR 7748553 OR 7748554 OR 7748555 OR 7748556 OR 7748558 OR 7748559 OR 7748560 OR 7748561 OR 7748563 OR 7748564 OR 7748565 OR 7748566 OR 7794412 OR 7826629 OR 7826630 OR 7826631 OR 7826632 OR 7826633 OR 7826634 OR 7826635 OR 7826636 OR 7826637 OR 7826638 OR 7826639 OR 7826640 OR 7826641 OR 7826642 OR 7826644 OR 7826645 OR 7857635 OR 7857636 OR 7857640 OR 7857642 OR 7857644 OR 7857645 OR 7857646 OR 7857647 OR 7857648 OR 7857652 OR 7902109 OR 7902110 OR 7903858 OR 7903859 OR 7906528 OR 7906529 OR 7906530 OR 7906531 OR 7909234 OR 7910467 OR 7912090 OR 7912091 OR 7912093 OR 7913820 OR 7917287 OR 7917288 OR 7917289 OR 7917290 OR 7917291 OR 7917292 OR 7917293 OR 7917294 OR 7917295 OR 7917296 OR 7917297 OR 7917298 OR 7917299 OR 7917300 OR 7917301 OR 7917302 OR 7917303 OR 7917304 OR 7946325 OR 7946326 OR 7946329 OR 7946330 OR 7946331 OR 7946332 OR 7946333 OR 7946334 OR 7946335 OR 7946336 OR 7946338 OR 7946339 OR 7946340 OR 7946341 OR 7946344 OR 7946345 OR 7946346 OR 7946347 OR 7946348 OR 7946349 OR 7946350 OR 7946351 OR 7946352 OR 7946355 OR 7946356 OR 7946357 OR 7946358 OR 7946359 OR 7946360 OR 7946361 OR 7993619 OR 7993621 OR 7993622 OR 7993623 OR 7993624 OR 7993626 OR 7993627 OR 7993628 OR 7993629 OR 7993631 OR 7993632 OR 7993633 OR 7993634 OR 7993635 OR 7993636 OR 7993637 OR 7993638 OR 8011334 OR 8011335 OR 8011336 OR 8011340 OR 8043271 OR 8043272 OR 8043274 OR 8043276 OR 8043277 OR 8043278 OR 8043279 OR 8043280 OR 8043281 OR 8043282 OR 8060613 OR 8060614 OR 8060615 OR 8060616 OR 8060617 OR 8060618 OR 8060620 OR 8060621 OR 8060622 OR 8060623 OR 8068082 OR 8080464 OR 8094963 OR 8096385 OR 8097399 OR 8098608 OR 8098609 OR 8098610 OR 8098611 OR 8100427 OR 8101711 OR 8101712 OR 8102532 OR 8102533 OR 8102534 OR 8104431 OR 8104432 OR 8104433 OR 8110456 OR 8110457 OR 8110458 OR 8110459 OR 8110460 OR 8110461 OR 8110462 OR 8110463 OR 8110464 OR 8110465 OR 8110466 OR 8155316 OR 8155317 OR 8155318 OR 8155319 OR 8155320 OR 8155321 OR 8155322 OR 8155323 OR 8155324 OR 8155325 OR 8155326 OR 8161448 OR 8161449 OR 8161450 OR 8161451 OR 8161452 OR 8161453 OR 8161454 OR 8161455 OR 8161456 OR 8161457 OR 8161458 OR 8161459 OR 8161460 OR 8185941 OR 8185942 OR 8185943 OR 8185944 OR 8185947 OR 8185948 OR 8185949 OR 8185950 OR 8185953 OR 8240805 OR 8240806 OR 8240807 OR 8240808 OR 8240809 OR 8240810 OR 8240811 OR 8240812 OR 8240813 OR 8240814 OR 8240815 OR 8240816 OR 8240817 OR 8240818 OR 8240819 OR 8274272 OR 8274274 OR 8274275 OR 8274277 OR 8274278 OR 8274279 OR 8274280 OR 8274281 OR 8274283 OR 8292355 OR 8292356 OR 8292358 OR 8292359 OR 8292360 OR 8292361 OR 8292362 OR 8292363 OR 8318226 OR 8318227 OR 8318228 OR 8318229 OR 8318230 OR 8318231 OR 8318232 OR 8318234 OR 8338662 OR 8338663 OR 8338664 OR 8338665 OR 8338666 OR 8338667 OR 8338668 OR 8338669 OR 8338670 OR 8352940 OR 8352941 OR 8352942 OR 8352943 OR 8352944 OR 8352945 OR 8352946 OR 8381289 OR 8381290 OR 8382496 OR 8382497 OR 8382498 OR 8382499 OR 8382500 OR 8382501 OR 8384857 OR 8384858 OR 8384859 OR 8386524 OR 8386525 OR 8386526 OR 8386527 OR 8386528 OR 8386529 OR 8386530 OR 8386531 OR 8386532 OR 8388224 OR 8388225 OR 8388226 OR 8391279 OR 8391280 OR 8391281 OR 8393322 OR 8393323 OR 8393324 OR 8394719 OR 8394720 OR 8394721 OR 8394722 OR 8394723 OR 8398136 OR 8398137 OR 8398139 OR 8398140 OR 8398141 OR 8398142 OR 8398143 OR 8398144 OR 8398145 OR 8398147 OR 8398149 OR 8398150 OR 8398151 OR 8398152 OR 8398156 OR 8398157 OR 8398158 OR 8427698 OR 8427699 OR 8427700 OR 8427701 OR 8427702 OR 8439408 OR 8439409 OR 8439410 OR 8439411 OR 8439412 OR 8439413 OR 8439414 OR 8461131 OR 8461132 OR 8461133 OR 8461134 OR 8461135 OR 8461136 OR 8461137 OR 8461138 OR 8461139 OR 8461140 OR 8461141 OR 8461142 OR 8476609 OR 8476610 OR 8476611 OR 8476612 OR 8476613 OR 8476614 OR 8494644 OR 8494645 OR 8494646 OR 8494648 OR 8562074 OR 8562075 OR 8562078 OR 8562079 OR 8562080 OR 8562082 OR 8562084 OR 8562085 OR 8562086 OR 8562088 OR 8562089 OR 8562091 OR 8562092 OR 8562093 OR 8562094 OR 8607986 OR 8607991 OR 8607992 OR 8607993 OR 8607995 OR 8607996 OR 8607997 OR 8607998 OR 8607999 OR 8608000 OR 8608001 OR 8608002 OR 8608003 OR 8608004 OR 8608006 OR 8630240 OR 8630241 OR 8630242 OR 8630243 OR 8630246 OR 8630251 OR 8630252 OR 8630253 OR 8630254 OR 8630255 OR 8630256 OR 8630257 OR 8630258 OR 8663985 OR 8663986 OR 8663987 OR 8663988 OR 8663989 OR 8663990 OR 8663991 OR 8663992 OR 8663993 OR 8663994 OR 8663995 OR 8663996 OR 8663997 OR 8663998 OR 8663999 OR 8755474 OR 8755475 OR 8755476 OR 8755477 OR 8755478 OR 8755479 OR 8755480 OR 8755481 OR 8755482 OR 8755483 OR 8755484 OR 8755485 OR 8755486 OR 8755487)</t>
+  </si>
+  <si>
+    <t>PMID=(8755488 OR 8755489 OR 8780645 OR 8780646 OR 8780647 OR 8780648 OR 8780649 OR 8780651 OR 8780652 OR 8780653 OR 8780654 OR 8780655 OR 8780656 OR 8780657 OR 8780658 OR 8785047 OR 8785048 OR 8785049 OR 8785050 OR 8785051 OR 8785052 OR 8785053 OR 8785054 OR 8785055 OR 8785056 OR 8785057 OR 8785058 OR 8785059 OR 8785060 OR 8785061 OR 8785062 OR 8785063 OR 8785064 OR 8789941 OR 8789943 OR 8789944 OR 8789945 OR 8789946 OR 8789947 OR 8789948 OR 8789949 OR 8789950 OR 8789952 OR 8789953 OR 8789954 OR 8789955 OR 8789956 OR 8789957 OR 8789958 OR 8789959 OR 8789960 OR 8816703 OR 8816704 OR 8816705 OR 8816706 OR 8816707 OR 8816708 OR 8816709 OR 8816710 OR 8816711 OR 8816712 OR 8816713 OR 8816714 OR 8816715 OR 8816716 OR 8816717 OR 8816718 OR 8845150 OR 8845151 OR 8845152 OR 8845153 OR 8845154 OR 8845155 OR 8845156 OR 8845157 OR 8845158 OR 8845159 OR 8845160 OR 8845161 OR 8845162 OR 8845163 OR 8845164 OR 8845165 OR 8845166 OR 8845167 OR 8845168 OR 8845169 OR 8893018 OR 8893019 OR 8893020 OR 8893021 OR 8893022 OR 8893023 OR 8893024 OR 8893025 OR 8893026 OR 8893028 OR 8893029 OR 8893030 OR 8893031 OR 8893032 OR 8893033 OR 8893034 OR 8893035 OR 8938116 OR 8938117 OR 8938118 OR 8938119 OR 8938120 OR 8938121 OR 8938122 OR 8938123 OR 8938124 OR 8938125 OR 8938126 OR 8938127 OR 8938128 OR 8938129 OR 8938131 OR 8938132 OR 8938133 OR 8982155 OR 8982156 OR 8982157 OR 8982158 OR 8982159 OR 8982160 OR 8982161 OR 8982162 OR 8982163 OR 8982164 OR 8982165 OR 8982166 OR 8982167 OR 8982168 OR 8982169 OR 8982170 OR 8982171 OR 9010203 OR 9010204 OR 9010205 OR 9010206 OR 9010207 OR 9010208 OR 9010210 OR 9010211 OR 9010212 OR 9010214 OR 9052791 OR 9052792 OR 9052793 OR 9052794 OR 9052795 OR 9052796 OR 9052797 OR 9052798 OR 9052799 OR 9052800 OR 9052801 OR 9052802 OR 9115732 OR 9115733 OR 9115734 OR 9115735 OR 9115737 OR 9115740 OR 9115741 OR 9115743 OR 9136763 OR 9136764 OR 9136765 OR 9136766 OR 9136767 OR 9136768 OR 9136769 OR 9136770 OR 9136771 OR 9136772 OR 9136773 OR 9136774 OR 9136775 OR 9182797 OR 9182798 OR 9182799 OR 9182800 OR 9182801 OR 9182802 OR 9182803 OR 9182804 OR 9182805 OR 9182806 OR 9208853 OR 9208855 OR 9208856 OR 9208857 OR 9208858 OR 9208859 OR 9208860 OR 9208861 OR 9208862 OR 9208863 OR 9208864 OR 9208865 OR 9208866 OR 9208867 OR 9208868 OR 9247259 OR 9247260 OR 9247261 OR 9247262 OR 9247263 OR 9247264 OR 9247265 OR 9247266 OR 9247267 OR 9247268 OR 9247269 OR 9247270 OR 9247271 OR 9247272 OR 9247273 OR 9247274 OR 9247275 OR 9247276 OR 9292716 OR 9292717 OR 9292718 OR 9292719 OR 9292720 OR 9292721 OR 9292722 OR 9292723 OR 9292724 OR 9292725 OR 9292726 OR 9292727 OR 9292728 OR 9292729 OR 9292730 OR 9292731 OR 9292732 OR 9292733 OR 9331338 OR 9331343 OR 9331344 OR 9331345 OR 9331346 OR 9331347 OR 9331348 OR 9331349 OR 9331350 OR 9331352 OR 9331353 OR 9331354 OR 9331355 OR 9331356 OR 9331357 OR 9331358 OR 9331359 OR 9331360 OR 9331361 OR 9354320 OR 9354321 OR 9354324 OR 9354325 OR 9354326 OR 9354327 OR 9354328 OR 9354329 OR 9354330 OR 9354331 OR 9354332 OR 9354334 OR 9354335 OR 9354336 OR 9354338 OR 9354339 OR 9390513 OR 9390514 OR 9390515 OR 9390516 OR 9390517 OR 9390518 OR 9390519 OR 9390520 OR 9390521 OR 9390522 OR 9390523 OR 9390524 OR 9390525 OR 9390526 OR 9427242 OR 9427243 OR 9427244 OR 9427245 OR 9427246 OR 9427247 OR 9427248 OR 9427249 OR 9427250 OR 9427251 OR 9427252 OR 9427253 OR 9427254 OR 9427255 OR 9427256 OR 9459439 OR 9459440 OR 9459441 OR 9459442 OR 9459443 OR 9459444 OR 9459445 OR 9459446 OR 9459447 OR 9459448 OR 9459449 OR 9459450 OR 9459451 OR 9491979 OR 9491982 OR 9491983 OR 9491984 OR 9491985 OR 9491986 OR 9491987 OR 9491988 OR 9491990 OR 9491991 OR 9491992 OR 9491993 OR 9491994 OR 9539122 OR 9539123 OR 9539124 OR 9539125 OR 9539126 OR 9539127 OR 9539128 OR 9539129 OR 9539130 OR 9539131 OR 9539132 OR 9539133 OR 9581754 OR 9581759 OR 9581760 OR 9581761 OR 9581762 OR 9581763 OR 9581764 OR 9581765 OR 9581766 OR 9581767 OR 9581768 OR 9581769 OR 9581770 OR 9581771 OR 9620689 OR 9620690 OR 9620691 OR 9620692 OR 9620693 OR 9620694 OR 9620695 OR 9620696 OR 9620697 OR 9620698 OR 9620699 OR 9620700 OR 9620701 OR 9620702 OR 9620703 OR 9620704 OR 9620705 OR 9620706 OR 9620707 OR 9655492 OR 9655497 OR 9655498 OR 9655499 OR 9655500 OR 9655501 OR 9655502 OR 9655503 OR 9655504 OR 9655505 OR 9655507 OR 9655508 OR 9655509 OR 9655510 OR 9655511 OR 9655512 OR 9655513 OR 9655514 OR 9697850 OR 9697851 OR 9697852 OR 9697853 OR 9697854 OR 9697855 OR 9697856 OR 9697857 OR 9697858 OR 9697859 OR 9697860 OR 9697861 OR 9697862 OR 9697863 OR 9697864 OR 9697865 OR 9697866 OR 9697867 OR 9697868 OR 9728905 OR 9728911 OR 9728912 OR 9728913 OR 9728914 OR 9728915 OR 9728916 OR 9728917 OR 9728919 OR 9728920 OR 9728921 OR 9728922 OR 9728923 OR 9728924 OR 9728925 OR 9768836 OR 9768837 OR 9768838 OR 9768839 OR 9768840 OR 9768841 OR 9768842 OR 9768843 OR 9768844 OR 9768845 OR 9768846 OR 9768847 OR 9768848 OR 9768849 OR 9808444 OR 9808455 OR 9808456 OR 9808457 OR 9808458 OR 9808459 OR 9808460)</t>
+  </si>
+  <si>
+    <t>PMID=(9808461 OR 9808462 OR 9808463 OR 9808464 OR 9808465 OR 9808466 OR 9808467 OR 9808468 OR 9808469 OR 9808470 OR 9808471 OR 9808472 OR 9808473 OR 9808474 OR 9808475 OR 9808476 OR 9856456 OR 9856457 OR 9856458 OR 9856459 OR 9856460 OR 9856461 OR 9856462 OR 9856463 OR 9856464 OR 9856465 OR 9856466 OR 9856467 OR 9856468 OR 9856469 OR 9856470 OR 9856471 OR 9856472 OR 9856473 OR 9856474 OR 9856475 OR 9883720 OR 9883721 OR 9883722 OR 9883723 OR 9883724 OR 9883725 OR 9883726 OR 9883727 OR 9883728 OR 9883729 OR 9883730 OR 9883731 OR 9883732 OR 9883733 OR 9883734 OR 9883735 OR 9883736 OR 9883737 OR 9883738 OR 9883739 OR 9883740 OR 10027287 OR 10027288 OR 10027289 OR 10027290 OR 10027291 OR 10027292 OR 10027293 OR 10027294 OR 10027295 OR 10027296 OR 10027297 OR 10027298 OR 10027299 OR 10027300 OR 10027301 OR 10069331 OR 10069332 OR 10069333 OR 10069334 OR 10069335 OR 10069336 OR 10069337 OR 10069338 OR 10069339 OR 10069340 OR 10069341 OR 10069342 OR 10069343 OR 10069344 OR 10195101 OR 10195102 OR 10195104 OR 10195105 OR 10195106 OR 10195107 OR 10195108 OR 10195109 OR 10195110 OR 10195111 OR 10195112 OR 10195113 OR 10195114 OR 10195122 OR 10195123 OR 10195124 OR 10195125 OR 10195126 OR 10195127 OR 10195128 OR 10195129 OR 10195130 OR 10195131 OR 10195132 OR 10195133 OR 10195141 OR 10195142 OR 10195143 OR 10195144 OR 10195145 OR 10195146 OR 10195147 OR 10195148 OR 10195151 OR 10195152 OR 10195157 OR 10195158 OR 10195160 OR 10195161 OR 10195162 OR 10195163 OR 10195164 OR 10195165 OR 10195166 OR 10195173 OR 10195174 OR 10195175 OR 10195176 OR 10195177 OR 10195178 OR 10195179 OR 10195180 OR 10195181 OR 10195182 OR 10195183 OR 10195184 OR 10195185 OR 10195193 OR 10195194 OR 10195195 OR 10195196 OR 10195197 OR 10195198 OR 10195199 OR 10195200 OR 10195201 OR 10195202 OR 10195203 OR 10195204 OR 10195205 OR 10195211 OR 10195213 OR 10195215 OR 10195216 OR 10195217 OR 10195218 OR 10195219 OR 10195220 OR 10195221 OR 10195222 OR 10195223 OR 10195224 OR 10196521 OR 10196522 OR 10196524 OR 10196525 OR 10196526 OR 10196527 OR 10196528 OR 10196529 OR 10196530 OR 10196531 OR 10196532 OR 10196533 OR 10196534 OR 10196542 OR 10196543 OR 10196544 OR 10196545 OR 10196546 OR 10196547 OR 10196548 OR 10196549 OR 10196550 OR 10196551 OR 10196560 OR 10196561 OR 10196562 OR 10196563 OR 10196564 OR 10196565 OR 10196566 OR 10196567 OR 10196568 OR 10196569 OR 10196570 OR 10196571 OR 10196572 OR 10196573 OR 10196578 OR 10196579 OR 10196581 OR 10196582 OR 10196583 OR 10196584 OR 10196585 OR 10196586 OR 10196587 OR 10196588 OR 10196589 OR 10196590 OR 10196591 OR 10196592 OR 10197518 OR 10197526 OR 10197527 OR 10197528 OR 10197529 OR 10197530 OR 10197531 OR 10197532 OR 10197533 OR 10197534 OR 10197535 OR 10197536 OR 10197537 OR 10197538 OR 10197539 OR 10197541 OR 10204538 OR 10204539 OR 10204540 OR 10204541 OR 10204543 OR 10204544 OR 10204545 OR 10204546 OR 10204547 OR 10230778 OR 10230780 OR 10230781 OR 10230788 OR 10230789 OR 10230790 OR 10230791 OR 10230792 OR 10230793 OR 10230794 OR 10230796 OR 10230797 OR 10230798 OR 10230799 OR 10230800 OR 10230801 OR 10230802 OR 10321241 OR 10321243 OR 10321244 OR 10321245 OR 10321246 OR 10321247 OR 10321248 OR 10321249 OR 10321250 OR 10321251 OR 10321252 OR 10321253 OR 10399931 OR 10399932 OR 10399933 OR 10399934 OR 10399935 OR 10399936 OR 10399937 OR 10399938 OR 10399939 OR 10399940 OR 10399941 OR 10399942 OR 10399943 OR 10399944 OR 10402191 OR 10402192 OR 10402193 OR 10402194 OR 10402195 OR 10402196 OR 10402197 OR 10402198 OR 10402199 OR 10402200 OR 10402201 OR 10402202 OR 10402203 OR 10402204 OR 10404179 OR 10404183 OR 10404192 OR 10404196 OR 10404197 OR 10404198 OR 10404199 OR 10404200 OR 10404201 OR 10404202 OR 10404203 OR 10409387 OR 10412055 OR 10412057 OR 10412058 OR 10412059 OR 10412060 OR 10412061 OR 10412062 OR 10412063 OR 10412064 OR 10412065 OR 10412066 OR 10433258 OR 10433259 OR 10433260 OR 10433261 OR 10433262 OR 10433263 OR 10433264 OR 10433265 OR 10433266 OR 10433267 OR 10433268 OR 10433269 OR 10433270 OR 10433271 OR 10433272 OR 10448211 OR 10448212 OR 10448213 OR 10448214 OR 10448215 OR 10448216 OR 10448217 OR 10448218 OR 10448219 OR 10448220 OR 10448221 OR 10448222 OR 10448223 OR 10448224 OR 10461216 OR 10461217 OR 10461218 OR 10461219 OR 10461220 OR 10461221 OR 10461223 OR 10461225 OR 10482224 OR 10482234 OR 10482235 OR 10482236 OR 10482237 OR 10482238 OR 10482239 OR 10482240 OR 10482242 OR 10482243 OR 10482244 OR 10482245 OR 10482246 OR 10482247 OR 10491597 OR 10491598 OR 10491599 OR 10491600 OR 10491605 OR 10491606 OR 10491607 OR 10491608 OR 10491609 OR 10491610 OR 10491612 OR 10526323 OR 10526324 OR 10526325 OR 10526326 OR 10526329 OR 10526330 OR 10526331 OR 10526333 OR 10526334 OR 10526335 OR 10526336 OR 10526337 OR 10526338 OR 10526339 OR 10526340 OR 10526343 OR 10570481 OR 10570482 OR 10570483 OR 10570485 OR 10570486 OR 10570487 OR 10570488 OR 10570489 OR 10570490 OR 10570491 OR 10570492 OR 10571227 OR 10571229 OR 10571231 OR 10571233 OR 10571234 OR 10571235 OR 10571236 OR 10571237 OR 10571238 OR 10571239 OR 10571240 OR 10571241 OR 10595507 OR 10595508 OR 10595509 OR 10595510 OR 10595511 OR 10595512 OR 10595513 OR 10595514 OR 10595515 OR 10595516 OR 10595517 OR 10595518 OR 10595519 OR 10595520 OR 10595521 OR 10595522 OR 10595523 OR 10595524 OR 10607390 OR 10607391 OR 10607392 OR 10607393 OR 10607394 OR 10607395 OR 10607397)</t>
+  </si>
+  <si>
+    <t>PMID=(10607398 OR 10624936 OR 10624937 OR 10624938 OR 10624939 OR 10624943 OR 10624944 OR 10624945 OR 10624946 OR 10624947 OR 10624948 OR 10624949 OR 10624950 OR 10624951 OR 10624954 OR 10624957 OR 10624958 OR 10624959 OR 10624960 OR 10624961 OR 10624962 OR 10624963 OR 10624964 OR 10624965 OR 10649564 OR 10649565 OR 10649566 OR 10649567 OR 10649568 OR 10649569 OR 10649570 OR 10649571 OR 10649572 OR 10649574 OR 10677022 OR 10677031 OR 10677032 OR 10677033 OR 10677034 OR 10677035 OR 10677036 OR 10677037 OR 10677038 OR 10677039 OR 10677040 OR 10677041 OR 10677042 OR 10677043 OR 10677044 OR 10700250 OR 10700251 OR 10700252 OR 10700253 OR 10700254 OR 10700255 OR 10700256 OR 10700257 OR 10700258 OR 10700260 OR 10700261 OR 10700262 OR 10700263 OR 10707970 OR 10707971 OR 10707972 OR 10707973 OR 10707974 OR 10707975 OR 10707976 OR 10707977 OR 10707978 OR 10707979 OR 10707980 OR 10707981 OR 10707982 OR 10707983 OR 10707984 OR 10707985 OR 10707986 OR 10707987 OR 10719885 OR 10719886 OR 10719887 OR 10719888 OR 10719889 OR 10719890 OR 10719891 OR 10719893 OR 10719894 OR 10719895 OR 10719896 OR 10719897 OR 10719898 OR 10719899 OR 10719900 OR 10719901 OR 10725917 OR 10725919 OR 10725920 OR 10725921 OR 10725922 OR 10725923 OR 10725924 OR 10725925 OR 10725926 OR 10725927 OR 10725928 OR 10725929 OR 10725930 OR 10725931 OR 10769379 OR 10769380 OR 10769382 OR 10769383 OR 10769384 OR 10769385 OR 10769386 OR 10769387 OR 10769388 OR 10769389 OR 10769390 OR 10769391 OR 10769392 OR 10769393 OR 10769394 OR 10774723 OR 10774724 OR 10774726 OR 10774727 OR 10774728 OR 10774729 OR 10774730 OR 10774731 OR 10774732 OR 10774733 OR 10774734 OR 10774735 OR 10774736 OR 10774737 OR 10774738 OR 10798390 OR 10798391 OR 10798392 OR 10798393 OR 10798394 OR 10798395 OR 10798396 OR 10798397 OR 10798398 OR 10798399 OR 10798400 OR 10798401 OR 10798402 OR 10798403 OR 10798404 OR 10798405 OR 10798406 OR 10798407 OR 10798408 OR 10798409 OR 10798410 OR 10816306 OR 10816307 OR 10816310 OR 10816311 OR 10816312 OR 10816313 OR 10816314 OR 10816315 OR 10816316 OR 10816318 OR 10816319 OR 10839350 OR 10839352 OR 10839353 OR 10839354 OR 10839355 OR 10839356 OR 10839357 OR 10839358 OR 10839359 OR 10839360 OR 10839361 OR 10839362 OR 10839363 OR 10839364 OR 10839365 OR 10839366 OR 10839367 OR 10839368 OR 10839369 OR 10839370 OR 10839371 OR 10862694 OR 10862695 OR 10862696 OR 10862698 OR 10862699 OR 10862700 OR 10862701 OR 10862702 OR 10862703 OR 10862704 OR 10862706 OR 10862708 OR 10896155 OR 10896156 OR 10896157 OR 10896158 OR 10896159 OR 10896160 OR 10896161 OR 10896162 OR 10896163 OR 10896164 OR 10896165 OR 10896166 OR 10896167 OR 10896168 OR 10896169 OR 10903565 OR 10903566 OR 10903569 OR 10903570 OR 10903571 OR 10903572 OR 10903573 OR 10903574 OR 10903575 OR 10903576 OR 10903577 OR 10903578 OR 10939323 OR 10939328 OR 10939329 OR 10939330 OR 10939331 OR 10939332 OR 10939333 OR 10939334 OR 10939335 OR 10939336 OR 10939337 OR 10939338 OR 10939339 OR 10939340 OR 10939341 OR 10966613 OR 10966614 OR 10966616 OR 10966617 OR 10966618 OR 10966619 OR 10966620 OR 10966621 OR 10966622 OR 10966623 OR 10966624 OR 10966625 OR 10966626 OR 10966627 OR 10966628 OR 10985339 OR 10985343 OR 10985345 OR 10985346 OR 10985347 OR 10985348 OR 10985349 OR 10985350 OR 10985351 OR 10985352 OR 10985353 OR 10985354 OR 10985355 OR 10985356 OR 10985357 OR 10985358 OR 11017168 OR 11017169 OR 11017170 OR 11017171 OR 11017172 OR 11017173 OR 11017174 OR 11017175 OR 11017176 OR 11017177 OR 11017178 OR 11017179 OR 11036260 OR 11036261 OR 11036262 OR 11036263 OR 11036264 OR 11036265 OR 11036266 OR 11036267 OR 11036268 OR 11036269 OR 11036270 OR 11036271 OR 11036272 OR 11036273 OR 11036274 OR 11055428 OR 11055429 OR 11055430 OR 11055431 OR 11055432 OR 11055433 OR 11055434 OR 11055435 OR 11055436 OR 11055437 OR 11055438 OR 11055439 OR 11055440 OR 11055441 OR 11055442 OR 11055443 OR 11055444 OR 11055445 OR 11086981 OR 11086982 OR 11086983 OR 11086984 OR 11086985 OR 11086986 OR 11086987 OR 11086988 OR 11086989 OR 11086990 OR 11086991 OR 11086992 OR 11086993 OR 11086994 OR 11086995 OR 11086996 OR 11086997 OR 11086998 OR 11086999 OR 11087000 OR 11087001 OR 11100141 OR 11100144 OR 11100145 OR 11100146 OR 11100147 OR 11100148 OR 11100149 OR 11100150 OR 11100151 OR 11100152 OR 11100153 OR 11100154 OR 11100155 OR 11100156 OR 11100157 OR 11135641 OR 11135642 OR 11135643 OR 11135644 OR 11135645 OR 11135646 OR 11135647 OR 11135652 OR 11144348 OR 11144350 OR 11144351 OR 11144352 OR 11144353 OR 11144354 OR 11144355 OR 11144356 OR 11144357 OR 11144358 OR 11144359 OR 11144360 OR 11144361 OR 11144362 OR 11144363 OR 11144364 OR 11144365 OR 11144366 OR 11144367 OR 11163258 OR 11163259 OR 11163260 OR 11163261 OR 11163262 OR 11163263 OR 11163264 OR 11163265 OR 11163266 OR 11163267 OR 11163268 OR 11163269 OR 11163270 OR 11163271 OR 11163272 OR 11163273 OR 11163274 OR 11163275 OR 11163276 OR 11163277 OR 11163278 OR 11163279 OR 11163280 OR 11175864 OR 11175869 OR 11175870 OR 11175872 OR 11175873 OR 11175874 OR 11175875 OR 11175876 OR 11175877 OR 11175878 OR 11175879 OR 11175880 OR 11175881 OR 11175882 OR 11175883 OR 11175884 OR 11182080 OR 11182081 OR 11182082 OR 11182083 OR 11182084 OR 11182085 OR 11182086 OR 11182087 OR 11182088 OR 11182089 OR 11182090 OR 11182091 OR 11182092 OR 11182093 OR 11182094 OR 11182095 OR 11182096 OR 11182097 OR 11224535 OR 11224536 OR 11224537 OR 11224538 OR 11224539 OR 11224540 OR 11224541)</t>
+  </si>
+  <si>
+    <t>PMID=(11224542 OR 11224543 OR 11224544 OR 11224545 OR 11224546 OR 11224547 OR 11224548 OR 11224549 OR 11224550 OR 11224551 OR 11239426 OR 11239427 OR 11239428 OR 11239429 OR 11239430 OR 11239431 OR 11239432 OR 11239433 OR 11239434 OR 11239435 OR 11239436 OR 11239437 OR 11239438 OR 11239439 OR 11239440 OR 11239441 OR 11239442 OR 11276221 OR 11276222 OR 11276223 OR 11276224 OR 11276226 OR 11276227 OR 11276228 OR 11276229 OR 11276230 OR 11276231 OR 11276232 OR 11276233 OR 11276234 OR 11276235 OR 11276236 OR 11276237 OR 11301021 OR 11301022 OR 11301023 OR 11301026 OR 11301027 OR 11301028 OR 11301029 OR 11301030 OR 11301031 OR 11301032 OR 11301033 OR 11301034 OR 11301035 OR 11319553 OR 11319555 OR 11319556 OR 11319557 OR 11319558 OR 11319559 OR 11319560 OR 11319561 OR 11319562 OR 11343643 OR 11343644 OR 11343645 OR 11343646 OR 11343647 OR 11343648 OR 11343649 OR 11343650 OR 11343651 OR 11343652 OR 11343653 OR 11343654 OR 11343655 OR 11343656 OR 11343657 OR 11343658 OR 11343659 OR 11343660 OR 11343661 OR 11343662 OR 11369935 OR 11369936 OR 11369938 OR 11369939 OR 11369940 OR 11369942 OR 11369943 OR 11369944 OR 11369945 OR 11369946 OR 11369947 OR 11369948 OR 11369949 OR 11394998 OR 11394999 OR 11395000 OR 11395001 OR 11395002 OR 11395003 OR 11395004 OR 11395005 OR 11395006 OR 11395007 OR 11395008 OR 11395009 OR 11395010 OR 11395011 OR 11395012 OR 11395013 OR 11395014 OR 11395015 OR 11395016 OR 11395017 OR 11395018 OR 11395019 OR 11426219 OR 11426220 OR 11426221 OR 11426222 OR 11426224 OR 11426225 OR 11426226 OR 11426227 OR 11426228 OR 11426229 OR 11426230 OR 11426233 OR 11430800 OR 11430801 OR 11430802 OR 11430803 OR 11430804 OR 11430805 OR 11430806 OR 11430807 OR 11430808 OR 11430809 OR 11430810 OR 11430811 OR 11430812 OR 11430813 OR 11430814 OR 11477421 OR 11477422 OR 11477424 OR 11477425 OR 11477426 OR 11477427 OR 11477428 OR 11477429 OR 11477430 OR 11477431 OR 11477432 OR 11498048 OR 11498049 OR 11498050 OR 11498051 OR 11498052 OR 11498053 OR 11498054 OR 11498055 OR 11498056 OR 11498057 OR 11498058 OR 11502254 OR 11502255 OR 11502256 OR 11502257 OR 11502258 OR 11502259 OR 11502260 OR 11502261 OR 11502262 OR 11516394 OR 11516395 OR 11516396 OR 11516397 OR 11516398 OR 11516399 OR 11516401 OR 11516402 OR 11516403 OR 11516404 OR 11516405 OR 11528414 OR 11528415 OR 11528416 OR 11528417 OR 11528419 OR 11528420 OR 11528421 OR 11528422 OR 11528423 OR 11528424 OR 11528425 OR 11528426 OR 11528427 OR 11528428 OR 11528429 OR 11544481 OR 11544482 OR 11544483 OR 11545713 OR 11545714 OR 11545715 OR 11545716 OR 11545717 OR 11545718 OR 11545719 OR 11545720 OR 11545721 OR 11545722 OR 11545723 OR 11547336 OR 11547337 OR 11547338 OR 11559850 OR 11559852 OR 11559853 OR 11559854 OR 11559855 OR 11567611 OR 11567612 OR 11567613 OR 11567614 OR 11567615 OR 11567616 OR 11567617 OR 11567618 OR 11567619 OR 11567620 OR 11567621 OR 11567622 OR 11567623 OR 11574831 OR 11574832 OR 11580892 OR 11580893 OR 11580894 OR 11580897 OR 11580898 OR 11580899 OR 11580900 OR 11580901 OR 11580902 OR 11584290 OR 11593232 OR 11593233 OR 11593234 OR 11600888 OR 11600889 OR 11600890 OR 11600891 OR 11604135 OR 11604136 OR 11604137 OR 11604138 OR 11604139 OR 11604140 OR 11604141 OR 11604142 OR 11604143 OR 11604144 OR 11604145 OR 11604146 OR 11604147 OR 11683991 OR 11683992 OR 11683993 OR 11683994 OR 11683995 OR 11683996 OR 11683997 OR 11683998 OR 11683999 OR 11684000 OR 11684001 OR 11684002 OR 11684004 OR 11685224 OR 11685225 OR 11687813 OR 11687814 OR 11687815 OR 11687816 OR 11687817 OR 11687818 OR 11694884 OR 11694885 OR 11694886 OR 11694887 OR 11704761 OR 11704762 OR 11704763 OR 11704764 OR 11704765 OR 11709151 OR 11709152 OR 11709153 OR 11709154 OR 11709155 OR 11709156 OR 11709157 OR 11709158 OR 11709159 OR 11709160 OR 11709161 OR 11709162 OR 11709163 OR 11713467 OR 11713468 OR 11713469 OR 11713470 OR 11713472 OR 11713473 OR 11713474 OR 11719199 OR 11719200 OR 11719201 OR 11719202 OR 11719203 OR 11719204 OR 11719205 OR 11719206 OR 11719207 OR 11719208 OR 11719209 OR 11719210 OR 11719211 OR 11719212 OR 11719213 OR 11731801 OR 11731802 OR 11738025 OR 11738026 OR 11738027 OR 11738028 OR 11738029 OR 11738030 OR 11738031 OR 11738032 OR 11738033 OR 11738034 OR 11738035 OR 11740500 OR 11740501 OR 11740502 OR 11740503 OR 11753412 OR 11753413 OR 11753414 OR 11753415 OR 11753416 OR 11753417 OR 11753418 OR 11753419 OR 11753420 OR 11753421 OR 11754833 OR 11754834 OR 11754835 OR 11754836 OR 11754837 OR 11754838 OR 11754839 OR 11754840 OR 11754841 OR 11754842 OR 11754843 OR 11754844 OR 11754845 OR 11754846 OR 11770485 OR 11779476 OR 11779477 OR 11779478 OR 11779479 OR 11779480 OR 11779481 OR 11779482 OR 11779483 OR 11779484 OR 11779485 OR 11779486 OR 11779487 OR 11780144 OR 11780145 OR 11788834 OR 11788835 OR 11788836 OR 11788837 OR 11802169 OR 11802170 OR 11802171 OR 11802172 OR 11802173 OR 11802174 OR 11802175 OR 11804566 OR 11804568 OR 11804569 OR 11804570 OR 11804571 OR 11804572 OR 11804573 OR 11804574 OR 11804575 OR 11804576 OR 11832224 OR 11832225 OR 11832226 OR 11832227 OR 11832228 OR 11832229 OR 11832230 OR 11832231 OR 11832232 OR 11832233 OR 11836530 OR 11836531 OR 11836532 OR 11836533 OR 11850630 OR 11850631 OR 11850632 OR 11850633 OR 11850634 OR 11850635 OR 11856526 OR 11856527 OR 11856528 OR 11856529 OR 11856530 OR 11856531 OR 11856532 OR 11856533 OR 11856534 OR 11856535 OR 11856536 OR 11856537 OR 11865310 OR 11865311 OR 11879646 OR 11879647 OR 11879648)</t>
+  </si>
+  <si>
+    <t>PMID=(11879649 OR 11879650 OR 11879651 OR 11879652 OR 11879653 OR 11879654 OR 11879655 OR 11879656 OR 11879657 OR 11879658 OR 11889468 OR 11889469 OR 11889470 OR 11896395 OR 11896396 OR 11896397 OR 11896398 OR 11896399 OR 11896400 OR 11906693 OR 11906694 OR 11906695 OR 11906696 OR 11906697 OR 11906698 OR 11906699 OR 11906700 OR 11906701 OR 11906702 OR 11906703 OR 11914719 OR 11914720 OR 11914721 OR 11914722 OR 11914723 OR 11914724 OR 11931739 OR 11931740 OR 11931741 OR 11931742 OR 11931743 OR 11931744 OR 11931745 OR 11931746 OR 11931747 OR 11931750 OR 11941374 OR 11953750 OR 11953751 OR 11953752 OR 11953753 OR 11967544 OR 11967546 OR 11967547 OR 11967548 OR 11970861 OR 11970862 OR 11970863 OR 11970864 OR 11970865 OR 11970866 OR 11970867 OR 11970868 OR 11970869 OR 11970870 OR 11970871 OR 11970872 OR 11976702 OR 11976703 OR 11976704 OR 11976705 OR 11976706 OR 11988166 OR 11988167 OR 11988168 OR 11988169 OR 11988170 OR 11988171 OR 11988172 OR 11988173 OR 11988174 OR 11988175 OR 11988176 OR 11988177 OR 11992113 OR 11992114 OR 11992116 OR 11992117 OR 11992118 OR 11992119 OR 12006981 OR 12006982 OR 12006983 OR 12021764 OR 12021765 OR 12021766 OR 12032543 OR 12042822 OR 12055631 OR 12055633 OR 12055634 OR 12055635 OR 12062018 OR 12062019 OR 12062020 OR 12062021 OR 12062022 OR 12062023 OR 12062024 OR 12062025 OR 12062026 OR 12062027 OR 12062028 OR 12062029 OR 12062036 OR 12062037 OR 12062038 OR 12062040 OR 12062041 OR 12062042 OR 12062043 OR 12062044 OR 12062045 OR 12062046 OR 12062047 OR 12062048 OR 12068302 OR 12068303 OR 12068305 OR 12080341 OR 12080342 OR 12080343 OR 12080344 OR 12086635 OR 12086636 OR 12086637 OR 12086638 OR 12086639 OR 12086640 OR 12086641 OR 12086642 OR 12086643 OR 12086644 OR 12086645 OR 12086646 OR 12086647 OR 12086648 OR 12089528 OR 12089529 OR 12089530 OR 12101402 OR 12118256 OR 12118257 OR 12118258 OR 12118259 OR 12118260 OR 12123606 OR 12123607 OR 12123608 OR 12123609 OR 12123610 OR 12123611 OR 12123612 OR 12123613 OR 12123614 OR 12123615 OR 12123616 OR 12123617 OR 12123618 OR 12123619 OR 12123620 OR 12134152 OR 12134153 OR 12134155 OR 12145636 OR 12145637 OR 12145638 OR 12160742 OR 12160743 OR 12160744 OR 12160745 OR 12160746 OR 12160747 OR 12160748 OR 12160749 OR 12160750 OR 12160751 OR 12160752 OR 12160753 OR 12160754 OR 12160755 OR 12160756 OR 12161754 OR 12161755 OR 12161756 OR 12161757 OR 12165467 OR 12165468 OR 12165469 OR 12165470 OR 12165471 OR 12165472 OR 12165473 OR 12165474 OR 12165475 OR 12165476 OR 12165478 OR 12165479 OR 12172550 OR 12172551 OR 12194865 OR 12194867 OR 12194868 OR 12194869 OR 12194870 OR 12194871 OR 12194872 OR 12194873 OR 12194874 OR 12194875 OR 12194876 OR 12194877 OR 12194878 OR 12195426 OR 12195427 OR 12195428 OR 12195429 OR 12195430 OR 12195431 OR 12195432 OR 12195433 OR 12195434 OR 12219092 OR 12219095 OR 12219096 OR 12219097 OR 12244322 OR 12244323 OR 12352982 OR 12352983 OR 12354394 OR 12354395 OR 12354396 OR 12354397 OR 12354398 OR 12354399 OR 12354400 OR 12354401 OR 12354402 OR 12354403 OR 12354404 OR 12354405 OR 12354406 OR 12367504 OR 12367505 OR 12367506 OR 12367507 OR 12367508 OR 12367509 OR 12367510 OR 12367511 OR 12367513 OR 12367514 OR 12367515 OR 12367516 OR 12368804 OR 12368805 OR 12368806 OR 12368807 OR 12368808 OR 12368809 OR 12368810 OR 12372280 OR 12372281 OR 12372282 OR 12372283 OR 12372284 OR 12372286 OR 12372287 OR 12372288 OR 12372289 OR 12372292 OR 12379859 OR 12379860 OR 12379861 OR 12379863 OR 12379864 OR 12389030 OR 12389031 OR 12402039 OR 12402040 OR 12402041 OR 12403978 OR 12404008 OR 12408841 OR 12408842 OR 12408843 OR 12408844 OR 12408845 OR 12408846 OR 12408847 OR 12408848 OR 12408849 OR 12408850 OR 12408851 OR 12408852 OR 12408853 OR 12408854 OR 12408855 OR 12411958 OR 12411959 OR 12411960 OR 12426571 OR 12426572 OR 12426573 OR 12426574 OR 12436113 OR 12436114 OR 12436115 OR 12441049 OR 12441050 OR 12441051 OR 12441052 OR 12441053 OR 12441054 OR 12441055 OR 12441056 OR 12441057 OR 12441058 OR 12441059 OR 12441060 OR 12441061 OR 12441062 OR 12441063 OR 12467585 OR 12467586 OR 12467587 OR 12467588 OR 12467589 OR 12467590 OR 12467591 OR 12467592 OR 12467593 OR 12467594 OR 12467595 OR 12467596 OR 12467597 OR 12467598 OR 12467599 OR 12467600 OR 12469125 OR 12469126 OR 12469128 OR 12469130 OR 12469131 OR 12469132 OR 12483214 OR 12483215 OR 12483216 OR 12483217 OR 12483218 OR 12495618 OR 12495619 OR 12495620 OR 12495621 OR 12495622 OR 12495623 OR 12495624 OR 12495625 OR 12495626 OR 12495627 OR 12495628 OR 12495629 OR 12495630 OR 12495631 OR 12495632 OR 12495633 OR 12495634 OR 12496761 OR 12496762 OR 12514737 OR 12514738 OR 12524545 OR 12524546 OR 12524547 OR 12526769 OR 12526770 OR 12526771 OR 12526772 OR 12526774 OR 12526775 OR 12526776 OR 12526778 OR 12526779 OR 12526782 OR 12536208 OR 12536209 OR 12536210 OR 12536211 OR 12536213 OR 12536214 OR 12546816 OR 12546817 OR 12546818 OR 12546819 OR 12546820 OR 12546821 OR 12546822 OR 12546823 OR 12546824 OR 12546825 OR 12546828 OR 12548289 OR 12563262 OR 12563263 OR 12563264 OR 12563265 OR 12575948 OR 12575949 OR 12575950 OR 12575951 OR 12575952 OR 12575953 OR 12575954 OR 12575955 OR 12575956 OR 12575957 OR 12575958 OR 12575959 OR 12577061 OR 12577062 OR 12577063 OR 12592405 OR 12592406 OR 12592407 OR 12592408 OR 12592409 OR 12597856 OR 12597857 OR 12597858 OR 12597859 OR 12597860 OR 12597861 OR 12597862 OR 12597863 OR 12597864 OR 12597865 OR 12597866 OR 12597867 OR 12598899)</t>
+  </si>
+  <si>
+    <t>PMID=(12598900 OR 12601381 OR 12612586 OR 12627164 OR 12627165 OR 12627166 OR 12627167 OR 12628165 OR 12628166 OR 12628167 OR 12628170 OR 12628172 OR 12628173 OR 12628174 OR 12628175 OR 12628177 OR 12640457 OR 12640458 OR 12640459 OR 12640460 OR 12640461 OR 12652303 OR 12652304 OR 12652305 OR 12665800 OR 12670420 OR 12670421 OR 12670422 OR 12670423 OR 12670424 OR 12670425 OR 12670426 OR 12670427 OR 12670428 OR 12670429 OR 12670430 OR 12679782 OR 12679783 OR 12691660 OR 12691661 OR 12691662 OR 12691663 OR 12691664 OR 12691665 OR 12691666 OR 12691667 OR 12691668 OR 12691669 OR 12691670 OR 12691671 OR 12692555 OR 12692556 OR 12692557 OR 12692558 OR 12704391 OR 12704392 OR 12704394 OR 12717437 OR 12717438 OR 12718852 OR 12718853 OR 12718854 OR 12718855 OR 12718856 OR 12718857 OR 12718858 OR 12718859 OR 12718860 OR 12718861 OR 12718862 OR 12718863 OR 12718864 OR 12730698 OR 12730699 OR 12730700 OR 12740580 OR 12740581 OR 12740582 OR 12740583 OR 12741986 OR 12741987 OR 12741988 OR 12741989 OR 12741990 OR 12741991 OR 12741992 OR 12741993 OR 12741994 OR 12741995 OR 12741996 OR 12754512 OR 12754513 OR 12754514 OR 12754515 OR 12754517 OR 12754518 OR 12765606 OR 12765608 OR 12765609 OR 12765610 OR 12765611 OR 12765612 OR 12765613 OR 12765614 OR 12765615 OR 12765616 OR 12797956 OR 12797958 OR 12797959 OR 12797960 OR 12797961 OR 12797962 OR 12797963 OR 12797964 OR 12797965 OR 12797966 OR 12818172 OR 12818173 OR 12818174 OR 12818175 OR 12818176 OR 12818177 OR 12818178 OR 12818179 OR 12818180 OR 12818181 OR 12818182 OR 12818183 OR 12833050 OR 12845327 OR 12845328 OR 12848931 OR 12848932 OR 12848933 OR 12848934 OR 12848935 OR 12848936 OR 12848937 OR 12848939 OR 12848940 OR 12848941 OR 12858177 OR 12858178 OR 12858179 OR 12858180 OR 12872124 OR 12872125 OR 12872126 OR 12872127 OR 12872128 OR 12886226 OR 12895416 OR 12895421 OR 12895423 OR 12895424 OR 12895425 OR 12895426 OR 12895428 OR 12897787 OR 12897789 OR 12910242 OR 12925275 OR 12925277 OR 12925278 OR 12925279 OR 12925280 OR 12925281 OR 12925282 OR 12925283 OR 12925284 OR 12925855 OR 12925856 OR 12937421 OR 12937422 OR 12947408 OR 12947409 OR 12947410 OR 12948442 OR 12948443 OR 12948445 OR 12948446 OR 12948448 OR 12948449 OR 12948450 OR 12948451 OR 12958600 OR 12958601 OR 12971892 OR 12971895 OR 12971896 OR 12971898 OR 12971900 OR 12971901 OR 12971903 OR 12973353 OR 12973354 OR 12973355 OR 12973356 OR 14502288 OR 14502289 OR 14502290 OR 14502291 OR 14502292 OR 14513037 OR 14527430 OR 14527432 OR 14527433 OR 14527434 OR 14527435 OR 14527436 OR 14527437 OR 14527438 OR 14527439 OR 14527440 OR 14527441 OR 14527442 OR 14595442 OR 14595443 OR 14608359 OR 14622574 OR 14622575 OR 14622576 OR 14622577 OR 14622579 OR 14622580 OR 14622581 OR 14622582 OR 14622583 OR 14622584 OR 14622585 OR 14622586 OR 14622587 OR 14622588 OR 14625553 OR 14625554 OR 14625555 OR 14634650 OR 14634657 OR 14642276 OR 14659088 OR 14659089 OR 14659092 OR 14659093 OR 14659095 OR 14659096 OR 14659097 OR 14659101 OR 14659102 OR 14661023 OR 14687542 OR 14687543 OR 14687545 OR 14687551 OR 14687554 OR 14687556 OR 14687557 OR 14699413 OR 14699414 OR 14699415 OR 14699416 OR 14699418 OR 14699420 OR 14703572 OR 14703573 OR 14703574 OR 14703937 OR 14715132 OR 14715133 OR 14715134 OR 14715135 OR 14715136 OR 14715137 OR 14715138 OR 14715139 OR 14715140 OR 14715141 OR 14715142 OR 14715143 OR 14730305 OR 14730306 OR 14730307 OR 14730308 OR 14730309 OR 14741096 OR 14741097 OR 14741098 OR 14741100 OR 14741101 OR 14741102 OR 14741103 OR 14741104 OR 14741105 OR 14741106 OR 14741107 OR 14741108 OR 14741109 OR 14745451 OR 14758364 OR 14758365 OR 14766185 OR 14770185 OR 14770186 OR 14770187 OR 14966521 OR 14966522 OR 14966523 OR 14966524 OR 14966525 OR 14966526 OR 14966527 OR 14980201 OR 14980202 OR 14980203 OR 14980204 OR 14980205 OR 14980206 OR 14980207 OR 14980208 OR 14980209 OR 14980210 OR 14980211 OR 14980212 OR 14980213 OR 14983182 OR 14983183 OR 14983184 OR 14990932 OR 14990933 OR 15003173 OR 15003175 OR 15003176 OR 15003179 OR 15004561 OR 15004562 OR 15034583 OR 15034584 OR 15034585 OR 15034589 OR 15034590 OR 15046718 OR 15046719 OR 15046720 OR 15046721 OR 15046722 OR 15046723 OR 15046724 OR 15046725 OR 15046726 OR 15046727 OR 15091341 OR 15091344 OR 15091345 OR 15091346 OR 15091347 OR 15091348 OR 15114360 OR 15114362 OR 15114363 OR 15114364 OR 15114365 OR 15134636 OR 15134637 OR 15134638 OR 15134639 OR 15134641 OR 15134644 OR 15134646 OR 15146187 OR 15156145 OR 15156147 OR 15156150 OR 15157417 OR 15157418 OR 15157419 OR 15157420 OR 15157421 OR 15157422 OR 15157423 OR 15157424 OR 15157425 OR 15157426 OR 15157427 OR 15157428 OR 15162167 OR 15220929 OR 15233913 OR 15233914 OR 15233915 OR 15233916 OR 15233917 OR 15233918 OR 15233919 OR 15233920 OR 15233921 OR 15233922 OR 15233923 OR 15233924 OR 15235606 OR 15235607 OR 15235608 OR 15247919 OR 15247920 OR 15258584 OR 15258585 OR 15258586 OR 15258587 OR 15260953 OR 15260954 OR 15260955 OR 15260956 OR 15260957 OR 15260958 OR 15260959 OR 15260960 OR 15260962 OR 15260963 OR 15273690 OR 15273691 OR 15273692 OR 15294139 OR 15312648 OR 15312650 OR 15312653 OR 15338009 OR 15339643 OR 15339645 OR 15339646 OR 15339647 OR 15339648 OR 15339649 OR 15339650 OR 15339651 OR 15339652 OR 15339653 OR 15339654 OR 15361876 OR 15361877 OR 15361878 OR 15361879 OR 15361880 OR 15378064 OR 15378065 OR 15378066 OR 15452577 OR 15452578 OR 15452580 OR 15452581 OR 15473963 OR 15473965 OR 15473966)</t>
+  </si>
+  <si>
+    <t>PMID=(15473967 OR 15473968 OR 15473969 OR 15473970 OR 15473971 OR 15473972 OR 15473973 OR 15473975 OR 15504319 OR 15504320 OR 15504321 OR 15541307 OR 15541309 OR 15541310 OR 15541311 OR 15541312 OR 15541313 OR 15541314 OR 15541315 OR 15541316 OR 15541317 OR 15541319 OR 15543140 OR 15543144 OR 15568021 OR 15568022 OR 15572107 OR 15572108 OR 15572109 OR 15572110 OR 15572111 OR 15572112 OR 15572113 OR 15572114 OR 15572115 OR 15572116 OR 15572117 OR 15572118 OR 15580269 OR 15580270 OR 15580271 OR 15592462 OR 15592463 OR 15592464 OR 15592465 OR 15592467 OR 15603737 OR 15608630 OR 15608631 OR 15608632 OR 15608634 OR 15608635 OR 15608636 OR 15629698 OR 15629699 OR 15629700 OR 15629701 OR 15629702 OR 15629703 OR 15629704 OR 15629705 OR 15629706 OR 15629707 OR 15629708 OR 15629709 OR 15629710 OR 15629711 OR 15664171 OR 15664173 OR 15664174 OR 15664175 OR 15664176 OR 15664177 OR 15664178 OR 15664179 OR 15664180 OR 15664181 OR 15694321 OR 15694322 OR 15694323 OR 15694324 OR 15694325 OR 15694326 OR 15694327 OR 15694328 OR 15694329 OR 15694330 OR 15694331 OR 15694332 OR 15748850 OR 15797545 OR 15797546 OR 15797547 OR 15797548 OR 15797549 OR 15797550 OR 15797551 OR 15797552 OR 15797553 OR 15797554 OR 15797555 OR 15797556 OR 15797557 OR 15806098 OR 15820690 OR 15820691 OR 15820692 OR 15820693 OR 15820694 OR 15820695 OR 15820697 OR 15820698 OR 15820699 OR 15821730 OR 15834417 OR 15834418 OR 15834419 OR 15834420 OR 15834421 OR 15848797 OR 15848800 OR 15848802 OR 15848804 OR 15848805 OR 15848807 OR 15848808 OR 15848809 OR 15848810 OR 15852009 OR 15852010 OR 15852011 OR 15852012 OR 15852013 OR 15852014 OR 15852015 OR 15864304 OR 15880105 OR 15880106 OR 15880107 OR 15880108 OR 15880109 OR 15880110 OR 15880111 OR 15882641 OR 15882642 OR 15882644 OR 15882646 OR 15882647 OR 15882648 OR 15895084 OR 15895085 OR 15895086 OR 15895087 OR 15895088 OR 15908947 OR 15908948 OR 15908949 OR 15924135 OR 15924136 OR 15924137 OR 15924138 OR 15924864 OR 15924866 OR 15937481 OR 15937482 OR 15937483 OR 15937484 OR 15951809 OR 15951810 OR 15951811 OR 15965470 OR 15965471 OR 15965472 OR 15965473 OR 15995700 OR 15995701 OR 15995702 OR 15995703 OR 15995704 OR 15996546 OR 15996547 OR 15996548 OR 15996549 OR 15996550 OR 15996551 OR 15996552 OR 15996553 OR 15996554 OR 15996555 OR 16007080 OR 16007081 OR 16007082 OR 16007083 OR 16007084 OR 16007085 OR 16025106 OR 16025107 OR 16025108 OR 16025109 OR 16025110 OR 16025111 OR 16039556 OR 16039557 OR 16039558 OR 16041369 OR 16041370 OR 16055059 OR 16055060 OR 16055061 OR 16055062 OR 16055063 OR 16055064 OR 16055065 OR 16055066 OR 16055068 OR 16102532 OR 16102533 OR 16102534 OR 16102535 OR 16102536 OR 16102537 OR 16102538 OR 16102539 OR 16102540 OR 16102541 OR 16102542 OR 16129394 OR 16129396 OR 16129397 OR 16129398 OR 16129399 OR 16129400 OR 16129401 OR 16129402 OR 16136672 OR 16136673 OR 16222227 OR 16251981 OR 16251984 OR 16251985 OR 16261132 OR 16261133 OR 16261134 OR 16261135 OR 16261136 OR 16286926 OR 16286928 OR 16286929 OR 16286930 OR 16286931 OR 16286932 OR 16286933 OR 16286934 OR 16299500 OR 16299501 OR 16299502 OR 16299503 OR 16299504 OR 16301171 OR 16301172 OR 16301173 OR 16301174 OR 16301175 OR 16301176 OR 16301177 OR 16301178 OR 16301179 OR 16301180 OR 16301181 OR 16301182 OR 16301183 OR 16311588 OR 16311589 OR 16311591 OR 16327782 OR 16327783 OR 16327785 OR 16337911 OR 16337912 OR 16337913 OR 16337914 OR 16337915 OR 16337916 OR 16337917 OR 16337918 OR 16337919 OR 16337920 OR 16337921 OR 16337922 OR 16341209 OR 16341211 OR 16341212 OR 16341213 OR 16341215 OR 16364895 OR 16364896 OR 16364897 OR 16364898 OR 16364899 OR 16364900 OR 16364901 OR 16364902 OR 16364903 OR 16364904 OR 16364905 OR 16364906 OR 16364907 OR 16369480 OR 16369481 OR 16369482 OR 16369483 OR 16387635 OR 16387636 OR 16387637 OR 16387638 OR 16387639 OR 16387640 OR 16387641 OR 16387642 OR 16387643 OR 16387644 OR 16387645 OR 16387646 OR 16387647 OR 16388306 OR 16388307 OR 16388308 OR 16388309 OR 16415864 OR 16415865 OR 16415866 OR 16415867 OR 16415868 OR 16415869 OR 16415870 OR 16423691 OR 16423692 OR 16423693 OR 16423694 OR 16423695 OR 16423696 OR 16423697 OR 16423698 OR 16423699 OR 16423700 OR 16423701 OR 16423703 OR 16429133 OR 16429134 OR 16429135 OR 16429136 OR 16429137 OR 16444270 OR 16462734 OR 16462735 OR 16462736 OR 16462737 OR 16462738 OR 16474388 OR 16474389 OR 16474390 OR 16474391 OR 16474392 OR 16474393 OR 16491078 OR 16491079 OR 16491080 OR 16491081 OR 16491082 OR 16501566 OR 16501567 OR 16501568 OR 16504939 OR 16520734 OR 16520735 OR 16520736 OR 16520737 OR 16531997 OR 16531998 OR 16531999 OR 16543126 OR 16547508 OR 16547509 OR 16547510 OR 16547511 OR 16547512 OR 16565717 OR 16600850 OR 16617339 OR 16630833 OR 16630834 OR 16630835 OR 16630836 OR 16630837 OR 16630838 OR 16630839 OR 16630840 OR 16630841 OR 16648847 OR 16648848 OR 16648849 OR 16675393 OR 16675394 OR 16675395 OR 16675396 OR 16675397 OR 16675398 OR 16675399 OR 16675400 OR 16675401 OR 16675402 OR 16675403 OR 16680163 OR 16680164 OR 16680165 OR 16680166 OR 16699505 OR 16699506 OR 16699507 OR 16699508 OR 16699509 OR 16699510 OR 16701205 OR 16701207 OR 16701208 OR 16701209 OR 16701210 OR 16701212 OR 16701213 OR 16701214 OR 16715079 OR 16715080 OR 16715082 OR 16731508 OR 16731509 OR 16731510 OR 16731511 OR 16731512 OR 16731513 OR 16731514 OR 16731515 OR 16731516 OR 16731517 OR 16815329 OR 16815330 OR 16815331 OR 16815332 OR 16815333 OR 16815334 OR 16815335)</t>
+  </si>
+  <si>
+    <t>PMID=(16815336 OR 16815337 OR 16815338 OR 16819519 OR 16819520 OR 16819521 OR 16819522 OR 16819523 OR 16819524 OR 16829955 OR 16829956 OR 16829957 OR 16845384 OR 16845385 OR 16845386 OR 16845387 OR 16862149 OR 16862150 OR 16878129 OR 16880132 OR 16892056 OR 16892057 OR 16892058 OR 16906152 OR 16906153 OR 16921368 OR 16921369 OR 16921370 OR 16921371 OR 16921372 OR 16921373 OR 16936722 OR 16936723 OR 16950153 OR 16950154 OR 16950155 OR 16950156 OR 16950157 OR 16950158 OR 16950159 OR 16950160 OR 16950161 OR 16950162 OR 16982417 OR 16982419 OR 16982420 OR 16982421 OR 16982422 OR 16982423 OR 16982424 OR 16982425 OR 16982426 OR 16982427 OR 16982428 OR 16982429 OR 16982430 OR 17013379 OR 17013380 OR 17013381 OR 17028583 OR 17028584 OR 17028585 OR 17041592 OR 17041593 OR 17041594 OR 17041595 OR 17046687 OR 17046688 OR 17046689 OR 17046690 OR 17046691 OR 17046692 OR 17046693 OR 17046694 OR 17046695 OR 17046696 OR 17046697 OR 17046698 OR 17046699 OR 17057706 OR 17057707 OR 17057708 OR 17072305 OR 17086178 OR 17088206 OR 17099706 OR 17099707 OR 17099708 OR 17114044 OR 17114045 OR 17114046 OR 17114047 OR 17114048 OR 17114049 OR 17114050 OR 17114051 OR 17114052 OR 17114053 OR 17114055 OR 17115036 OR 17115037 OR 17115038 OR 17115039 OR 17115040 OR 17115041 OR 17115042 OR 17115043 OR 17115044 OR 17115045 OR 17128266 OR 17128283 OR 17143271 OR 17143272 OR 17145499 OR 17145500 OR 17145501 OR 17145502 OR 17145503 OR 17145504 OR 17145505 OR 17145506 OR 17145507 OR 17145508 OR 17145509 OR 17145510 OR 17145511 OR 17159989 OR 17159990 OR 17159991 OR 17159992 OR 17173043 OR 17173044 OR 17173045 OR 17173047 OR 17178398 OR 17178400 OR 17178401 OR 17178402 OR 17178403 OR 17178404 OR 17178405 OR 17178406 OR 17178407 OR 17178408 OR 17178409 OR 17178410 OR 17178411 OR 17178412 OR 17187064 OR 17187065 OR 17195842 OR 17195843 OR 17196527 OR 17196528 OR 17196529 OR 17196530 OR 17196531 OR 17196532 OR 17196533 OR 17196534 OR 17196535 OR 17196536 OR 17196537 OR 17206140 OR 17220882 OR 17220883 OR 17220884 OR 17220885 OR 17220886 OR 17220887 OR 17224401 OR 17224402 OR 17224403 OR 17224404 OR 17224405 OR 17224406 OR 17224407 OR 17224408 OR 17224409 OR 17224410 OR 17237775 OR 17237776 OR 17237777 OR 17237778 OR 17237779 OR 17237780 OR 17259980 OR 17259981 OR 17259982 OR 17270731 OR 17270732 OR 17270733 OR 17270734 OR 17270735 OR 17270736 OR 17270737 OR 17270738 OR 17270739 OR 17270740 OR 17277773 OR 17277774 OR 17293858 OR 17293860 OR 17293861 OR 17293862 OR 17296551 OR 17296552 OR 17296553 OR 17296554 OR 17296555 OR 17296556 OR 17296557 OR 17296558 OR 17296559 OR 17296560 OR 17310244 OR 17310246 OR 17310247 OR 17310248 OR 17322874 OR 17322875 OR 17322876 OR 17329205 OR 17329206 OR 17329207 OR 17329208 OR 17329209 OR 17329210 OR 17329211 OR 17329212 OR 17329213 OR 17329214 OR 17334360 OR 17334361 OR 17334362 OR 17351633 OR 17351634 OR 17351635 OR 17351636 OR 17351637 OR 17351638 OR 17359915 OR 17359916 OR 17359918 OR 17359919 OR 17359920 OR 17359921 OR 17359922 OR 17359924 OR 17369822 OR 17369823 OR 17369824 OR 17369825 OR 17369826 OR 17396120 OR 17396121 OR 17396122 OR 17396123 OR 17396124 OR 17408574 OR 17408576 OR 17408577 OR 17408578 OR 17408579 OR 17408580 OR 17408581 OR 17408582 OR 17408583 OR 17408584 OR 17408585 OR 17417632 OR 17417633 OR 17417634 OR 17417635 OR 17435752 OR 17435753 OR 17435754 OR 17435755 OR 17442239 OR 17442240 OR 17442243 OR 17442244 OR 17442245 OR 17442246 OR 17442247 OR 17442248 OR 17442249 OR 17442250 OR 17442251 OR 17442252 OR 17450135 OR 17450136 OR 17450137 OR 17450138 OR 17450139 OR 17468748 OR 17468749 OR 17468750 OR 17468751 OR 17468752 OR 17468753 OR 17481389 OR 17481391 OR 17481392 OR 17481393 OR 17481394 OR 17481395 OR 17481396 OR 17481397 OR 17481398 OR 17481399 OR 17486101 OR 17486102 OR 17486103 OR 17486104 OR 17496890 OR 17496891 OR 17515898 OR 17515899 OR 17515900 OR 17515901 OR 17515902 OR 17521563 OR 17521564 OR 17521565 OR 17521567 OR 17521568 OR 17521569 OR 17521570 OR 17521571 OR 17521572 OR 17521573 OR 17521574 OR 17521575 OR 17521576 OR 17529985 OR 17529986 OR 17529987 OR 17553420 OR 17553421 OR 17553422 OR 17553423 OR 17553424 OR 17553425 OR 17553426 OR 17553427 OR 17553428 OR 17553429 OR 17558399 OR 17558400 OR 17558401 OR 17558402 OR 17558404 OR 17558405 OR 17572671 OR 17572672 OR 17582326 OR 17582327 OR 17582329 OR 17582330 OR 17582331 OR 17582332 OR 17582333 OR 17582334 OR 17582335 OR 17582336 OR 17582337 OR 17582338 OR 17589505 OR 17589506 OR 17589507 OR 17603477 OR 17603478 OR 17603479 OR 17603480 OR 17603481 OR 17610813 OR 17610815 OR 17610816 OR 17610817 OR 17610818 OR 17610819 OR 17610820 OR 17610821 OR 17610822 OR 17610823 OR 17610824 OR 17618276 OR 17618277 OR 17618278 OR 17618279 OR 17618280 OR 17618281 OR 17632506 OR 17632507 OR 17632508 OR 17640520 OR 17640523 OR 17640524 OR 17640525 OR 17640528 OR 17640529 OR 17640530 OR 17640531 OR 17640532 OR 17643119 OR 17643120 OR 17660812 OR 17660813 OR 17660814 OR 17660815 OR 17676057 OR 17676058 OR 17676059 OR 17676060 OR 17678853 OR 17678854 OR 17678855 OR 17678856 OR 17678857 OR 17678858 OR 17678859 OR 17678860 OR 17678861 OR 17678862 OR 17694050 OR 17694051 OR 17694052 OR 17694053 OR 17698008 OR 17698009 OR 17698010 OR 17698011 OR 17698012 OR 17698013 OR 17698014 OR 17698015 OR 17698016 OR 17698017 OR 17704774 OR 17704775 OR 17721516 OR 17785178 OR 17785179 OR 17785180 OR 17785181 OR 17785182 OR 17785183 OR 17785184 OR 17785185)</t>
+  </si>
+  <si>
+    <t>PMID=(17785186 OR 17785187 OR 17828253 OR 17828254 OR 17828255 OR 17828256 OR 17828257 OR 17828258 OR 17828259 OR 17828260 OR 17828261 OR 17828262 OR 17873869 OR 17873870 OR 17873871 OR 17873872 OR 17873873 OR 17880891 OR 17880892 OR 17880893 OR 17880895 OR 17880896 OR 17880897 OR 17880898 OR 17880899 OR 17880900 OR 17891142 OR 17906619 OR 17906620 OR 17906621 OR 17906622 OR 17920010 OR 17920014 OR 17920015 OR 17920016 OR 17920017 OR 17920018 OR 17920019 OR 17920020 OR 17920021 OR 17920022 OR 17920023 OR 17920024 OR 17922006 OR 17922007 OR 17922008 OR 17934455 OR 17934456 OR 17934457 OR 17934458 OR 17934459 OR 17952067 OR 17952068 OR 17952069 OR 17965653 OR 17965710 OR 17965711 OR 17965712 OR 17982449 OR 17982450 OR 17982451 OR 17982452 OR 17982453 OR 17988629 OR 17988630 OR 17988631 OR 17988632 OR 17988633 OR 17988634 OR 17988635 OR 17988636 OR 17988637 OR 17988638 OR 17994013 OR 17994014 OR 17994015 OR 17994016 OR 18026096 OR 18026097 OR 18026098 OR 18026099 OR 18031679 OR 18031680 OR 18031681 OR 18031682 OR 18031683 OR 18031684 OR 18031685 OR 18031686 OR 18031687 OR 18031688 OR 18031689 OR 18037883 OR 18037884 OR 18054856 OR 18054857 OR 18054858 OR 18054859 OR 18054860 OR 18054861 OR 18054862 OR 18054863 OR 18054864 OR 18054865 OR 18054866 OR 18059264 OR 18059265 OR 18066056 OR 18066057 OR 18066058 OR 18066059 OR 18066060 OR 18066061 OR 18084286 OR 18084287 OR 18084288 OR 18084289 OR 18093519 OR 18093520 OR 18093522 OR 18093523 OR 18093524 OR 18093525 OR 18093526 OR 18093527 OR 18093528 OR 18093529 OR 18093530 OR 18093531 OR 18093532 OR 18157125 OR 18157126 OR 18159219 OR 18160954 OR 18160955 OR 18160956 OR 18160957 OR 18176559 OR 18176560 OR 18184560 OR 18184562 OR 18184563 OR 18184564 OR 18184565 OR 18184566 OR 18184567 OR 18184568 OR 18184569 OR 18184570 OR 18184571 OR 18184572 OR 18193039 OR 18193040 OR 18193041 OR 18193042 OR 18204441 OR 18204442 OR 18204443 OR 18204444 OR 18204445 OR 18213359 OR 18215619 OR 18215620 OR 18215621 OR 18215622 OR 18215623 OR 18215624 OR 18215625 OR 18215626 OR 18215627 OR 18223647 OR 18223648 OR 18223649 OR 18246064 OR 18246065 OR 18255029 OR 18255030 OR 18255031 OR 18255032 OR 18255033 OR 18255034 OR 18255035 OR 18255036 OR 18255037 OR 18255038 OR 18264094 OR 18264095 OR 18278039 OR 18278040 OR 18278041 OR 18278042 OR 18278043 OR 18297065 OR 18297066 OR 18297067 OR 18297068 OR 18311133 OR 18311135 OR 18311136 OR 18344990 OR 18344994 OR 18344995 OR 18344997 OR 18345353 OR 18367083 OR 18367084 OR 18367085 OR 18367086 OR 18367087 OR 18367088 OR 18367089 OR 18367090 OR 18367091 OR 18367092 OR 18367093 OR 18371326 OR 18371327 OR 18371330 OR 18371331 OR 18371332 OR 18371335 OR 18371336 OR 18371337 OR 18371338 OR 18371339 OR 18371340 OR 18371342 OR 18371343 OR 18371345 OR 18371348 OR 18371349 OR 18371350 OR 18371351 OR 18371352 OR 18371353 OR 18371359 OR 18371362 OR 18371363 OR 18371364 OR 18371365 OR 18371366 OR 18371367 OR 18371368 OR 18371370 OR 18371373 OR 18371377 OR 18371378 OR 18371379 OR 18371380 OR 18371381 OR 18371382 OR 18371391 OR 18371392 OR 18371393 OR 18371394 OR 18371395 OR 18371405 OR 18371406 OR 18371407 OR 18371408 OR 18371409 OR 18371420 OR 18371421 OR 18371422 OR 18371423 OR 18371424 OR 18371425 OR 18371432 OR 18371435 OR 18371436 OR 18371437 OR 18371438 OR 18371439 OR 18371447 OR 18371448 OR 18371449 OR 18371450 OR 18371451 OR 18371452 OR 18371453 OR 18376400 OR 18382462 OR 18383627 OR 18391942 OR 18391943 OR 18391944 OR 18391945 OR 18391946 OR 18397753 OR 18397754 OR 18397755 OR 18397756 OR 18397757 OR 18397758 OR 18408715 OR 18408716 OR 18408717 OR 18425121 OR 18425122 OR 18425123 OR 18425124 OR 18432196 OR 18432197 OR 18432198 OR 18439401 OR 18439403 OR 18439404 OR 18439405 OR 18439406 OR 18439407 OR 18439408 OR 18439409 OR 18439410 OR 18439411 OR 18439412 OR 18454144 OR 18454145 OR 18462688 OR 18462691 OR 18462692 OR 18462694 OR 18462695 OR 18462696 OR 18462697 OR 18462698 OR 18462699 OR 18466743 OR 18466744 OR 18466745 OR 18466746 OR 18466747 OR 18466748 OR 18466749 OR 18466750 OR 18466751 OR 18466752 OR 18466753 OR 18466754 OR 18469810 OR 18469811 OR 18488022 OR 18488023 OR 18488024 OR 18488025 OR 18498732 OR 18498733 OR 18498734 OR 18498735 OR 18498736 OR 18498737 OR 18498738 OR 18498739 OR 18498740 OR 18498741 OR 18498742 OR 18500338 OR 18516033 OR 18516034 OR 18516035 OR 18516036 OR 18522848 OR 18522849 OR 18522850 OR 18522851 OR 18522852 OR 18522853 OR 18536709 OR 18536710 OR 18536711 OR 18536712 OR 18549778 OR 18549780 OR 18549781 OR 18549782 OR 18549783 OR 18549784 OR 18549785 OR 18549786 OR 18549787 OR 18549788 OR 18549789 OR 18549790 OR 18549791 OR 18552840 OR 18552841 OR 18552842 OR 18552843 OR 18552844 OR 18568020 OR 18568021 OR 18568022 OR 18587389 OR 18587390 OR 18587391 OR 18587392 OR 18587393 OR 18593551 OR 18593552 OR 18593554 OR 18593557 OR 18593558 OR 18593559 OR 18593560 OR 18593561 OR 18593562 OR 18593563 OR 18604203 OR 18604204 OR 18604205 OR 18614027 OR 18614028 OR 18614029 OR 18614030 OR 18614031 OR 18614032 OR 18614033 OR 18614034 OR 18614035 OR 18614036 OR 18614037 OR 18614038 OR 18622399 OR 18622400 OR 18622401 OR 18622402 OR 18641642 OR 18641643 OR 18641644 OR 18641645 OR 18660806 OR 18660807 OR 18660808 OR 18682239 OR 18682240 OR 18682241 OR 18682242 OR 18682243 OR 18701062 OR 18701064 OR 18701065 OR 18701066 OR 18701067 OR 18701068 OR 18701069 OR 18701070 OR 18701071 OR 18701072 OR 18701073 OR 18701074 OR 18701075)</t>
+  </si>
+  <si>
+    <t>PMID=(18711393 OR 18758458 OR 18758459 OR 18758460 OR 18760692 OR 18760693 OR 18760696 OR 18760697 OR 18760698 OR 18760699 OR 18776892 OR 18776893 OR 18776894 OR 18776895 OR 18776896 OR 18776897 OR 18786354 OR 18786355 OR 18786356 OR 18786357 OR 18786358 OR 18786359 OR 18786360 OR 18786361 OR 18786362 OR 18786363 OR 18786364 OR 18786365 OR 18786407 OR 18786408 OR 18786410 OR 18786413 OR 18786414 OR 18786415 OR 18786416 OR 18786417 OR 18786418 OR 18786419 OR 18786421 OR 18794839 OR 18794840 OR 18804426 OR 18806784 OR 18806785 OR 18806786 OR 18817733 OR 18817734 OR 18817735 OR 18817736 OR 18817737 OR 18817738 OR 18817739 OR 18818591 OR 18820690 OR 18820691 OR 18820692 OR 18820693 OR 18820694 OR 18820695 OR 18836441 OR 18836442 OR 18836443 OR 18849983 OR 18849984 OR 18849985 OR 18849986 OR 18931664 OR 18931665 OR 18931666 OR 18938742 OR 18938746 OR 18940731 OR 18940732 OR 18940733 OR 18940734 OR 18940735 OR 18940736 OR 18953346 OR 18953347 OR 18953348 OR 18956012 OR 18957216 OR 18957217 OR 18957218 OR 18957219 OR 18957220 OR 18957221 OR 18957222 OR 18957223 OR 18957224 OR 18957225 OR 18957226 OR 18957227 OR 18957228 OR 18978778 OR 18978779 OR 18978780 OR 18978781 OR 18983965 OR 18983966 OR 18983967 OR 18983968 OR 18983969 OR 18983970 OR 18995816 OR 18995818 OR 18995819 OR 18995820 OR 18995821 OR 18995827 OR 18997789 OR 18997790 OR 18997791 OR 19011624 OR 19011625 OR 19029885 OR 19029887 OR 19029888 OR 19029889 OR 19029890 OR 19038214 OR 19038215 OR 19038216 OR 19038217 OR 19038218 OR 19038219 OR 19038220 OR 19038221 OR 19038222 OR 19038223 OR 19038224 OR 19038225 OR 19038226 OR 19038227 OR 19041778 OR 19041779 OR 19041780 OR 19041781 OR 19041782 OR 19041783 OR 19043409 OR 19043410 OR 19060895 OR 19079249 OR 19079250 OR 19079251 OR 19081373 OR 19081374 OR 19081375 OR 19081376 OR 19081377 OR 19081378 OR 19081379 OR 19081380 OR 19081381 OR 19081382 OR 19081384 OR 19081385 OR 19098904 OR 19098905 OR 19109905 OR 19109906 OR 19109907 OR 19109908 OR 19109909 OR 19109910 OR 19109911 OR 19109912 OR 19109913 OR 19109914 OR 19109915 OR 19109917 OR 19109918 OR 19109919 OR 19119091 OR 19122665 OR 19122666 OR 19128787 OR 19128789 OR 19128791 OR 19128792 OR 19128793 OR 19128794 OR 19128795 OR 19136969 OR 19136970 OR 19136971 OR 19136972 OR 19136973 OR 19136974 OR 19146810 OR 19146811 OR 19146812 OR 19146813 OR 19146814 OR 19146815 OR 19146816 OR 19146817 OR 19146818 OR 19151709 OR 19151710 OR 19151711 OR 19151712 OR 19160494 OR 19160495 OR 19160496 OR 19160497 OR 19160498 OR 19160499 OR 19160500 OR 19160501 OR 19160502 OR 19160503 OR 19160504 OR 19160505 OR 19160506 OR 19160507 OR 19160508 OR 19160509 OR 19160510 OR 19169249 OR 19169250 OR 19169251 OR 19169252 OR 19186162 OR 19186163 OR 19186164 OR 19186165 OR 19186166 OR 19186167 OR 19186168 OR 19186169 OR 19186170 OR 19186171 OR 19186172 OR 19200796 OR 19200800 OR 19200802 OR 19200803 OR 19200804 OR 19200805 OR 19209466 OR 19217371 OR 19217373 OR 19217374 OR 19217375 OR 19217376 OR 19217377 OR 19217378 OR 19217379 OR 19217380 OR 19217381 OR 19217382 OR 19217383 OR 19249272 OR 19249273 OR 19249274 OR 19249275 OR 19249276 OR 19249277 OR 19249278 OR 19249279 OR 19249280 OR 19249281 OR 19249282 OR 19252494 OR 19252495 OR 19252496 OR 19252497 OR 19252498 OR 19265651 OR 19265653 OR 19265655 OR 19265659 OR 19265661 OR 19265662 OR 19265663 OR 19265664 OR 19265665 OR 19270686 OR 19270687 OR 19270688 OR 19270689 OR 19270690 OR 19285465 OR 19285466 OR 19285468 OR 19285469 OR 19285470 OR 19285471 OR 19285472 OR 19285473 OR 19285474 OR 19285475 OR 19287386 OR 19287387 OR 19287388 OR 19287389 OR 19305400 OR 19305401 OR 19305402 OR 19322241 OR 19323994 OR 19323995 OR 19323996 OR 19323997 OR 19323998 OR 19323999 OR 19324000 OR 19324001 OR 19324002 OR 19324003 OR 19330001 OR 19330002 OR 19330003 OR 19330004 OR 19341616 OR 19341618 OR 19341619 OR 19341621 OR 19341622 OR 19341623 OR 19341624 OR 19341625 OR 19345177 OR 19349974 OR 19349975 OR 19349976 OR 19349977 OR 19363489 OR 19363490 OR 19363491 OR 19363492 OR 19376064 OR 19376065 OR 19376067 OR 19376068 OR 19376069 OR 19376070 OR 19376071 OR 19376072 OR 19376073 OR 19376074 OR 19377470 OR 19377471 OR 19377472 OR 19377473 OR 19396165 OR 19398399 OR 19409264 OR 19409265 OR 19409266 OR 19409267 OR 19409268 OR 19409269 OR 19409270 OR 19409271 OR 19409272 OR 19409273 OR 19412165 OR 19412166 OR 19412167 OR 19412168 OR 19427283 OR 19427286 OR 19427288 OR 19427290 OR 19427291 OR 19427292 OR 19427293 OR 19427294 OR 19430469 OR 19430470 OR 19430471 OR 19430472 OR 19430473 OR 19430474 OR 19447089 OR 19447090 OR 19447092 OR 19447093 OR 19447094 OR 19447095 OR 19447098 OR 19448628 OR 19448629 OR 19477150 OR 19477151 OR 19477152 OR 19477153 OR 19477154 OR 19477155 OR 19477156 OR 19477157 OR 19477158 OR 19477159 OR 19481515 OR 19483686 OR 19483687 OR 19483688 OR 19483689 OR 19497280 OR 19497281 OR 19497282 OR 19497283 OR 19497284 OR 19497285 OR 19503082 OR 19503083 OR 19503084 OR 19503085 OR 19503086 OR 19503087 OR 19524523 OR 19524524 OR 19524525 OR 19524526 OR 19524527 OR 19524528 OR 19524529 OR 19524530 OR 19524531 OR 19525941 OR 19525942 OR 19525943 OR 19525944 OR 19525945 OR 19525946 OR 19540188 OR 19543280 OR 19543281 OR 19555646 OR 19555647 OR 19555648 OR 19555649 OR 19555650 OR 19555651 OR 19555652 OR 19555653 OR 19555654 OR 19561601 OR 19561602 OR 19561603 OR 19570509 OR 19570512 OR 19570513 OR 19570514 OR 19570515 OR 19570516 OR 19570517)</t>
+  </si>
+  <si>
+    <t>PMID=(19570518 OR 19578379 OR 19578380 OR 19578381 OR 19578382 OR 19597494 OR 19597495 OR 19607788 OR 19607789 OR 19607790 OR 19607791 OR 19607792 OR 19607793 OR 19607794 OR 19607795 OR 19607796 OR 19607797 OR 19607798 OR 19620975 OR 19620976 OR 19620977 OR 19620978 OR 19631602 OR 19633665 OR 19633666 OR 19633667 OR 19640477 OR 19640478 OR 19640479 OR 19640480 OR 19640481 OR 19640482 OR 19640483 OR 19640484 OR 19648911 OR 19648912 OR 19648913 OR 19648914 OR 19648915 OR 19657336 OR 19664980 OR 19664984 OR 19664985 OR 19664988 OR 19664990 OR 19664991 OR 19664992 OR 19664993 OR 19664994 OR 19664995 OR 19668198 OR 19668199 OR 19668200 OR 19668201 OR 19679071 OR 19679072 OR 19679073 OR 19679074 OR 19679075 OR 19679076 OR 19679077 OR 19679078 OR 19679079 OR 19684588 OR 19684589 OR 19684590 OR 19684591 OR 19684592 OR 19684593 OR 19699165 OR 19701197 OR 19701198 OR 19716359 OR 19718034 OR 19718035 OR 19718036 OR 19733528 OR 19733531 OR 19733533 OR 19733540 OR 19733541 OR 19733542 OR 19733543 OR 19733544 OR 19734891 OR 19734892 OR 19734893 OR 19734894 OR 19734895 OR 19734896 OR 19734897 OR 19749747 OR 19749748 OR 19749749 OR 19749750 OR 19749751 OR 19755100 OR 19755102 OR 19755103 OR 19755104 OR 19755105 OR 19755106 OR 19755107 OR 19755108 OR 19755109 OR 19755110 OR 19755111 OR 19759538 OR 19767747 OR 19778502 OR 19778505 OR 19778506 OR 19778507 OR 19778508 OR 19778509 OR 19778510 OR 19778511 OR 19778512 OR 19778513 OR 19778514 OR 19778515 OR 19778516 OR 19778517 OR 19783975 OR 19783978 OR 19783979 OR 19783992 OR 19783993 OR 19783994 OR 19796610 OR 19796612 OR 19796616 OR 19796619 OR 19796620 OR 19796621 OR 19796622 OR 19796623 OR 19796624 OR 19801986 OR 19801987 OR 19801988 OR 19801989 OR 19818703 OR 19820704 OR 19820705 OR 19820706 OR 19820707 OR 19838177 OR 19838178 OR 19838179 OR 19838180 OR 19840541 OR 19840542 OR 19840543 OR 19840544 OR 19840547 OR 19855389 OR 19855390 OR 19874785 OR 19874786 OR 19874787 OR 19874788 OR 19874789 OR 19874790 OR 19874791 OR 19874792 OR 19874793 OR 19874794 OR 19881502 OR 19881503 OR 19881504 OR 19881505 OR 19881506 OR 19896441 OR 19896442 OR 19896443 OR 19896444 OR 19896445 OR 19898467 OR 19898468 OR 19898469 OR 19898470 OR 19904261 OR 19914180 OR 19914181 OR 19914182 OR 19914183 OR 19914184 OR 19914185 OR 19914186 OR 19914187 OR 19914188 OR 19914189 OR 19914190 OR 19915562 OR 19915563 OR 19915564 OR 19915565 OR 19915566 OR 19915567 OR 19935653 OR 19935654 OR 19935655 OR 19946318 OR 19946319 OR 19951688 OR 19951689 OR 19951690 OR 19951691 OR 19951692 OR 19951693 OR 19966837 OR 19966838 OR 19966839 OR 19966840 OR 19966842 OR 20005817 OR 20005819 OR 20005821 OR 20005822 OR 20005823 OR 20005824 OR 20005825 OR 20005826 OR 20005827 OR 20005828 OR 20005829 OR 20005830 OR 20010818 OR 20010819 OR 20010820 OR 20010821 OR 20010822 OR 20010823 OR 20010824 OR 20023650 OR 20023651 OR 20023652 OR 20023653 OR 20023654 OR 20023655 OR 20023656 OR 20036631 OR 20037574 OR 20037575 OR 20037576 OR 20037577 OR 20037578 OR 20037579 OR 20062052 OR 20062053 OR 20064381 OR 20064385 OR 20064387 OR 20064388 OR 20064389 OR 20064390 OR 20064391 OR 20064392 OR 20064393 OR 20064394 OR 20064395 OR 20064397 OR 20064398 OR 20064399 OR 20074533 OR 20074534 OR 20074535 OR 20074536 OR 20081850 OR 20081851 OR 20081852 OR 20085737 OR 20085738 OR 20085739 OR 20085740 OR 20085741 OR 20096661 OR 20098418 OR 20098419 OR 20098420 OR 20118924 OR 20118925 OR 20118926 OR 20118927 OR 20139973 OR 20139974 OR 20139976 OR 20144783 OR 20144785 OR 20144786 OR 20144787 OR 20144788 OR 20144789 OR 20152111 OR 20152112 OR 20152113 OR 20152114 OR 20152115 OR 20152116 OR 20152117 OR 20152118 OR 20152119 OR 20154682 OR 20154683 OR 20154684 OR 20159445 OR 20159446 OR 20159447 OR 20159448 OR 20159449 OR 20159450 OR 20159451 OR 20159452 OR 20159453 OR 20159454 OR 20173744 OR 20173745 OR 20173746 OR 20188651 OR 20188652 OR 20188653 OR 20188654 OR 20188655 OR 20188656 OR 20188657 OR 20188658 OR 20188659 OR 20188660 OR 20207221 OR 20207222 OR 20207225 OR 20207226 OR 20207227 OR 20207228 OR 20207229 OR 20207230 OR 20223197 OR 20223198 OR 20223199 OR 20223200 OR 20223201 OR 20223202 OR 20223203 OR 20223204 OR 20223205 OR 20223206 OR 20348915 OR 20348916 OR 20348917 OR 20348918 OR 20348919 OR 20348920 OR 20362535 OR 20362536 OR 20362537 OR 20362538 OR 20362539 OR 20362540 OR 20362541 OR 20362542 OR 20364143 OR 20364144 OR 20364145 OR 20383135 OR 20383136 OR 20383137 OR 20383138 OR 20399725 OR 20399727 OR 20399728 OR 20399730 OR 20399732 OR 20399733 OR 20399734 OR 20399735 OR 20399736 OR 20400959 OR 20400960 OR 20414199 OR 20418874 OR 20418875 OR 20434996 OR 20434997 OR 20434998 OR 20434999 OR 20435000 OR 20435001 OR 20435002 OR 20435003 OR 20435004 OR 20435005 OR 20435006 OR 20436478 OR 20436479 OR 20436480 OR 20436481 OR 20436482 OR 20452313 OR 20452314 OR 20452315 OR 20452317 OR 20452318 OR 20452319 OR 20452320 OR 20452321 OR 20452322 OR 20453850 OR 20453851 OR 20453852 OR 20453853 OR 20471349 OR 20471350 OR 20471351 OR 20471352 OR 20471353 OR 20471354 OR 20471355 OR 20471356 OR 20471357 OR 20471358 OR 20473290 OR 20473291 OR 20473292 OR 20473293 OR 20495557 OR 20495558 OR 20495559 OR 20510855 OR 20512132 OR 20512133 OR 20512134 OR 20512135 OR 20512136 OR 20512137 OR 20526331 OR 20526332 OR 20526333 OR 20526334 OR 20543841 OR 20543842 OR 20543843 OR 20562869 OR 20569687 OR 20569688 OR 20569689 OR 20569691 OR 20569693 OR 20569694 OR 20569695)</t>
+  </si>
+  <si>
+    <t>PMID=(20569697 OR 20578343 OR 20581814 OR 20581815 OR 20581816 OR 20581840 OR 20581841 OR 20581842 OR 20581843 OR 20601946 OR 20601947 OR 20601948 OR 20619762 OR 20619763 OR 20620868 OR 20620869 OR 20620870 OR 20620871 OR 20620872 OR 20620873 OR 20620874 OR 20620875 OR 20620876 OR 20620877 OR 20620878 OR 20620879 OR 20621043 OR 20621044 OR 20621045 OR 20621046 OR 20621049 OR 20621050 OR 20621051 OR 20621052 OR 20621053 OR 20621054 OR 20621055 OR 20621056 OR 20622871 OR 20622872 OR 20622873 OR 20624589 OR 20624590 OR 20624591 OR 20624592 OR 20624593 OR 20624594 OR 20624595 OR 20624596 OR 20624597 OR 20624598 OR 20624599 OR 20639873 OR 20639874 OR 20639875 OR 20657591 OR 20657592 OR 20670829 OR 20670830 OR 20670831 OR 20670832 OR 20670833 OR 20670834 OR 20670835 OR 20670836 OR 20670837 OR 20670838 OR 20670839 OR 20676103 OR 20676104 OR 20676105 OR 20680010 OR 20682443 OR 20682445 OR 20682446 OR 20682447 OR 20682448 OR 20682449 OR 20682450 OR 20682451 OR 20694001 OR 20694002 OR 20694003 OR 20694004 OR 20711183 OR 20711184 OR 20711185 OR 20711186 OR 20727844 OR 20729843 OR 20729844 OR 20729845 OR 20729846 OR 20797533 OR 20797535 OR 20797536 OR 20797537 OR 20797538 OR 20797540 OR 20797541 OR 20797542 OR 20802489 OR 20802490 OR 20804965 OR 20804969 OR 20804970 OR 20804971 OR 20804972 OR 20804973 OR 20804974 OR 20804975 OR 20818384 OR 20818385 OR 20818386 OR 20826301 OR 20826302 OR 20826303 OR 20826308 OR 20826309 OR 20826310 OR 20826311 OR 20826312 OR 20826313 OR 20826314 OR 20826315 OR 20826316 OR 20826317 OR 20826318 OR 20835249 OR 20835250 OR 20835251 OR 20835252 OR 20835253 OR 20852623 OR 20852624 OR 20852625 OR 20852626 OR 20869591 OR 20869592 OR 20869593 OR 20869594 OR 20869595 OR 20869596 OR 20869597 OR 20869598 OR 20869599 OR 20869600 OR 20869601 OR 20871602 OR 20871603 OR 20887947 OR 20887952 OR 20887953 OR 20887954 OR 20887955 OR 20887956 OR 20887957 OR 20887958 OR 20888316 OR 20890293 OR 20890294 OR 20890295 OR 20890296 OR 20920788 OR 20920789 OR 20920790 OR 20920791 OR 20920792 OR 20920793 OR 20920794 OR 20920795 OR 20920796 OR 20920797 OR 20935640 OR 20935641 OR 20935642 OR 20935643 OR 20935644 OR 20935645 OR 20953193 OR 20953194 OR 20953195 OR 20953196 OR 20953197 OR 20955921 OR 20955922 OR 20955923 OR 20955925 OR 20955927 OR 20955931 OR 20975754 OR 20975755 OR 20975756 OR 21040839 OR 21040842 OR 21040843 OR 21040844 OR 21040845 OR 21040846 OR 21040847 OR 21040848 OR 21040849 OR 21040850 OR 21040851 OR 21040852 OR 21040853 OR 21040854 OR 21040855 OR 21040856 OR 21040895 OR 21040897 OR 21040898 OR 21040899 OR 21040900 OR 21040901 OR 21040902 OR 21040903 OR 21076425 OR 21076426 OR 21102449 OR 21102451 OR 21112562 OR 21112563 OR 21112564 OR 21112565 OR 21112566 OR 21112567 OR 21112568 OR 21113162 OR 21131950 OR 21131951 OR 21131952 OR 21131953 OR 21131954 OR 21131955 OR 21144998 OR 21145001 OR 21145003 OR 21145004 OR 21145005 OR 21145006 OR 21145008 OR 21145009 OR 21145010 OR 21145011 OR 21150916 OR 21151119 OR 21151120 OR 21151121 OR 21167805 OR 21170052 OR 21170053 OR 21170054 OR 21170055 OR 21170056 OR 21185252 OR 21186355 OR 21186356 OR 21186357 OR 21186358 OR 21186359 OR 21186360 OR 21187849 OR 21209617 OR 21211781 OR 21211782 OR 21211783 OR 21211784 OR 21211785 OR 21217762 OR 21217763 OR 21217764 OR 21217765 OR 21220097 OR 21220098 OR 21220099 OR 21220100 OR 21220101 OR 21220102 OR 21220103 OR 21220104 OR 21220105 OR 21220106 OR 21220107 OR 21240273 OR 21258326 OR 21258327 OR 21258328 OR 21262461 OR 21262462 OR 21262463 OR 21262464 OR 21262465 OR 21262466 OR 21262467 OR 21262468 OR 21262469 OR 21262470 OR 21262471 OR 21262472 OR 21262473 OR 21262474 OR 21270780 OR 21270781 OR 21270782 OR 21278728 OR 21278729 OR 21278730 OR 21278732 OR 21278733 OR 21295269 OR 21295271 OR 21295272 OR 21295273 OR 21295274 OR 21295275 OR 21295276 OR 21295277 OR 21295278 OR 21297628 OR 21297629 OR 21297630 OR 21297631 OR 21317905 OR 21317906 OR 21336270 OR 21336271 OR 21336272 OR 21338871 OR 21338872 OR 21338873 OR 21338881 OR 21338882 OR 21338883 OR 21338884 OR 21338885 OR 21338886 OR 21338887 OR 21338888 OR 21358640 OR 21358641 OR 21358642 OR 21358643 OR 21358644 OR 21358645 OR 21362566 OR 21362567 OR 21362568 OR 21362569 OR 21362570 OR 21362571 OR 21362572 OR 21362573 OR 21378970 OR 21378972 OR 21378973 OR 21378974 OR 21382548 OR 21382549 OR 21382550 OR 21382551 OR 21382552 OR 21382553 OR 21382554 OR 21382555 OR 21382556 OR 21382557 OR 21382558 OR 21382559 OR 21382560 OR 21399631 OR 21399632 OR 21419747 OR 21423190 OR 21423191 OR 21435553 OR 21435554 OR 21435556 OR 21435557 OR 21435558 OR 21435559 OR 21435560 OR 21435561 OR 21435562 OR 21435563 OR 21441919 OR 21441920 OR 21441921 OR 21441922 OR 21441923 OR 21441924 OR 21441925 OR 21458401 OR 21460831 OR 21460832 OR 21460833 OR 21460834 OR 21474098 OR 21474100 OR 21474101 OR 21474102 OR 21474103 OR 21474104 OR 21474105 OR 21474106 OR 21474107 OR 21478884 OR 21478885 OR 21478886 OR 21478887 OR 21499253 OR 21499254 OR 21499255 OR 21516098 OR 21516099 OR 21516100 OR 21516101 OR 21516102 OR 21521610 OR 21521611 OR 21521612 OR 21521614 OR 21521615 OR 21521618 OR 21521619 OR 21521620 OR 21532576 OR 21532577 OR 21532578 OR 21532579 OR 21532580 OR 21549321 OR 21549325 OR 21549326 OR 21549327 OR 21549328 OR 21549329 OR 21549330 OR 21549331 OR 21552273 OR 21552274 OR 21552275 OR 21555070 OR 21555071 OR 21555072 OR 21555073 OR 21555074 OR 21555075 OR 21555076 OR 21555077)</t>
+  </si>
+  <si>
+    <t>PMID=(21555078 OR 21555079 OR 21572432 OR 21572433 OR 21572434 OR 21596650 OR 21602821 OR 21602822 OR 21620789 OR 21623361 OR 21623362 OR 21623363 OR 21623364 OR 21623365 OR 21624809 OR 21624810 OR 21624811 OR 21624812 OR 21624813 OR 21642972 OR 21642973 OR 21642974 OR 21642975 OR 21642976 OR 21658579 OR 21658580 OR 21658581 OR 21658583 OR 21658584 OR 21658585 OR 21658586 OR 21658587 OR 21658590 OR 21658591 OR 21666671 OR 21666672 OR 21666673 OR 21666674 OR 21683670 OR 21685916 OR 21685917 OR 21685918 OR 21685919 OR 21689595 OR 21689596 OR 21689598 OR 21689599 OR 21689600 OR 21689601 OR 21689602 OR 21689603 OR 21689604 OR 21689605 OR 21706017 OR 21706018 OR 21706020 OR 21706021 OR 21725311 OR 21725312 OR 21725313 OR 21725314 OR 21725315 OR 21726828 OR 21726829 OR 21726830 OR 21726831 OR 21726832 OR 21726833 OR 21726834 OR 21743470 OR 21743471 OR 21743472 OR 21743473 OR 21745635 OR 21745638 OR 21745639 OR 21745640 OR 21745641 OR 21745642 OR 21745643 OR 21745644 OR 21745645 OR 21745646 OR 21745647 OR 21750548 OR 21765421 OR 21765422 OR 21765423 OR 21765424 OR 21765425 OR 21765426 OR 21785434 OR 21785435 OR 21785436 OR 21791283 OR 21791284 OR 21791285 OR 21791286 OR 21791288 OR 21791289 OR 21791290 OR 21791291 OR 21791292 OR 21791294 OR 21792192 OR 21802386 OR 21804537 OR 21804538 OR 21816361 OR 21816363 OR 21816364 OR 21816365 OR 21816366 OR 21816367 OR 21822269 OR 21822270 OR 21822271 OR 21835340 OR 21835341 OR 21835342 OR 21835343 OR 21835344 OR 21835345 OR 21835346 OR 21835347 OR 21835348 OR 21835349 OR 21841774 OR 21841775 OR 21841776 OR 21841777 OR 21852222 OR 21857656 OR 21857657 OR 21857658 OR 21857659 OR 21867878 OR 21867879 OR 21867880 OR 21867881 OR 21867882 OR 21867883 OR 21867884 OR 21867885 OR 21867886 OR 21867887 OR 21867888 OR 21867889 OR 21874013 OR 21874014 OR 21874015 OR 21874016 OR 21874017 OR 21878933 OR 21885013 OR 21885015 OR 21885018 OR 21885019 OR 21885020 OR 21885021 OR 21885022 OR 21892154 OR 21892155 OR 21892156 OR 21892157 OR 21903074 OR 21903075 OR 21903077 OR 21903078 OR 21903079 OR 21903080 OR 21903082 OR 21903083 OR 21903084 OR 21903085 OR 21909085 OR 21909086 OR 21909087 OR 21909088 OR 21909089 OR 21909090 OR 21926982 OR 21926983 OR 21926984 OR 21926985 OR 21943598 OR 21943599 OR 21943600 OR 21943601 OR 21943602 OR 21943603 OR 21943604 OR 21943605 OR 21943606 OR 21943607 OR 21943608 OR 21943609 OR 21944778 OR 21944779 OR 21946326 OR 21946327 OR 21946328 OR 21962918 OR 21964488 OR 21964489 OR 21964490 OR 21982232 OR 21982233 OR 21982234 OR 21982235 OR 21982236 OR 21982367 OR 21982368 OR 21982369 OR 21982370 OR 21982371 OR 21982372 OR 21982373 OR 21982374 OR 21982375 OR 21982376 OR 21982377 OR 21982378 OR 21983681 OR 21983682 OR 21983683 OR 21983684 OR 22002768 OR 22017985 OR 22017987 OR 22017988 OR 22017989 OR 22017990 OR 22017991 OR 22017992 OR 22017993 OR 22017994 OR 22017995 OR 22017996 OR 22017997 OR 22019014 OR 22019730 OR 22019731 OR 22019732 OR 22030546 OR 22030547 OR 22030551 OR 22037496 OR 22037498 OR 22037499 OR 22037500 OR 22037501 OR 22056139 OR 22056140 OR 22056141 OR 22056142 OR 22056143 OR 22057188 OR 22057189 OR 22057190 OR 22057191 OR 22057192 OR 22057193 OR 22078507 OR 22081156 OR 22081157 OR 22081158 OR 22081159 OR 22081160 OR 22081161 OR 22100412 OR 22101640 OR 22101641 OR 22101642 OR 22101643 OR 22101644 OR 22101645 OR 22119902 OR 22119903 OR 22136926 OR 22136928 OR 22136929 OR 22136930 OR 22136931 OR 22136932 OR 22138642 OR 22138643 OR 22138644 OR 22138645 OR 22138646 OR 22138647 OR 22153366 OR 22153367 OR 22153369 OR 22153370 OR 22153371 OR 22153372 OR 22153373 OR 22153374 OR 22153375 OR 22153376 OR 22153377 OR 22153378 OR 22153379 OR 22153380 OR 22153381 OR 22158510 OR 22158511 OR 22158512 OR 22158513 OR 22158514 OR 22179109 OR 22179110 OR 22179111 OR 22179112 OR 22179113 OR 22197828 OR 22197830 OR 22197831 OR 22197832 OR 22197833 OR 22226352 OR 22226354 OR 22226355 OR 22226356 OR 22226357 OR 22226358 OR 22226359 OR 22231425 OR 22231426 OR 22231427 OR 22231428 OR 22243744 OR 22243745 OR 22243746 OR 22243747 OR 22243748 OR 22243750 OR 22243751 OR 22243752 OR 22243753 OR 22243754 OR 22243755 OR 22243756 OR 22243757 OR 22246433 OR 22246434 OR 22246435 OR 22246436 OR 22246437 OR 22246438 OR 22267160 OR 22267161 OR 22267162 OR 22267163 OR 22281715 OR 22284180 OR 22284181 OR 22284182 OR 22284183 OR 22284184 OR 22284185 OR 22284186 OR 22284187 OR 22284188 OR 22284189 OR 22284190 OR 22284191 OR 22286174 OR 22286175 OR 22305565 OR 22305566 OR 22305567 OR 22305568 OR 22305569 OR 22305570 OR 22305571 OR 22306606 OR 22306607 OR 22306608 OR 22325196 OR 22325198 OR 22325199 OR 22325200 OR 22325201 OR 22325202 OR 22325203 OR 22325204 OR 22325205 OR 22325206 OR 22325207 OR 22325208 OR 22325209 OR 22325210 OR 22327473 OR 22365540 OR 22365542 OR 22365543 OR 22365544 OR 22365545 OR 22365546 OR 22365547 OR 22365548 OR 22365549 OR 22365550 OR 22365552 OR 22365553 OR 22365554 OR 22385654 OR 22385655 OR 22385656 OR 22385657 OR 22385658 OR 22385659 OR 22385660 OR 22405201 OR 22405202 OR 22405203 OR 22405206 OR 22405207 OR 22405208 OR 22405209 OR 22405210 OR 22405211 OR 22405212 OR 22406547 OR 22406549 OR 22406551 OR 22424902 OR 22426252 OR 22426253 OR 22426255 OR 22445337 OR 22445338 OR 22445339 OR 22445341 OR 22445342 OR 22445343 OR 22445344 OR 22445345 OR 22445346 OR 22445347 OR 22445348 OR 22445349 OR 22445517 OR 22445518 OR 22446878 OR 22446880 OR 22446881 OR 22446882)</t>
+  </si>
+  <si>
+    <t>PMID=(22449960 OR 22466505 OR 22466506 OR 22482503 OR 22482504 OR 22482505 OR 22482506 OR 22482507 OR 22482508 OR 22484571 OR 22486005 OR 22500627 OR 22500628 OR 22500629 OR 22500630 OR 22500631 OR 22500632 OR 22500633 OR 22500634 OR 22500635 OR 22500636 OR 22500637 OR 22500638 OR 22500639 OR 22500640 OR 22504346 OR 22522400 OR 22522401 OR 22522402 OR 22542159 OR 22542160 OR 22542177 OR 22542180 OR 22542181 OR 22542182 OR 22542183 OR 22542184 OR 22542185 OR 22542186 OR 22542189 OR 22542190 OR 22542191 OR 22542192 OR 22544310 OR 22544311 OR 22544312 OR 22544313 OR 22560075 OR 22560076 OR 22560077 OR 22560078 OR 22560079 OR 22560080 OR 22560081 OR 22560082 OR 22561452 OR 22561453 OR 22561454 OR 22561455 OR 22578499 OR 22578500 OR 22578501 OR 22578502 OR 22578503 OR 22578504 OR 22578505 OR 22578506 OR 22578507 OR 22578508 OR 22581183 OR 22581184 OR 22581185 OR 22608532 OR 22610068 OR 22610069 OR 22632720 OR 22632721 OR 22632722 OR 22632723 OR 22632724 OR 22632725 OR 22632726 OR 22632727 OR 22632728 OR 22632729 OR 22632730 OR 22632731 OR 22632732 OR 22634728 OR 22634729 OR 22634730 OR 22634731 OR 22660477 OR 22660478 OR 22660479 OR 22660480 OR 22681682 OR 22681684 OR 22681685 OR 22681686 OR 22681687 OR 22681688 OR 22681689 OR 22681690 OR 22681691 OR 22681692 OR 22681693 OR 22681694 OR 22681695 OR 22681696 OR 22681697 OR 22683203 OR 22683204 OR 22683681 OR 22683682 OR 22683683 OR 22704497 OR 22704498 OR 22704499 OR 22704500 OR 22704501 OR 22704502 OR 22704503 OR 22704504 OR 22704505 OR 22704507 OR 22704510 OR 22704516 OR 22704518 OR 22706266 OR 22706267 OR 22706268 OR 22706269 OR 22706270 OR 22726828 OR 22726831 OR 22726832 OR 22726833 OR 22726834 OR 22726835 OR 22726836 OR 22726837 OR 22726838 OR 22726839 OR 22726840 OR 22726841 OR 22729174 OR 22729175 OR 22729176 OR 22729177 OR 22748967 OR 22748968 OR 22751036 OR 22770236 OR 22770237 OR 22770240 OR 22770241 OR 22770242 OR 22770243 OR 22770244 OR 22770245 OR 22770246 OR 22770845 OR 22772332 OR 22772333 OR 22794259 OR 22794260 OR 22794261 OR 22794262 OR 22794263 OR 22794264 OR 22794265 OR 22794266 OR 22794267 OR 22794268 OR 22797695 OR 22820465 OR 22820466 OR 22837034 OR 22837035 OR 22837036 OR 22837037 OR 22841310 OR 22841311 OR 22841312 OR 22841313 OR 22841314 OR 22841315 OR 22841316 OR 22841317 OR 22841318 OR 22842144 OR 22842145 OR 22842146 OR 22842147 OR 22842148 OR 22862941 OR 22862942 OR 22862943 OR 22862944 OR 22862945 OR 22862946 OR 22862947 OR 22862948 OR 22862949 OR 22863532 OR 22863533 OR 22863534 OR 22864610 OR 22864611 OR 22864612 OR 22864613 OR 22884324 OR 22884325 OR 22884327 OR 22884328 OR 22884329 OR 22884330 OR 22884331 OR 22884332 OR 22884333 OR 22884334 OR 22884335 OR 22885848 OR 22885849 OR 22885850 OR 22885851 OR 22902294 OR 22902295 OR 22902718 OR 22902719 OR 22902720 OR 22920251 OR 22920252 OR 22920253 OR 22920255 OR 22920257 OR 22920258 OR 22920259 OR 22920260 OR 22920262 OR 22922782 OR 22922783 OR 22922784 OR 22922785 OR 22922786 OR 22941107 OR 22941108 OR 22941109 OR 22941110 OR 22941111 OR 22958819 OR 22958820 OR 22958821 OR 22958822 OR 22958823 OR 22958824 OR 22958825 OR 22958828 OR 22958829 OR 22958830 OR 22958930 OR 22958931 OR 22958932 OR 22958933 OR 22958934 OR 22960931 OR 22960932 OR 22960933 OR 22960934 OR 22981823 OR 22983208 OR 22983209 OR 22983211 OR 22998867 OR 22998869 OR 22998870 OR 22998871 OR 22998872 OR 22998873 OR 22998875 OR 22998876 OR 22998877 OR 22998878 OR 22998879 OR 23001059 OR 23001060 OR 23001061 OR 23001062 OR 23023292 OR 23023293 OR 23023294 OR 23040474 OR 23040476 OR 23040477 OR 23040478 OR 23040479 OR 23040480 OR 23040481 OR 23040482 OR 23042081 OR 23042082 OR 23064101 OR 23064379 OR 23064381 OR 23064382 OR 23083732 OR 23083733 OR 23083734 OR 23083736 OR 23083737 OR 23083738 OR 23083739 OR 23083740 OR 23083741 OR 23083742 OR 23083743 OR 23083744 OR 23083745 OR 23084023 OR 23086334 OR 23086335 OR 23086336 OR 23103054 OR 23103964 OR 23103965 OR 23122285 OR 23122286 OR 23122287 OR 23122289 OR 23122290 OR 23122291 OR 23122292 OR 23122293 OR 23122294 OR 23141062 OR 23141063 OR 23141064 OR 23141065 OR 23141066 OR 23141067 OR 23141068 OR 23141069 OR 23141071 OR 23141072 OR 23141075 OR 23142520 OR 23142521 OR 23143511 OR 23143512 OR 23143513 OR 23143514 OR 23143515 OR 23143516 OR 23143517 OR 23143518 OR 23143519 OR 23143520 OR 23143521 OR 23143522 OR 23160043 OR 23160044 OR 23160045 OR 23168163 OR 23168164 OR 23177958 OR 23177959 OR 23177960 OR 23177961 OR 23177962 OR 23177963 OR 23177965 OR 23177966 OR 23177967 OR 23178974 OR 23178975 OR 23201972 OR 23217418 OR 23217419 OR 23217420 OR 23217423 OR 23217424 OR 23217425 OR 23217739 OR 23217740 OR 23217741 OR 23217742 OR 23217743 OR 23217744 OR 23217745 OR 23217746 OR 23217747 OR 23217748 OR 23217749 OR 23217750 OR 23222911 OR 23222912 OR 23222913 OR 23222914 OR 23242309 OR 23242310 OR 23242311 OR 23242312 OR 23246482 OR 23246483 OR 23259944 OR 23259945 OR 23259946 OR 23259947 OR 23259948 OR 23259949 OR 23259950 OR 23259951 OR 23259952 OR 23259953 OR 23259954 OR 23259955 OR 23259956 OR 23260487 OR 23260488 OR 23263442 OR 23263443 OR 23290135 OR 23290136 OR 23290137 OR 23290138 OR 23290139 OR 23290140 OR 23292679 OR 23292680 OR 23292681 OR 23292682 OR 23292683 OR 23312514 OR 23312515 OR 23312516 OR 23312517 OR 23312518 OR 23312519 OR 23312520 OR 23312521 OR 23312522 OR 23312523 OR 23312524 OR 23312525 OR 23312526 OR 23313908 OR 23313909 OR 23313910 OR 23313911)</t>
+  </si>
+  <si>
+    <t>PMID=(23313912 OR 23318055 OR 23318056 OR 23333148 OR 23333149 OR 23333150 OR 23334578 OR 23334579 OR 23334580 OR 23334581 OR 23352160 OR 23352161 OR 23352162 OR 23352164 OR 23352165 OR 23352166 OR 23352167 OR 23352168 OR 23352169 OR 23352170 OR 23352171 OR 23352605 OR 23354328 OR 23354329 OR 23354330 OR 23354331 OR 23354332 OR 23354333 OR 23354385 OR 23377126 OR 23377127 OR 23377128 OR 23395371 OR 23395373 OR 23395374 OR 23395375 OR 23395376 OR 23395377 OR 23395378 OR 23395380 OR 23395381 OR 23395382 OR 23395444 OR 23395445 OR 23395446 OR 23395447 OR 23396101 OR 23396102 OR 23415312 OR 23415913 OR 23415914 OR 23415915 OR 23416448 OR 23416450 OR 23416452 OR 23434393 OR 23434911 OR 23434912 OR 23434913 OR 23434914 OR 23434978 OR 23439118 OR 23439119 OR 23439120 OR 23439121 OR 23439122 OR 23439123 OR 23439124 OR 23439125 OR 23439126 OR 23439127 OR 23439128 OR 23439129 OR 23455607 OR 23455608 OR 23455609 OR 23455610 OR 23472870 OR 23472872 OR 23472873 OR 23472874 OR 23473315 OR 23473316 OR 23473317 OR 23473318 OR 23473319 OR 23473320 OR 23473321 OR 23473322 OR 23473323 OR 23473324 OR 23473325 OR 23473326 OR 23475112 OR 23475113 OR 23498975 OR 23499384 OR 23499385 OR 23502535 OR 23502536 OR 23522040 OR 23522041 OR 23522042 OR 23522043 OR 23522044 OR 23522045 OR 23522046 OR 23522047 OR 23522048 OR 23522049 OR 23522050 OR 23522051 OR 23523177 OR 23523592 OR 23523593 OR 23525040 OR 23525041 OR 23525042 OR 23525043 OR 23542688 OR 23542689 OR 23542690 OR 23542691 OR 23542692 OR 23561443 OR 23561444 OR 23562540 OR 23563578 OR 23563579 OR 23563580 OR 23563581 OR 23563582 OR 23583100 OR 23583109 OR 23583110 OR 23583111 OR 23583112 OR 23583113 OR 23583114 OR 23583622 OR 23583623 OR 23584742 OR 23602499 OR 23602500 OR 23602540 OR 23602541 OR 23603708 OR 23603709 OR 23622062 OR 23622063 OR 23622064 OR 23622065 OR 23622066 OR 23622067 OR 23622068 OR 23622069 OR 23623697 OR 23623698 OR 23624512 OR 23624513 OR 23624514 OR 23624515 OR 23642359 OR 23642361 OR 23642363 OR 23642364 OR 23642365 OR 23642366 OR 23642367 OR 23642368 OR 23643935 OR 23644483 OR 23644484 OR 23644485 OR 23664551 OR 23664612 OR 23664613 OR 23664614 OR 23664615 OR 23664616 OR 23664617 OR 23664618 OR 23664619 OR 23665120 OR 23665121 OR 23666178 OR 23666179 OR 23666180 OR 23666181 OR 23684539 OR 23684540 OR 23685719 OR 23685720 OR 23685721 OR 23685722 OR 23707614 OR 23708140 OR 23708142 OR 23708143 OR 23708144 OR 23719159 OR 23719161 OR 23719162 OR 23719163 OR 23719164 OR 23719165 OR 23719166 OR 23719167 OR 23727119 OR 23727120 OR 23727819 OR 23727820 OR 23727821 OR 23746629 OR 23746630 OR 23746975 OR 23746976 OR 23746977 OR 23746978 OR 23746979 OR 23746980 OR 23746981 OR 23746982 OR 23747202 OR 23747203 OR 23749144 OR 23749145 OR 23749146 OR 23749147 OR 23764282 OR 23764283 OR 23764284 OR 23764285 OR 23764286 OR 23764287 OR 23764288 OR 23764290 OR 23764291 OR 23770078 OR 23770079 OR 23770080 OR 23770256 OR 23770257 OR 23770565 OR 23790753 OR 23790754 OR 23791193 OR 23791194 OR 23791195 OR 23791196 OR 23791197 OR 23791198 OR 23791199 OR 23791200 OR 23791201 OR 23791481 OR 23792942 OR 23792943 OR 23792944 OR 23792945 OR 23792947 OR 23799472 OR 23810540 OR 23817545 OR 23817546 OR 23817547 OR 23817549 OR 23817550 OR 23827708 OR 23827709 OR 23827710 OR 23827711 OR 23827712 OR 23830830 OR 23830831 OR 23831966 OR 23849197 OR 23849198 OR 23849199 OR 23849200 OR 23849201 OR 23849202 OR 23849203 OR 23850243 OR 23850244 OR 23850245 OR 23850594 OR 23850595 OR 23852111 OR 23852112 OR 23852115 OR 23852116 OR 23852118 OR 23871232 OR 23871233 OR 23871604 OR 23871605 OR 23871606 OR 23872594 OR 23872595 OR 23872596 OR 23872597 OR 23872598 OR 23872599 OR 23889931 OR 23889932 OR 23889933 OR 23889934 OR 23889935 OR 23889936 OR 23889937 OR 23889938 OR 23891400 OR 23891401 OR 23892552 OR 23892553 OR 23892554 OR 23910081 OR 23910083 OR 23910084 OR 23910085 OR 23910086 OR 23911103 OR 23911104 OR 23912944 OR 23912945 OR 23912946 OR 23912947 OR 23912948 OR 23931994 OR 23931996 OR 23931997 OR 23931998 OR 23931999 OR 23932000 OR 23932001 OR 23932002 OR 23932490 OR 23932491 OR 23933087 OR 23933088 OR 23933748 OR 23933749 OR 23933750 OR 23933751 OR 23933752 OR 23933753 OR 23954030 OR 23954031 OR 23954751 OR 23954752 OR 23955559 OR 23955560 OR 23972593 OR 23972594 OR 23972595 OR 23972596 OR 23972597 OR 23972598 OR 23972599 OR 23972601 OR 23972602 OR 23973208 OR 23973209 OR 23974706 OR 23974707 OR 23974708 OR 23974709 OR 23974710 OR 23974711 OR 23993699 OR 23993700 OR 23995066 OR 23995067 OR 23995068 OR 23995069 OR 23995070 OR 23995071 OR 24012002 OR 24012003 OR 24012004 OR 24012005 OR 24012006 OR 24012007 OR 24012008 OR 24012009 OR 24012010 OR 24012279 OR 24012280 OR 24012369 OR 24013593 OR 24013594 OR 24035353 OR 24035354 OR 24035355 OR 24035762 OR 24035763 OR 24036913 OR 24036914 OR 24050398 OR 24050399 OR 24050400 OR 24050401 OR 24050403 OR 24050404 OR 24050405 OR 24050406 OR 24050407 OR 24050408 OR 24054998 OR 24055015 OR 24055016 OR 24056696 OR 24056697 OR 24056698 OR 24056699 OR 24056700 OR 24066359 OR 24075977 OR 24075978 OR 24077561 OR 24077562 OR 24077563 OR 24077564 OR 24077565 OR 24094102 OR 24094103 OR 24094104 OR 24094105 OR 24094106 OR 24094107 OR 24094108 OR 24094109 OR 24094110 OR 24094111 OR 24094112 OR 24094319 OR 24094320 OR 24094321 OR 24094323 OR 24094324 OR 24094325 OR 24094326 OR 24095676 OR 24097038 OR 24097039 OR 24097040 OR 24097041 OR 24097042 OR 24097043)</t>
+  </si>
+  <si>
+    <t>PMID=(24097044 OR 24120743 OR 24120744 OR 24120845 OR 24121737 OR 24121738 OR 24139037 OR 24139038 OR 24139039 OR 24139040 OR 24139041 OR 24139042 OR 24139043 OR 24139044 OR 24139045 OR 24139046 OR 24139047 OR 24139048 OR 24139049 OR 24139050 OR 24139757 OR 24139758 OR 24139759 OR 24139817 OR 24139818 OR 24141309 OR 24141310 OR 24141311 OR 24141312 OR 24141313 OR 24141314 OR 24162650 OR 24162651 OR 24162652 OR 24162653 OR 24162654 OR 24162656 OR 24183008 OR 24183013 OR 24183704 OR 24183705 OR 24185423 OR 24185424 OR 24185425 OR 24185426 OR 24185427 OR 24185428 OR 24206669 OR 24206670 OR 24209760 OR 24209762 OR 24210904 OR 24210905 OR 24210906 OR 24210907 OR 24210908 OR 24212670 OR 24212671 OR 24212672 OR 24212673 OR 24212674 OR 24239124 OR 24239125 OR 24239126 OR 24239284 OR 24239285 OR 24241394 OR 24241395 OR 24241396 OR 24241397 OR 24267649 OR 24267650 OR 24267651 OR 24267652 OR 24267653 OR 24267654 OR 24267655 OR 24267656 OR 24267657 OR 24268418 OR 24268419 OR 24268694 OR 24268695 OR 24270184 OR 24270185 OR 24270186 OR 24270187 OR 24270188 OR 24290204 OR 24292232 OR 24292233 OR 24314724 OR 24314726 OR 24314727 OR 24314728 OR 24314729 OR 24314730 OR 24314731 OR 24314732 OR 24314733 OR 24315438 OR 24315439 OR 24315440 OR 24315441 OR 24315442 OR 24315443 OR 24315444 OR 24316888 OR 24316889 OR 24316890 OR 24332836 OR 24332837 OR 24333053 OR 24333055 OR 24336150 OR 24336151 OR 24360541 OR 24360542 OR 24360543 OR 24360544 OR 24360545 OR 24360546 OR 24360547 OR 24360548 OR 24360549 OR 24360550 OR 24360551 OR 24360883 OR 24360884 OR 24361076 OR 24361077 OR 24361078 OR 24362759 OR 24362760 OR 24362761 OR 24362762 OR 24362763 OR 24373883 OR 24373884 OR 24388172 OR 24388174 OR 24388175 OR 24389009 OR 24389010 OR 24390225 OR 24390226 OR 24411732 OR 24411734 OR 24411735 OR 24411736 OR 24411737 OR 24411738 OR 24411739 OR 24412311 OR 24412312 OR 24413696 OR 24413698 OR 24413699 OR 24413700 OR 24440227 OR 24440228 OR 24440599 OR 24440600 OR 24441679 OR 24441680 OR 24441681 OR 24441682 OR 24462039 OR 24462040 OR 24462094 OR 24462095 OR 24462096 OR 24462097 OR 24462098 OR 24462100 OR 24462101 OR 24462102 OR 24462103 OR 24462105 OR 24464039 OR 24464040 OR 24464041 OR 24464042 OR 24464043 OR 24475471 OR 24486086 OR 24486087 OR 24487231 OR 24487232 OR 24487233 OR 24487234 OR 24487235 OR 24506881 OR 24506883 OR 24506884 OR 24506885 OR 24506886 OR 24507183 OR 24507188 OR 24507189 OR 24507190 OR 24507191 OR 24507192 OR 24507193 OR 24507195 OR 24507196 OR 24507197 OR 24507198 OR 24507199 OR 24508384 OR 24508385 OR 24509428 OR 24509429 OR 24529595 OR 24529596 OR 24529597 OR 24529980 OR 24529981 OR 24531306 OR 24531307 OR 24559668 OR 24559671 OR 24559672 OR 24559673 OR 24559674 OR 24559675 OR 24559676 OR 24559677 OR 24559678 OR 24559679 OR 24559680 OR 24559681 OR 24560702 OR 24560703 OR 24561082 OR 24561083 OR 24561084 OR 24561995 OR 24561996 OR 24561997 OR 24561999 OR 24562000 OR 24582926 OR 24582927 OR 24583022 OR 24583023 OR 24584049 OR 24584050 OR 24584051 OR 24584052 OR 24584054 OR 24607225 OR 24607226 OR 24607227 OR 24607228 OR 24607229 OR 24607230 OR 24607231 OR 24607232 OR 24607233 OR 24607234 OR 24607235 OR 24607236 OR 24607406 OR 24607407 OR 24609463 OR 24609466 OR 24613417 OR 24613418 OR 24630793 OR 24630794 OR 24631345 OR 24633127 OR 24656249 OR 24656250 OR 24656251 OR 24656252 OR 24656253 OR 24656254 OR 24656255 OR 24656256 OR 24656257 OR 24656258 OR 24656769 OR 24657965 OR 24657966 OR 24657967 OR 24657968 OR 24667574 OR 24671059 OR 24685176 OR 24686783 OR 24686786 OR 24686787 OR 24698267 OR 24698269 OR 24698270 OR 24698271 OR 24698272 OR 24698273 OR 24698274 OR 24698275 OR 24698276 OR 24698277 OR 24698278 OR 24702994 OR 24702996 OR 24702997 OR 24702998 OR 24704492 OR 24704493 OR 24704494 OR 24705183 OR 24705184 OR 24726192 OR 24726381 OR 24726382 OR 24728267 OR 24728268 OR 24728269 OR 24742458 OR 24742459 OR 24742460 OR 24742461 OR 24742462 OR 24742463 OR 24742464 OR 24742465 OR 24742466 OR 24742467 OR 24746419 OR 24746675 OR 24747574 OR 24747575 OR 24747576 OR 24747577 OR 24755780 OR 24768299 OR 24768300 OR 24777419 OR 24777420 OR 24792115 OR 24792116 OR 24792117 OR 24792118 OR 24792119 OR 24793032 OR 24794094 OR 24794095 OR 24811378 OR 24811379 OR 24811380 OR 24811381 OR 24811382 OR 24811383 OR 24811384 OR 24811385 OR 24813856 OR 24813857 OR 24814534 OR 24814535 OR 24816140 OR 24835569 OR 24835570 OR 24835571 OR 24836076 OR 24836077 OR 24836505 OR 24836506 OR 24853934 OR 24853937 OR 24853940 OR 24853941 OR 24853942 OR 24853943 OR 24853944 OR 24853945 OR 24853946 OR 24857020 OR 24857021 OR 24859199 OR 24859200 OR 24859201 OR 24859202 OR 24880214 OR 24880215 OR 24880216 OR 24880217 OR 24881834 OR 24905162 OR 24905167 OR 24905168 OR 24905170 OR 24908101 OR 24908103 OR 24908483 OR 24908484 OR 24908485 OR 24908486 OR 24908487 OR 24908488 OR 24908489 OR 24908490 OR 24908491 OR 24908492 OR 24908493 OR 24910077 OR 24910078 OR 24929661 OR 24930700 OR 24930701 OR 24931489 OR 24945770 OR 24945771 OR 24945772 OR 24945773 OR 24945774 OR 24945775 OR 24945776 OR 24945777 OR 24945778 OR 24952642 OR 24952643 OR 24952644 OR 24952960 OR 24952961 OR 24953180 OR 24953181 OR 24953182 OR 24974795 OR 24974797 OR 24976214 OR 24976215 OR 24991954 OR 24991955 OR 24991956 OR 24991957 OR 24991958 OR 24991959 OR 24991960 OR 24991961 OR 24991962 OR 24991963 OR 24996167 OR 24996168 OR 24996169 OR 24996170 OR 24997762 OR 24997763 OR 24997764)</t>
+  </si>
+  <si>
+    <t>PMID=(24997765 OR 25002228 OR 25002229 OR 25017010 OR 25017011 OR 25017720 OR 25017721 OR 25017722 OR 25032261 OR 25033176 OR 25033179 OR 25033180 OR 25033181 OR 25033182 OR 25033183 OR 25033184 OR 25033185 OR 25033186 OR 25033187 OR 25033188 OR 25042701 OR 25042702 OR 25043419 OR 25043420 OR 25043421 OR 25043422 OR 25064849 OR 25064850 OR 25064851 OR 25064852 OR 25066082 OR 25066084 OR 25066085 OR 25066086 OR 25066087 OR 25086606 OR 25086607 OR 25086608 OR 25086609 OR 25086610 OR 25088363 OR 25088364 OR 25088365 OR 25088366 OR 25090446 OR 25102560 OR 25102562 OR 25105579 OR 25108910 OR 25108911 OR 25108912 OR 25108913 OR 25123306 OR 25123307 OR 25123308 OR 25123309 OR 25123310 OR 25123311 OR 25123312 OR 25123313 OR 25123314 OR 25129075 OR 25129076 OR 25129077 OR 25129078 OR 25130491 OR 25130492 OR 25132466 OR 25132468 OR 25132469 OR 25144876 OR 25144877 OR 25151262 OR 25151263 OR 25151265 OR 25151266 OR 25155954 OR 25155955 OR 25155956 OR 25155957 OR 25155959 OR 25155960 OR 25158935 OR 25158936 OR 25174002 OR 25174003 OR 25174004 OR 25174005 OR 25174006 OR 25175878 OR 25175879 OR 25175880 OR 25175881 OR 25189209 OR 25189210 OR 25192459 OR 25192461 OR 25192463 OR 25192464 OR 25195102 OR 25195103 OR 25195104 OR 25195105 OR 25199702 OR 25199703 OR 25199705 OR 25199706 OR 25199707 OR 25217827 OR 25220291 OR 25220810 OR 25220811 OR 25220812 OR 25220813 OR 25220814 OR 25242216 OR 25242217 OR 25242218 OR 25242219 OR 25242221 OR 25242222 OR 25242304 OR 25242305 OR 25242306 OR 25242307 OR 25262493 OR 25262494 OR 25262495 OR 25262496 OR 25263752 OR 25263753 OR 25263754 OR 25263755 OR 25277454 OR 25277455 OR 25277456 OR 25280219 OR 25280220 OR 25280221 OR 25282614 OR 25282615 OR 25282616 OR 25284005 OR 25284006 OR 25284007 OR 25306549 OR 25306550 OR 25308330 OR 25308331 OR 25312494 OR 25312495 OR 25312496 OR 25326689 OR 25326690 OR 25344628 OR 25344630 OR 25344631 OR 25347353 OR 25362470 OR 25362471 OR 25362472 OR 25362473 OR 25362474 OR 25374357 OR 25374358 OR 25374359 OR 25374360 OR 25374361 OR 25374362 OR 25374363 OR 25374364 OR 25383899 OR 25383900 OR 25383901 OR 25383902 OR 25383903 OR 25383904 OR 25402853 OR 25402854 OR 25402856 OR 25402857 OR 25402858 OR 25420066 OR 25420067 OR 25420068 OR 25420069 OR 25420070 OR 25433636 OR 25433637 OR 25433639 OR 25433640 OR 25436666 OR 25442928 OR 25442930 OR 25447740 OR 25447741 OR 25447742 OR 25451192 OR 25451193 OR 25451194 OR 25451195 OR 25451196 OR 25451197 OR 25453841 OR 25453842 OR 25453843 OR 25453844 OR 25456497 OR 25456498 OR 25456499 OR 25456500 OR 25456834 OR 25459407 OR 25459408 OR 25459409 OR 25465113 OR 25465114 OR 25465115 OR 25465116 OR 25467916 OR 25467978 OR 25467979 OR 25467980 OR 25467981 OR 25467982 OR 25467983 OR 25467984 OR 25467985 OR 25467986 OR 25469543 OR 25479748 OR 25479749 OR 25479750 OR 25479751 OR 25479752 OR 25482025 OR 25482027 OR 25485755 OR 25485756 OR 25485757 OR 25485758 OR 25485759 OR 25500157 OR 25500502 OR 25501035 OR 25501036 OR 25501037 OR 25515522 OR 25517460 OR 25517461 OR 25517462 OR 25517463 OR 25517465 OR 25517466 OR 25517467 OR 25517468 OR 25517469 OR 25521377 OR 25521378 OR 25521379 OR 25521380 OR 25521381 OR 25531569 OR 25531570 OR 25531571 OR 25531572 OR 25531573 OR 25533131 OR 25533481 OR 25533482 OR 25533483 OR 25533484 OR 25533485 OR 25543456 OR 25543457 OR 25543458 OR 25556833 OR 25556834 OR 25556835 OR 25556836 OR 25559081 OR 25559082 OR 25569347 OR 25569348 OR 25569349 OR 25569350 OR 25569351 OR 25575079 OR 25575080 OR 25575081 OR 25578362 OR 25578363 OR 25578364 OR 25581359 OR 25581360 OR 25581361 OR 25581362 OR 25581363 OR 25581364 OR 25599221 OR 25599222 OR 25599223 OR 25599224 OR 25600124 OR 25600643 OR 25611508 OR 25611509 OR 25611510 OR 25611511 OR 25611512 OR 25611513 OR 25611514 OR 25619653 OR 25619654 OR 25619655 OR 25619656 OR 25619657 OR 25619658 OR 25619659 OR 25620640 OR 25622143 OR 25622144 OR 25622145 OR 25622146 OR 25640075 OR 25640077 OR 25640078 OR 25643294 OR 25643295 OR 25643296 OR 25643297 OR 25643298 OR 25643299 OR 25654255 OR 25654256 OR 25654258 OR 25654259 OR 25658368 OR 25658370 OR 25658371 OR 25658372 OR 25658373 OR 25661179 OR 25661180 OR 25661182 OR 25661184 OR 25661185 OR 25664911 OR 25664912 OR 25664913 OR 25664914 OR 25683224 OR 25695269 OR 25695270 OR 25695271 OR 25704240 OR 25704948 OR 25704949 OR 25704950 OR 25704951 OR 25706471 OR 25706472 OR 25706473 OR 25706475 OR 25706476 OR 25710834 OR 25714049 OR 25728570 OR 25728571 OR 25728572 OR 25730668 OR 25730669 OR 25730670 OR 25730671 OR 25730672 OR 25730673 OR 25732245 OR 25741721 OR 25741722 OR 25741723 OR 25741724 OR 25741725 OR 25741726 OR 25741727 OR 25741728 OR 25741729 OR 25741730 OR 25741731 OR 25748933 OR 25748934 OR 25748935 OR 25751531 OR 25751532 OR 25751533 OR 25751534 OR 25754820 OR 25754821 OR 25754822 OR 25754823 OR 25754824 OR 25754825 OR 25754826 OR 25754827 OR 25772071 OR 25772072 OR 25772073 OR 25772189 OR 25774450 OR 25774451 OR 25789755 OR 25789756 OR 25799040 OR 25800778 OR 25800779 OR 25801703 OR 25801704 OR 25801705 OR 25801706 OR 25803835 OR 25819610 OR 25819612 OR 25819613 OR 25819614 OR 25821910 OR 25821912 OR 25821913 OR 25821914 OR 25842974 OR 25842977 OR 25842978 OR 25842979 OR 25843401 OR 25843402 OR 25843403 OR 25843404 OR 25843405 OR 25843406 OR 25843407 OR 25849986 OR 25849988 OR 25849989 OR 25856479 OR 25864631 OR 25864632 OR 25864633 OR 25864636 OR 25865501 OR 25867120 OR 25867121 OR 25867122)</t>
+  </si>
+  <si>
+    <t>PMID=(25891906 OR 25891907 OR 25892299 OR 25892301 OR 25892302 OR 25892303 OR 25892305 OR 25913856 OR 25913857 OR 25913858 OR 25913860 OR 25913861 OR 25915473 OR 25915474 OR 25915475 OR 25915476 OR 25915477 OR 25919956 OR 25921272 OR 25921273 OR 25936915 OR 25936916 OR 25936917 OR 25937169 OR 25937170 OR 25937171 OR 25937173 OR 25937174 OR 25938883 OR 25938884 OR 25938885 OR 25957901 OR 25957903 OR 25957904 OR 25959730 OR 25959731 OR 25959732 OR 25959733 OR 25959734 OR 25961790 OR 25961791 OR 25961792 OR 25982367 OR 25984889 OR 25996135 OR 25996136 OR 25996137 OR 26004780 OR 26004781 OR 26004914 OR 26004915 OR 26005848 OR 26005849 OR 26005850 OR 26005851 OR 26005852 OR 26028574 OR 26028575 OR 26030846 OR 26030847 OR 26030848 OR 26030849 OR 26030850 OR 26030851 OR 26046757 OR 26046758 OR 26046762 OR 26050035 OR 26050036 OR 26050037 OR 26050038 OR 26050039 OR 26050040 OR 26050041 OR 26050042 OR 26050043 OR 26050044 OR 26050045 OR 26051420 OR 26051421 OR 26053402 OR 26053403 OR 26074003 OR 26074004 OR 26074005 OR 26074006 OR 26075643 OR 26087164 OR 26087166 OR 26087167 OR 26087168 OR 26094607 OR 26094608 OR 26095046 OR 26095047 OR 26095048 OR 26098757 OR 26098758 OR 26119026 OR 26119234 OR 26119235 OR 26119236 OR 26120961 OR 26120962 OR 26120963 OR 26120964 OR 26139371 OR 26139372 OR 26139373 OR 26139374 OR 26139375 OR 26139376 OR 26140603 OR 26140605 OR 26140606 OR 26143660 OR 26145478 OR 26147532 OR 26147533 OR 26165924 OR 26165925 OR 26167904 OR 26167905 OR 26167906 OR 26182412 OR 26182416 OR 26182417 OR 26182418 OR 26182419 OR 26182420 OR 26182422 OR 26182423 OR 26182424 OR 26189426 OR 26192746 OR 26192747 OR 26192748 OR 26212079 OR 26212080 OR 26212709 OR 26212710 OR 26212711 OR 26212712 OR 26214369 OR 26214370 OR 26214371 OR 26214372 OR 26214373 OR 26235340 OR 26235341 OR 26237362 OR 26237364 OR 26237365 OR 26237366 OR 26237367 OR 26247067 OR 26247861 OR 26247862 OR 26247863 OR 26247864 OR 26247865 OR 26247867 OR 26253200 OR 26253201 OR 26253202 OR 26257053 OR 26258682 OR 26279266 OR 26279267 OR 26280760 OR 26291158 OR 26291159 OR 26291160 OR 26291161 OR 26291162 OR 26291163 OR 26291164 OR 26291165 OR 26291166 OR 26291167 OR 26291168 OR 26298276 OR 26298277 OR 26299473 OR 26299474 OR 26299571 OR 26299572 OR 26299573 OR 26301325 OR 26301326 OR 26301327 OR 26308983 OR 26321199 OR 26321200 OR 26321201 OR 26321202 OR 26322925 OR 26322926 OR 26322927 OR 26322928 OR 26335637 OR 26335643 OR 26335644 OR 26335645 OR 26335646 OR 26335647 OR 26335648 OR 26335649 OR 26340527 OR 26340528 OR 26352792 OR 26365765 OR 26365766 OR 26365767 OR 26368943 OR 26368944 OR 26386518 OR 26387754 OR 26387755 OR 26387756 OR 26389840 OR 26389841 OR 26389842 OR 26402602 OR 26402603 OR 26402605 OR 26402606 OR 26402607 OR 26402608 OR 26402609 OR 26402610 OR 26402611 OR 26402612 OR 26412489 OR 26412490 OR 26412491 OR 26412560 OR 26412561 OR 26412562 OR 26414614 OR 26414615 OR 26414616 OR 26431182 OR 26431183 OR 26436900 OR 26436901 OR 26436902 OR 26436904 OR 26439527 OR 26439528 OR 26439529 OR 26439530 OR 26440282 OR 26456047 OR 26456048 OR 26456685 OR 26456686 OR 26457551 OR 26457552 OR 26457553 OR 26457554 OR 26457555 OR 26479587 OR 26479588 OR 26479589 OR 26479590 OR 26481035 OR 26481037 OR 26481038 OR 26481520 OR 26494277 OR 26494278 OR 26494279 OR 26494280 OR 26502260 OR 26502261 OR 26502262 OR 26523642 OR 26523643 OR 26523644 OR 26523645 OR 26523646 OR 26526390 OR 26526392 OR 26526393 OR 26526723 OR 26526724 OR 26526725 OR 26526726 OR 26539889 OR 26539890 OR 26539891 OR 26539892 OR 26539893 OR 26539894 OR 26549106 OR 26549107 OR 26549331 OR 26549332 OR 26551541 OR 26551542 OR 26551543 OR 26551544 OR 26551545 OR 26551546 OR 26571459 OR 26571460 OR 26586181 OR 26586183 OR 26590343 OR 26590344 OR 26590345 OR 26590346 OR 26590347 OR 26590348 OR 26593091 OR 26593092 OR 26593093 OR 26593094 OR 26593959 OR 26595651 OR 26595652 OR 26595653 OR 26595654 OR 26595655 OR 26595656 OR 26606996 OR 26606997 OR 26606998 OR 26607000 OR 26607380 OR 26607381 OR 26607382 OR 26619357 OR 26619358 OR 26627309 OR 26627310 OR 26627311 OR 26627312 OR 26627594 OR 26637796 OR 26637797 OR 26637798 OR 26637799 OR 26637800 OR 26637943 OR 26642087 OR 26642088 OR 26642089 OR 26642090 OR 26642091 OR 26642092 OR 26656643 OR 26656644 OR 26656645 OR 26656646 OR 26669894 OR 26669898 OR 26669899 OR 26671460 OR 26671461 OR 26671462 OR 26671463 OR 26673659 OR 26686465 OR 26686466 OR 26687220 OR 26687221 OR 26687222 OR 26687223 OR 26687224 OR 26687225 OR 26687838 OR 26687840 OR 26687841 OR 26691828 OR 26691829 OR 26691830 OR 26691831 OR 26691832 OR 26691833 OR 26691834 OR 26711115 OR 26711116 OR 26711117 OR 26711118 OR 26711119 OR 26712580 OR 26713739 OR 26713740 OR 26727548 OR 26727549 OR 26748088 OR 26748089 OR 26748090 OR 26748091 OR 26748092 OR 26748418 OR 26748419 OR 26748751 OR 26748752 OR 26748753 OR 26748757 OR 26748758 OR 26752157 OR 26752158 OR 26752159 OR 26752160 OR 26752161 OR 26752162 OR 26774159 OR 26774160 OR 26774161 OR 26774162 OR 26777273 OR 26777274 OR 26777275 OR 26777276 OR 26777277 OR 26780508 OR 26780509 OR 26780511 OR 26780512 OR 26796690 OR 26796691 OR 26796692 OR 26804989 OR 26804990 OR 26804991 OR 26804992 OR 26804993 OR 26804994 OR 26804995 OR 26804996 OR 26804997 OR 26807950 OR 26807951 OR 26807952 OR 26829649 OR 26831517 OR 26831518 OR 26833134 OR 26833135 OR 26833136 OR 26844830 OR 26844831 OR 26844832 OR 26844833 OR 26844834 OR 26844835)</t>
+  </si>
+  <si>
+    <t>PMID=(26844836 OR 26849305 OR 26853301 OR 26853302 OR 26853303 OR 26853304 OR 26853305 OR 26853306 OR 26853856 OR 26854803 OR 26854804 OR 26875622 OR 26875623 OR 26875624 OR 26875625 OR 26875626 OR 26877223 OR 26877224 OR 26878671 OR 26878672 OR 26878674 OR 26889811 OR 26898775 OR 26898776 OR 26898777 OR 26898778 OR 26898779 OR 26900923 OR 26900924 OR 26900925 OR 26900926 OR 26900927 OR 26906503 OR 26908146 OR 26923201 OR 26923202 OR 26924434 OR 26924435 OR 26924436 OR 26924437 OR 26924438 OR 26924439 OR 26924440 OR 26928063 OR 26928064 OR 26928065 OR 26928066 OR 26938441 OR 26938442 OR 26938443 OR 26942852 OR 26942853 OR 26948889 OR 26948890 OR 26948891 OR 26948895 OR 26948896 OR 26950004 OR 26950005 OR 26950006 OR 26952870 OR 26971819 OR 26971820 OR 26971945 OR 26971946 OR 26971947 OR 26971948 OR 26971949 OR 26971950 OR 26974950 OR 26974951 OR 26985724 OR 26996083 OR 26996084 OR 26996597 OR 26996598 OR 26996599 OR 26998601 OR 27019013 OR 27019014 OR 27019015 OR 27021170 OR 27021171 OR 27021172 OR 27021173 OR 27038591 OR 27041497 OR 27041498 OR 27041499 OR 27041500 OR 27041501 OR 27041502 OR 27041503 OR 27043290 OR 27044474 OR 27053299 OR 27053300 OR 27058933 OR 27058937 OR 27058938 OR 27065363 OR 27065364 OR 27065365 OR 27068789 OR 27068790 OR 27068791 OR 27089019 OR 27089020 OR 27089021 OR 27100196 OR 27100197 OR 27100198 OR 27110916 OR 27110917 OR 27110918 OR 27110919 OR 27112494 OR 27112495 OR 27112496 OR 27112497 OR 27112498 OR 27112499 OR 27116388 OR 27133462 OR 27133463 OR 27133464 OR 27133465 OR 27133466 OR 27133794 OR 27133795 OR 27133796 OR 27135215 OR 27135216 OR 27135217 OR 27146266 OR 27146267 OR 27146268 OR 27146269 OR 27146270 OR 27146271 OR 27151456 OR 27151457 OR 27151458 OR 27151639 OR 27151641 OR 27152440 OR 27152441 OR 27152443 OR 27159800 OR 27161522 OR 27161523 OR 27161524 OR 27161525 OR 27161526 OR 27161527 OR 27161528 OR 27162029 OR 27179424 OR 27181058 OR 27181059 OR 27181060 OR 27181061 OR 27181062 OR 27182817 OR 27182818 OR 27184401 OR 27196974 OR 27196975 OR 27196976 OR 27196977 OR 27196978 OR 27210550 OR 27210551 OR 27210552 OR 27210553 OR 27210554 OR 27210555 OR 27212702 OR 27212703 OR 27214567 OR 27214568 OR 27237736 OR 27237737 OR 27238864 OR 27238865 OR 27238866 OR 27238867 OR 27238868 OR 27239936 OR 27239937 OR 27239938 OR 27239939 OR 27239940 OR 27253448 OR 27257757 OR 27257758 OR 27257759 OR 27257763 OR 27263968 OR 27263969 OR 27263970 OR 27263971 OR 27263972 OR 27263973 OR 27263974 OR 27263975 OR 27273766 OR 27273767 OR 27273768 OR 27273769 OR 27292187 OR 27292188 OR 27292189 OR 27292535 OR 27292536 OR 27292537 OR 27292538 OR 27292539 OR 27294508 OR 27294509 OR 27294510 OR 27294511 OR 27294512 OR 27294513 OR 27320040 OR 27320041 OR 27320042 OR 27321921 OR 27321922 OR 27321923 OR 27321924 OR 27321925 OR 27321926 OR 27321927 OR 27322417 OR 27322418 OR 27322419 OR 27322420 OR 27345836 OR 27345837 OR 27345838 OR 27346528 OR 27346529 OR 27346530 OR 27346531 OR 27346532 OR 27346533 OR 27348214 OR 27348215 OR 27348216 OR 27373830 OR 27373831 OR 27373832 OR 27373833 OR 27373834 OR 27373835 OR 27374787 OR 27374788 OR 27374789 OR 27376765 OR 27376984 OR 27387648 OR 27387649 OR 27387650 OR 27392223 OR 27397516 OR 27397518 OR 27397520 OR 27399842 OR 27399843 OR 27399844 OR 27424782 OR 27424783 OR 27424784 OR 27427459 OR 27427460 OR 27427461 OR 27427462 OR 27428650 OR 27428651 OR 27428652 OR 27428653 OR 27437910 OR 27452173 OR 27452175 OR 27452176 OR 27455109 OR 27455110 OR 27476965 OR 27476966 OR 27476967 OR 27477018 OR 27477019 OR 27477020 OR 27478016 OR 27478017 OR 27478018 OR 27478019 OR 27479844 OR 27494673 OR 27497216 OR 27497217 OR 27497218 OR 27497221 OR 27497222 OR 27497223 OR 27497224 OR 27499081 OR 27499082 OR 27499083 OR 27499084 OR 27499085 OR 27499086 OR 27499087 OR 27500407 OR 27523426 OR 27524438 OR 27524439 OR 27524440 OR 27524441 OR 27526204 OR 27526205 OR 27526206 OR 27537478 OR 27537479 OR 27537480 OR 27537481 OR 27537483 OR 27537484 OR 27537485 OR 27537486 OR 27537487 OR 27545503 OR 27545504 OR 27545505 OR 27545506 OR 27545711 OR 27545712 OR 27545713 OR 27545714 OR 27545715 OR 27548245 OR 27568515 OR 27568516 OR 27568517 OR 27568518 OR 27568519 OR 27570066 OR 27570067 OR 27570068 OR 27571008 OR 27571009 OR 27571010 OR 27571191 OR 27588745 OR 27593177 OR 27593178 OR 27593179 OR 27593180 OR 27593181 OR 27595384 OR 27595385 OR 27595386 OR 27608754 OR 27608755 OR 27608756 OR 27608757 OR 27608758 OR 27608760 OR 27618216 OR 27618217 OR 27618218 OR 27618309 OR 27618310 OR 27618311 OR 27618671 OR 27618672 OR 27618674 OR 27618675 OR 27618676 OR 27618677 OR 27641304 OR 27641305 OR 27641306 OR 27641493 OR 27641494 OR 27641495 OR 27641496 OR 27643429 OR 27643430 OR 27643431 OR 27643432 OR 27657444 OR 27657445 OR 27657446 OR 27657447 OR 27657449 OR 27657450 OR 27657451 OR 27657452 OR 27666009 OR 27666010 OR 27666011 OR 27667003 OR 27667004 OR 27667005 OR 27667006 OR 27667007 OR 27667008 OR 27668389 OR 27668390 OR 27669988 OR 27669989 OR 27669990 OR 27693254 OR 27693255 OR 27693256 OR 27693258 OR 27694990 OR 27694991 OR 27694992 OR 27694993 OR 27694994 OR 27694995 OR 27710784 OR 27710786 OR 27710787 OR 27710788 OR 27710789 OR 27710790 OR 27710791 OR 27710792 OR 27710793 OR 27716522 OR 27720481 OR 27720482 OR 27720483 OR 27720484 OR 27720485 OR 27720486 OR 27720487 OR 27720488 OR 27723744 OR 27723745 OR 27723746 OR 27746098 OR 27746130 OR 27746131 OR 27746132 OR 27749825)</t>
+  </si>
+  <si>
+    <t>PMID=(27749826 OR 27749827 OR 27749828 OR 27749829 OR 27764656 OR 27764657 OR 27764658 OR 27764659 OR 27764660 OR 27764662 OR 27764663 OR 27764667 OR 27764668 OR 27764669 OR 27764670 OR 27764671 OR 27764672 OR 27764673 OR 27764674 OR 27773583 OR 27775719 OR 27775720 OR 27775721 OR 27775722 OR 27798629 OR 27798630 OR 27798631 OR 27798632 OR 27798633 OR 27809998 OR 27810002 OR 27810010 OR 27814478 OR 27814480 OR 27817979 OR 27820602 OR 27839998 OR 27839999 OR 27840000 OR 27840001 OR 27840020 OR 27840021 OR 27840022 OR 27842071 OR 27866796 OR 27866797 OR 27866798 OR 27866799 OR 27866800 OR 27867035 OR 27867036 OR 27867037 OR 27869800 OR 27869801 OR 27883896 OR 27883897 OR 27883898 OR 27883899 OR 27883900 OR 27889097 OR 27889317 OR 27889318 OR 27889319 OR 27893726 OR 27893727 OR 27912089 OR 27912091 OR 27916453 OR 27916456 OR 27916457 OR 27916458 OR 27918529 OR 27918530 OR 27918531 OR 27918532 OR 27930903 OR 27930904 OR 27930905 OR 27930906 OR 27930907 OR 27930908 OR 27939217 OR 27939218 OR 27939219 OR 27939579 OR 27939580 OR 27939581 OR 27939583 OR 27939584 OR 27941788 OR 27941789 OR 27941790 OR 27974162 OR 27974163 OR 27974164 OR 27989456 OR 27989457 OR 27989458 OR 27989461 OR 27989463 OR 27989768 OR 27989769 OR 27989770 OR 27991897 OR 27991898 OR 27991899 OR 27991900 OR 27991901 OR 28009267 OR 28009268 OR 28009269 OR 28009270 OR 28009271 OR 28009272 OR 28009274 OR 28009276 OR 28009277 OR 28009278 OR 28017470 OR 28017471 OR 28017472 OR 28017794 OR 28017795 OR 28017796 OR 28024158 OR 28024159 OR 28025983 OR 28025984 OR 28041881 OR 28041882 OR 28041883 OR 28041884 OR 28041894 OR 28041895 OR 28041896 OR 28056340 OR 28056342 OR 28056344 OR 28056345 OR 28056346 OR 28056347 OR 28061350 OR 28065650 OR 28067902 OR 28067903 OR 28067904 OR 28067905 OR 28089908 OR 28089909 OR 28089910 OR 28092659 OR 28094016 OR 28094017 OR 28094018 OR 28103471 OR 28103472 OR 28103473 OR 28103474 OR 28103478 OR 28103479 OR 28103480 OR 28103481 OR 28103482 OR 28103483 OR 28111077 OR 28111080 OR 28111081 OR 28111082 OR 28111199 OR 28111200 OR 28111201 OR 28114293 OR 28114294 OR 28114295 OR 28114296 OR 28132824 OR 28132825 OR 28132826 OR 28132827 OR 28132828 OR 28132829 OR 28132830 OR 28132833 OR 28132834 OR 28132835 OR 28135239 OR 28135240 OR 28135241 OR 28135242 OR 28135243 OR 28157497 OR 28162806 OR 28162807 OR 28162808 OR 28162809 OR 28166219 OR 28166220 OR 28166221 OR 28182899 OR 28182900 OR 28182901 OR 28182902 OR 28182903 OR 28182906 OR 28190640 OR 28190641 OR 28190642 OR 28190643 OR 28192394 OR 28192395 OR 28192396 OR 28196600 OR 28196601 OR 28215557 OR 28215558 OR 28215559 OR 28215825 OR 28218914 OR 28218915 OR 28218916 OR 28218917 OR 28231464 OR 28231465 OR 28231466 OR 28231467 OR 28231468 OR 28231469 OR 28231470 OR 28238546 OR 28238547 OR 28238549 OR 28238551 OR 28250408 OR 28250409 OR 28253233 OR 28262416 OR 28262417 OR 28263300 OR 28263301 OR 28263302 OR 28279351 OR 28279352 OR 28279353 OR 28279354 OR 28279355 OR 28279356 OR 28285819 OR 28285820 OR 28285821 OR 28285822 OR 28285823 OR 28285824 OR 28285903 OR 28285904 OR 28285905 OR 28288124 OR 28288125 OR 28288126 OR 28288127 OR 28288128 OR 28318784 OR 28319608 OR 28319609 OR 28319610 OR 28330582 OR 28334598 OR 28334599 OR 28334600 OR 28334601 OR 28334602 OR 28334606 OR 28334607 OR 28334608 OR 28334609 OR 28334610 OR 28334611 OR 28334612 OR 28343864 OR 28343865 OR 28343867 OR 28343868 OR 28343869 OR 28343982 OR 28343983 OR 28343984 OR 28346452 OR 28346453 OR 28366587 OR 28366588 OR 28366589 OR 28368384 OR 28368385 OR 28384467 OR 28384468 OR 28384469 OR 28384470 OR 28384472 OR 28384475 OR 28384476 OR 28384479 OR 28388428 OR 28388429 OR 28388430 OR 28388431 OR 28388432 OR 28392070 OR 28392071 OR 28392072 OR 28394322 OR 28394323 OR 28394324 OR 28414331 OR 28414332 OR 28414333 OR 28416077 OR 28426960 OR 28426961 OR 28426962 OR 28426963 OR 28426964 OR 28426965 OR 28426966 OR 28426967 OR 28426968 OR 28426969 OR 28426970 OR 28426971 OR 28434800 OR 28434801 OR 28434802 OR 28436980 OR 28436981 OR 28436982 OR 28457596 OR 28457748 OR 28457749 OR 28457750 OR 28459441 OR 28459442 OR 28472644 OR 28472645 OR 28472646 OR 28472647 OR 28472651 OR 28472653 OR 28472654 OR 28472656 OR 28472659 OR 28472660 OR 28472661 OR 28475884 OR 28481348 OR 28481349 OR 28481350 OR 28504117 OR 28504671 OR 28504672 OR 28504673 OR 28506464 OR 28506465 OR 28521119 OR 28521120 OR 28521121 OR 28521122 OR 28521123 OR 28521124 OR 28521125 OR 28521129 OR 28521130 OR 28521131 OR 28521132 OR 28521133 OR 28521134 OR 28521135 OR 28521138 OR 28521139 OR 28521140 OR 28521141 OR 28526555 OR 28530661 OR 28530662 OR 28530663 OR 28530664 OR 28552314 OR 28553943 OR 28553944 OR 28581479 OR 28581480 OR 28602620 OR 28602689 OR 28604683 OR 28604684 OR 28604685 OR 28625485 OR 28625486 OR 28625487 OR 28625488 OR 28628100 OR 28628101 OR 28628102 OR 28628103 OR 28628104 OR 28641101 OR 28641102 OR 28641103 OR 28641104 OR 28641105 OR 28641109 OR 28641110 OR 28641111 OR 28641112 OR 28641113 OR 28641114 OR 28641115 OR 28641116 OR 28648363 OR 28648364 OR 28648365 OR 28648497 OR 28648498 OR 28648499 OR 28648500 OR 28669543 OR 28669544 OR 28669545 OR 28669546 OR 28671691 OR 28671692 OR 28671693 OR 28671694 OR 28671695 OR 28671696 OR 28683262 OR 28683263 OR 28683264 OR 28683266 OR 28683267 OR 28683269 OR 28683270 OR 28683271 OR 28683272 OR 28683273 OR 28686860 OR 28686865 OR 28686870 OR 28689980 OR 28689981 OR 28689982 OR 28689983 OR 28689984)</t>
+  </si>
+  <si>
+    <t>PMID=(28692061 OR 28692062 OR 28712652 OR 28712653 OR 28712654 OR 28712938 OR 28714951 OR 28714952 OR 28714953 OR 28714954 OR 28728018 OR 28728022 OR 28728023 OR 28728024 OR 28728025 OR 28728026 OR 28735746 OR 28735747 OR 28735748 OR 28735749 OR 28735750 OR 28736215 OR 28736216 OR 28736217 OR 28757304 OR 28757305 OR 28757306 OR 28757360 OR 28758994 OR 28758995 OR 28758996 OR 28758997 OR 28758998 OR 28758999 OR 28772121 OR 28772122 OR 28772123 OR 28772124 OR 28772125 OR 28777942 OR 28777944 OR 28777945 OR 28777946 OR 28781167 OR 28781168 OR 28781169 OR 28783139 OR 28783140 OR 28803732 OR 28803918 OR 28803919 OR 28803920 OR 28805814 OR 28805815 OR 28805816 OR 28817792 OR 28817793 OR 28817794 OR 28817795 OR 28817796 OR 28817799 OR 28817800 OR 28817801 OR 28817802 OR 28817804 OR 28817805 OR 28823726 OR 28823728 OR 28823729 OR 28823730 OR 28825718 OR 28825719 OR 28826723 OR 28844526 OR 28844837 OR 28846081 OR 28846083 OR 28858611 OR 28858614 OR 28858616 OR 28858617 OR 28858618 OR 28858619 OR 28858621 OR 28858624 OR 28858625 OR 28858626 OR 28858627 OR 28867551 OR 28867552 OR 28869581 OR 28869582 OR 28869583 OR 28869584 OR 28886366 OR 28886367 OR 28890345 OR 28892057 OR 28892058 OR 28910611 OR 28910612 OR 28910613 OR 28910614 OR 28910615 OR 28910619 OR 28910620 OR 28910621 OR 28910622 OR 28910623 OR 28910624 OR 28919175 OR 28919367 OR 28920932 OR 28920933 OR 28920934 OR 28920935 OR 28920936 OR 28943028 OR 28943029 OR 28943231 OR 28945220 OR 28945221 OR 28945222 OR 28957662 OR 28957663 OR 28957664 OR 28957665 OR 28957667 OR 28957668 OR 28957669 OR 28957670 OR 28957671 OR 28957674 OR 28957677 OR 28957678 OR 28957679 OR 28957680 OR 28957681 OR 28965765 OR 28965766 OR 28965767 OR 28965997 OR 28967909 OR 28967910 OR 28985523 OR 28985524 OR 28985526 OR 28985527 OR 28985528 OR 28985529 OR 29024648 OR 29024650 OR 29024651 OR 29024657 OR 29024658 OR 29024659 OR 29024660 OR 29024661 OR 29024662 OR 29024663 OR 29024664 OR 29024665 OR 29024666 OR 29024667 OR 29024668 OR 29024669 OR 29033205 OR 29033351 OR 29033352 OR 29033353 OR 29056294 OR 29056295 OR 29056296 OR 29056297 OR 29056298 OR 29056299 OR 29100010 OR 29100012 OR 29100013 OR 29100014 OR 29100015 OR 29103804 OR 29103805 OR 29103806 OR 29103807 OR 29103808 OR 29107517 OR 29107518 OR 29107519 OR 29107520 OR 29107521 OR 29107522 OR 29107523 OR 29129523 OR 29144974 OR 29154125 OR 29154126 OR 29154127 OR 29154128 OR 29154129 OR 29154130 OR 29174331 OR 29174332 OR 29174333 OR 29180747 OR 29180748 OR 29184197 OR 29184198 OR 29184199 OR 29184200 OR 29184201 OR 29184202 OR 29184203 OR 29184204 OR 29184206 OR 29184207 OR 29184208 OR 29184209 OR 29184212 OR 29198754 OR 29198756 OR 29198757 OR 29198940 OR 29198941 OR 29198942 OR 29203896 OR 29203897 OR 29216448 OR 29216449 OR 29216450 OR 29216451 OR 29220665 OR 29220666 OR 29220667 OR 29224721 OR 29224722 OR 29224723 OR 29224724 OR 29224725 OR 29224726 OR 29224727 OR 29230051 OR 29230052 OR 29230053 OR 29230054 OR 29230055 OR 29230056 OR 29230057 OR 29230058 OR 29230059 OR 29249282 OR 29249283 OR 29249284 OR 29249285 OR 29249286 OR 29249287 OR 29249288 OR 29249289 OR 29249462 OR 29249463 OR 29249464 OR 29268095 OR 29268096 OR 29268097 OR 29268098 OR 29268099 OR 29273772 OR 29276054 OR 29276055 OR 29276056 OR 29276141 OR 29276142 OR 29276143 OR 29290548 OR 29290549 OR 29290550 OR 29290552 OR 29290553 OR 29290554 OR 29290616 OR 29290617 OR 29292378 OR 29301098 OR 29301100 OR 29301106 OR 29304339 OR 29304344 OR 29307709 OR 29307710 OR 29307712 OR 29311741 OR 29311742 OR 29311743 OR 29311744 OR 29311745 OR 29311746 OR 29335603 OR 29335604 OR 29335605 OR 29335606 OR 29335607 OR 29335608 OR 29337181 OR 29337182 OR 29337183 OR 29346752 OR 29346754 OR 29358017 OR 29358044 OR 29358666 OR 29379116 OR 29379117 OR 29395054 OR 29395055 OR 29395056 OR 29395906 OR 29395907 OR 29395908 OR 29395909 OR 29395910 OR 29395911 OR 29395912 OR 29395913 OR 29395914 OR 29395915 OR 29395916 OR 29397273 OR 29398355 OR 29398356 OR 29398357 OR 29398358 OR 29398359 OR 29398360 OR 29398361 OR 29398362 OR 29398363 OR 29398364 OR 29398365 OR 29398366 OR 29403029 OR 29403030 OR 29403032 OR 29403033 OR 29403034 OR 29420933 OR 29420934 OR 29420935 OR 29429933 OR 29429934 OR 29429935 OR 29429936 OR 29429937 OR 29429938 OR 29429939 OR 29429943 OR 29434375 OR 29434377 OR 29451855 OR 29456026 OR 29456158 OR 29456159 OR 29459763 OR 29459764 OR 29463850 OR 29470967 OR 29472620 OR 29478844 OR 29478915 OR 29478916 OR 29478917 OR 29483663 OR 29483664 OR 29499147 OR 29499153 OR 29499154 OR 29499155 OR 29503184 OR 29503185 OR 29503186 OR 29503187 OR 29503188 OR 29503189 OR 29503190 OR 29503191 OR 29503192 OR 29507408 OR 29507409 OR 29507410 OR 29507411 OR 29507412 OR 29507413 OR 29507414 OR 29518356 OR 29518357 OR 29518358 OR 29518359 OR 29526553 OR 29526554 OR 29531361 OR 29531362 OR 29531364 OR 29551301 OR 29551489 OR 29551490 OR 29551491 OR 29551492 OR 29551493 OR 29556025 OR 29556028 OR 29556029 OR 29556030 OR 29566793 OR 29566794 OR 29576387 OR 29576388 OR 29576389 OR 29576390 OR 29606579 OR 29606580 OR 29606581 OR 29606582 OR 29621484 OR 29621485 OR 29621487 OR 29621490 OR 29625067 OR 29625068 OR 29625069 OR 29625070 OR 29625071 OR 29625072 OR 29628186 OR 29628187 OR 29628188 OR 29632359 OR 29632360 OR 29632361 OR 29656871 OR 29656872 OR 29656873 OR 29656874 OR 29656875 OR 29656876 OR 29656941 OR 29656943 OR 29662213 OR 29662214 OR 29662216 OR 29662217 OR 29673481)</t>
+  </si>
+  <si>
+    <t>PMID=(29673482 OR 29673483 OR 29673484 OR 29673485 OR 29681515 OR 29681516 OR 29681530 OR 29681531 OR 29681532 OR 29681533 OR 29681534 OR 29686260 OR 29686261 OR 29686262 OR 29706577 OR 29706582 OR 29706583 OR 29706584 OR 29706585 OR 29713079 OR 29713080 OR 29727680 OR 29727681 OR 29727682 OR 29727683 OR 29731251 OR 29731252 OR 29731253 OR 29754750 OR 29754752 OR 29754754 OR 29754779 OR 29760525 OR 29760527 OR 29772202 OR 29772203 OR 29779889 OR 29779890 OR 29779891 OR 29779941 OR 29779943 OR 29786081 OR 29786082 OR 29786083 OR 29786085 OR 29802388 OR 29802390 OR 29802391 OR 29804889 OR 29804890 OR 29804891 OR 29804919 OR 29804920 OR 29859170 OR 29859171 OR 29861281 OR 29861282 OR 29861283 OR 29861284 OR 29861285 OR 29861286 OR 29867081 OR 29879384 OR 29879392 OR 29887317 OR 29887318 OR 29887338 OR 29887339 OR 29887340 OR 29892048 OR 29909995 OR 29909996 OR 29909997 OR 29909998 OR 29909999 OR 29910000 OR 29910149 OR 29910151 OR 29915192 OR 29915193 OR 29915194 OR 29915195 OR 29937200 OR 29937201 OR 29937202 OR 29937203 OR 29937275 OR 29937276 OR 29937277 OR 29937279 OR 29937281 OR 29942037 OR 29950668 OR 29950669 OR 29950670 OR 29953872 OR 29979986 OR 29979988 OR 29979993 OR 29983322 OR 29983323 OR 29983324 OR 29983325 OR 29983327 OR 29988069 OR 30001507 OR 30001512 OR 30008297 OR 30008298 OR 30013171 OR 30017392 OR 30017393 OR 30017394 OR 30017395 OR 30017396 OR 30017589 OR 30017590 OR 30017591 OR 30033119 OR 30033120 OR 30033151 OR 30033152 OR 30033153 OR 30033154 OR 30038273 OR 30038275 OR 30038276 OR 30038277 OR 30038279 OR 30038280 OR 30038282 OR 30048615 OR 30049452 OR 30050107 OR 30056831 OR 30056832 OR 30057201 OR 30057202 OR 30057203 OR 30057204 OR 30057205 OR 30057206 OR 30075129 OR 30075130 OR 30077356 OR 30078576 OR 30078577 OR 30078578 OR 30078579 OR 30078580 OR 30082067 OR 30082068 OR 30082915 OR 30092214 OR 30092215 OR 30100166 OR 30100167 OR 30100168 OR 30100254 OR 30100255 OR 30100256 OR 30104731 OR 30104732 OR 30104733 OR 30104734 OR 30122373 OR 30122374 OR 30122375 OR 30122377 OR 30122378 OR 30122379 OR 30122380 OR 30122381 OR 30122475 OR 30122476 OR 30127424 OR 30127427 OR 30127430 OR 30138589 OR 30138590 OR 30138591 OR 30146299 OR 30146300 OR 30146301 OR 30146302 OR 30146303 OR 30146304 OR 30146305 OR 30146306 OR 30146307 OR 30146308 OR 30146410 OR 30146411 OR 30146412 OR 30150661 OR 30150662 OR 30150663 OR 30154505 OR 30154506 OR 30174114 OR 30174115 OR 30174116 OR 30174117 OR 30174118 OR 30174119 OR 30174295 OR 30174296 OR 30174297 OR 30177795 OR 30189202 OR 30189209 OR 30197236 OR 30197237 OR 30220509 OR 30220510 OR 30220511 OR 30220512 OR 30220521 OR 30224803 OR 30224804 OR 30224805 OR 30224807 OR 30224808 OR 30224809 OR 30224810 OR 30236284 OR 30236285 OR 30244867 OR 30244869 OR 30244870 OR 30244883 OR 30244884 OR 30244885 OR 30244886 OR 30250263 OR 30258238 OR 30258239 OR 30269902 OR 30269903 OR 30269904 OR 30269986 OR 30269987 OR 30269988 OR 30269989 OR 30269990 OR 30269991 OR 30269992 OR 30269993 OR 30290177 OR 30290178 OR 30290179 OR 30290982 OR 30293821 OR 30293822 OR 30293823 OR 30297807 OR 30308165 OR 30308166 OR 30308173 OR 30318302 OR 30318303 OR 30318409 OR 30318410 OR 30318411 OR 30318412 OR 30318413 OR 30318414 OR 30318415 OR 30318416 OR 30323275 OR 30323276 OR 30344040 OR 30344041 OR 30344042 OR 30344043 OR 30344044 OR 30344045 OR 30344046 OR 30344047 OR 30344048 OR 30344100 OR 30349100 OR 30349101 OR 30349103 OR 30349104 OR 30349105 OR 30349106 OR 30349107 OR 30349110 OR 30349111 OR 30361547 OR 30382196 OR 30392793 OR 30392794 OR 30392795 OR 30392796 OR 30392797 OR 30392798 OR 30392799 OR 30392800 OR 30397325 OR 30401455 OR 30408443 OR 30408444 OR 30415993 OR 30415995 OR 30415996 OR 30415998 OR 30416070 OR 30416071 OR 30416072 OR 30420732 OR 30449656 OR 30449657 OR 30449714 OR 30449715 OR 30455454 OR 30455455 OR 30455456 OR 30455457 OR 30455458 OR 30465766 OR 30467079 OR 30467080 OR 30472076 OR 30472077 OR 30472156 OR 30472157 OR 30472158 OR 30473013 OR 30473014 OR 30482688 OR 30482689 OR 30482690 OR 30482691 OR 30482692 OR 30482693 OR 30482694 OR 30482945 OR 30482946 OR 30482947 OR 30482948 OR 30482949 OR 30497771 OR 30497772 OR 30502044 OR 30503141 OR 30503142 OR 30503143 OR 30503172 OR 30503173 OR 30503644 OR 30503645 OR 30521777 OR 30521779 OR 30522820 OR 30526881 OR 30526882 OR 30528064 OR 30528065 OR 30528555 OR 30545599 OR 30551997 OR 30551998 OR 30553546 OR 30554781 OR 30554961 OR 30554962 OR 30554964 OR 30559469 OR 30559470 OR 30559471 OR 30559472 OR 30559475 OR 30559476 OR 30559478 OR 30559479 OR 30559480 OR 30573346 OR 30578106 OR 30581011 OR 30581012 OR 30581079 OR 30581080 OR 30594427 OR 30595332 OR 30595499 OR 30598527 OR 30606613 OR 30606614 OR 30609396 OR 30617257 OR 30617258 OR 30635232 OR 30638744 OR 30638745 OR 30638901 OR 30638902 OR 30639035 OR 30639036 OR 30639037 OR 30643291 OR 30643292 OR 30643294 OR 30643295 OR 30643296 OR 30643297 OR 30643298 OR 30643299 OR 30653935 OR 30654923 OR 30654924 OR 30658859 OR 30658860 OR 30661738 OR 30661739 OR 30661958 OR 30661959 OR 30661960 OR 30664766 OR 30664767 OR 30664768 OR 30664769 OR 30664770 OR 30664771 OR 30664772 OR 30679017 OR 30679018 OR 30683545 OR 30683546 OR 30685224 OR 30686732 OR 30686733 OR 30686763 OR 30686764 OR 30686765 OR 30692687 OR 30692688 OR 30692689 OR 30692690 OR 30692691 OR 30704910 OR 30704911 OR 30709656 OR 30711355 OR 30713093 OR 30713094 OR 30718900 OR 30718902 OR 30718903)</t>
+  </si>
+  <si>
+    <t>PMID=(30718904 OR 30731062 OR 30733148 OR 30733149 OR 30733150 OR 30737130 OR 30742114 OR 30742115 OR 30742116 OR 30742117 OR 30744986 OR 30744987 OR 30765165 OR 30765166 OR 30770252 OR 30770301 OR 30778148 OR 30778149 OR 30792150 OR 30795900 OR 30795902 OR 30799020 OR 30799021 OR 30799279 OR 30804529 OR 30804530 OR 30819547 OR 30824353 OR 30833699 OR 30833700 OR 30846309 OR 30849366 OR 30849367 OR 30850257 OR 30853298 OR 30853299 OR 30853300 OR 30853556 OR 30853557 OR 30853558 OR 30858601 OR 30858603 OR 30858604 OR 30858605 OR 30871858 OR 30871859 OR 30876848 OR 30876849 OR 30878289 OR 30879785 OR 30880024 OR 30880025 OR 30880026 OR 30886406 OR 30886407 OR 30886408 OR 30902550 OR 30905618 OR 30905619 OR 30905620 OR 30911182 OR 30911183 OR 30911184 OR 30911185 OR 30926280 OR 30928170 OR 30930044 OR 30930145 OR 30930146 OR 30930147 OR 30936555 OR 30936556 OR 30936557 OR 30936558 OR 30951662 OR 30962628 OR 30962630 OR 30962632 OR 30979537 OR 30981533 OR 30982627 OR 30982770 OR 30982771 OR 30988523 OR 30988524 OR 30988525 OR 30988526 OR 30988527 OR 31003725 OR 31005376 OR 31006620 OR 31006621 OR 31006622 OR 31011224 OR 31011226 OR 31011227 OR 31023509 OR 31027966 OR 31029403 OR 31030955 OR 31031137 OR 31031138 OR 31031139 OR 31036941 OR 31036942 OR 31036944 OR 31036945 OR 31036947 OR 31047778 OR 31047779 OR 31051134 OR 31054873 OR 31056352 OR 31056353 OR 31061493 OR 31061494 OR 31072787 OR 31076274 OR 31078368 OR 31079872 OR 31080134 OR 31080135 OR 31080136 OR 31086314 OR 31086315 OR 31086316 OR 31097360 OR 31097361 OR 31101394 OR 31101395 OR 31103358 OR 31104942 OR 31104943 OR 31104950 OR 31104951 OR 31110321 OR 31110323 OR 31110324 OR 31121123 OR 31122676 OR 31122677 OR 31127258 OR 31127260 OR 31130330 OR 31130512 OR 31130513 OR 31130514 OR 31133689 OR 31147152 OR 31147153 OR 31151773 OR 31151774 OR 31153646 OR 31153647 OR 31155482 OR 31155483 OR 31155484 OR 31160741 OR 31171447 OR 31171448 OR 31173711 OR 31173712 OR 31173713 OR 31173715 OR 31173718 OR 31174959 OR 31174960 OR 31178114 OR 31178115 OR 31178255 OR 31182866 OR 31182867 OR 31182869 OR 31196672 OR 31196673 OR 31201122 OR 31201123 OR 31202541 OR 31204082 OR 31204176 OR 31204177 OR 31209376 OR 31209378 OR 31209379 OR 31209380 OR 31209381 OR 31221559 OR 31221560 OR 31227309 OR 31227310 OR 31230761 OR 31230859 OR 31230860 OR 31235906 OR 31235907 OR 31235908 OR 31235930 OR 31235931 OR 31235932 OR 31235933 OR 31248728 OR 31253468 OR 31253469 OR 31255486 OR 31257105 OR 31263205 OR 31271748 OR 31271750 OR 31272828 OR 31272829 OR 31277924 OR 31279774 OR 31280924 OR 31285612 OR 31285613 OR 31285614 OR 31285615 OR 31285616 OR 31296412 OR 31300277 OR 31301936 OR 31303374 OR 31303547 OR 31303548 OR 31303549 OR 31308530 OR 31319048 OR 31324538 OR 31327663 OR 31327664 OR 31332371 OR 31332372 OR 31332373 OR 31332375 OR 31345643 OR 31346295 OR 31346296 OR 31350097 OR 31351757 OR 31353074 OR 31358989 OR 31358990 OR 31358991 OR 31358992 OR 31371111 OR 31374198 OR 31374199 OR 31376984 OR 31384015 OR 31395429 OR 31399280 OR 31406364 OR 31406365 OR 31406366 OR 31416668 OR 31420117 OR 31422912 OR 31422913 OR 31427770 OR 31427771 OR 31439429 OR 31447169 OR 31451801 OR 31451803 OR 31455879 OR 31455884 OR 31455886 OR 31455887 OR 31466734 OR 31471123 OR 31473062 OR 31474560 OR 31477898 OR 31488328 OR 31491396 OR 31492534 OR 31493975 OR 31495645 OR 31495646 OR 31495780 OR 31495781 OR 31495782 OR 31501571 OR 31501572 OR 31501573 OR 31515109 OR 31521441 OR 31522764 OR 31523027 OR 31523028 OR 31527803 OR 31542321 OR 31543297 OR 31543366 OR 31543367 OR 31548723 OR 31551592 OR 31551593 OR 31551596 OR 31551598 OR 31551599 OR 31551601 OR 31551603 OR 31551604 OR 31558350 OR 31561919 OR 31563294 OR 31564548 OR 31564549 OR 31564591 OR 31564592 OR 31570859 OR 31570865 OR 31582313 OR 31585093 OR 31585094 OR 31585809 OR 31586516 OR 31587918 OR 31587919 OR 31588046 OR 31588047 OR 31591558 OR 31591559 OR 31591560 OR 31591561 OR 31601510 OR 31604597 OR 31606247 OR 31606248 OR 31607423 OR 31611705 OR 31611706 OR 31611707 OR 31611708 OR 31623918 OR 31623919 OR 31627985 OR 31629603 OR 31630908 OR 31631012 OR 31631013 OR 31636447 OR 31636448 OR 31636449 OR 31636451 OR 31648898 OR 31648899 OR 31648900 OR 31653463 OR 31659341 OR 31659342 OR 31668484 OR 31668485 OR 31668844 OR 31672263 OR 31676170 OR 31677957 OR 31679900 OR 31686023 OR 31704028 OR 31706697 OR 31708306 OR 31708402 OR 31712775 OR 31719672 OR 31727548 OR 31727549 OR 31732258 OR 31733940 OR 31735403 OR 31740813 OR 31740814 OR 31753579 OR 31753580 OR 31757603 OR 31757604 OR 31759806 OR 31759807 OR 31759808 OR 31761708 OR 31761709 OR 31761710 OR 31761722 OR 31761723 OR 31761724 OR 31768050 OR 31768051 OR 31768052 OR 31768054 OR 31768056 OR 31768057 OR 31780328 OR 31780329 OR 31780330 OR 31784285 OR 31784286 OR 31784287 OR 31784288 OR 31786011 OR 31786012 OR 31786013 OR 31786014 OR 31786016 OR 31792463 OR 31792464 OR 31792465 OR 31792466 OR 31792467 OR 31806491 OR 31806492 OR 31806493 OR 31809737 OR 31809738 OR 31809739 OR 31809740 OR 31810837 OR 31810838 OR 31810839 OR 31812514 OR 31812515 OR 31812516 OR 31813651 OR 31813652 OR 31813653 OR 31831331 OR 31831332 OR 31836321 OR 31836322 OR 31837915 OR 31839569 OR 31839570 OR 31844311 OR 31844313 OR 31844314 OR 31844315 OR 31844317 OR 31859030 OR 31859031 OR 31862210 OR 31864947 OR 31866091 OR 31866222 OR 31866223 OR 31866224 OR 31873194 OR 31873285 OR 31873286 OR 31879163 OR 31883788)</t>
+  </si>
+  <si>
+    <t>PMID=(31883789 OR 31883834 OR 31883835 OR 31899071 OR 31899072 OR 31901251 OR 31901304 OR 31902528 OR 31907436 OR 31907437 OR 31907438 OR 31907439 OR 31924446 OR 31926610 OR 31928842 OR 31928944 OR 31932764 OR 31932766 OR 31932767 OR 31932769 OR 31932770 OR 31948733 OR 31948734 OR 31952856 OR 31954621 OR 31955944 OR 31956038 OR 31956039 OR 31956040 OR 31959933 OR 31959934 OR 31959935 OR 31959936 OR 31959937 OR 31972144 OR 31974009 OR 31978363 OR 31978364 OR 31978365 OR 31980319 OR 31982322 OR 31983538 OR 31995730 OR 32001108 OR 32004439 OR 32004478 OR 32004479 OR 32015540 OR 32023429 OR 32027824 OR 32027825 OR 32032525 OR 32032526 OR 32042174 OR 32042175 OR 32042176 OR 32048996 OR 32053769 OR 32059759 OR 32059806 OR 32059807 OR 32059808 OR 32066981 OR 32066983 OR 32066984 OR 32066985 OR 32066986 OR 32066987 OR 32070475 OR 32075716 OR 32078800 OR 32084331 OR 32084388 OR 32084389 OR 32084390 OR 32094970 OR 32097629 OR 32097630 OR 32101698 OR 32105611 OR 32109363 OR 32109376 OR 32109377 OR 32109378 OR 32112058 OR 32112061 OR 32123378 OR 32126198 OR 32130872 OR 32135084 OR 32142646 OR 32142647 OR 32142648 OR 32142663 OR 32142681 OR 32142682 OR 32142683 OR 32145183 OR 32145184 OR 32152537 OR 32155441 OR 32155442 OR 32160515 OR 32164873 OR 32164874 OR 32164875 OR 32169166 OR 32169167 OR 32169170 OR 32169171 OR 32171388 OR 32183943 OR 32187528 OR 32191871 OR 32197063 OR 32197066 OR 32199103 OR 32199104 OR 32203495 OR 32203496 OR 32203497 OR 32203499 OR 32208171 OR 32209430 OR 32213321 OR 32220666 OR 32229307 OR 32229310 OR 32229311 OR 32231338 OR 32231340 OR 32240599 OR 32243780 OR 32243781 OR 32243809 OR 32251386 OR 32259476 OR 32259481 OR 32272058 OR 32272064 OR 32275860 OR 32284604 OR 32284605 OR 32284606 OR 32284607 OR 32284608 OR 32289250 OR 32294466 OR 32302522 OR 32302523 OR 32302532 OR 32304628 OR 32313267 OR 32315603 OR 32320644 OR 32320679 OR 32325031 OR 32330411 OR 32333845 OR 32341540 OR 32341541 OR 32341542 OR 32343945 OR 32348717 OR 32348727 OR 32348728 OR 32353253 OR 32359400 OR 32362337 OR 32367065 OR 32369733 OR 32375063 OR 32375064 OR 32380032 OR 32386524 OR 32386552 OR 32386554 OR 32386572 OR 32392471 OR 32392472 OR 32393895 OR 32393896 OR 32396852 OR 32396862 OR 32396863 OR 32396864 OR 32402250 OR 32402251 OR 32407670 OR 32413331 OR 32413332 OR 32416059 OR 32424284 OR 32424285 OR 32424286 OR 32424287 OR 32428433 OR 32433908 OR 32442395 OR 32442399 OR 32445624 OR 32451482 OR 32451483 OR 32451484 OR 32451485 OR 32451487 OR 32459995 OR 32459996 OR 32464095 OR 32464096 OR 32473094 OR 32483349 OR 32485136 OR 32492366 OR 32514135 OR 32514136 OR 32514137 OR 32514138 OR 32514139 OR 32516567 OR 32516573 OR 32521223 OR 32526196 OR 32526197 OR 32531207 OR 32533915 OR 32541962 OR 32541964 OR 32544386 OR 32553204 OR 32559415 OR 32559418 OR 32562661 OR 32562662 OR 32572235 OR 32572236 OR 32572237 OR 32574559 OR 32579880 OR 32589864 OR 32589877 OR 32589878 OR 32592656 OR 32603655 OR 32610039 OR 32610040 OR 32615067 OR 32616470 OR 32619510 OR 32619511 OR 32619517 OR 32619518 OR 32632286 OR 32632287 OR 32640183 OR 32640191 OR 32645299 OR 32649865 OR 32661394 OR 32661395 OR 32661396 OR 32663438 OR 32673563 OR 32673568 OR 32673569 OR 32679036 OR 32681824 OR 32681825 OR 32690967 OR 32690968 OR 32690969 OR 32693086 OR 32693087 OR 32697942 OR 32697949 OR 32702287 OR 32707082 OR 32707083 OR 32710818 OR 32710819 OR 32719561 OR 32719562 OR 32719563 OR 32721381 OR 32730753 OR 32735778 OR 32735781 OR 32747787 OR 32747789 OR 32747790 OR 32750316 OR 32755548 OR 32758424 OR 32758425 OR 32758426 OR 32763144 OR 32763145 OR 32763182 OR 32778789 OR 32778791 OR 32778793 OR 32778794 OR 32783881 OR 32783882 OR 32783885 OR 32783886 OR 32791039 OR 32795399 OR 32795400 OR 32807948 OR 32807949 OR 32807950 OR 32810432 OR 32810433 OR 32810435 OR 32814018 OR 32818433 OR 32822582 OR 32822583 OR 32822613 OR 32839618 OR 32841590 OR 32846139 OR 32846140 OR 32853550 OR 32853551 OR 32868932 OR 32877641 OR 32888408 OR 32888424 OR 32888425 OR 32891188 OR 32891189 OR 32895565 OR 32895566 OR 32895567 OR 32905785 OR 32910893 OR 32910894 OR 32916090 OR 32916091 OR 32929244 OR 32929245 OR 32931729 OR 32931730 OR 32931754 OR 32931755 OR 32937099 OR 32946744 OR 32946745 OR 32946788 OR 32949502 OR 32961128 OR 32961129 OR 32961143 OR 32966764 OR 32966778 OR 32970991 OR 32976770 OR 32979312 OR 32979316 OR 32989293 OR 32989294 OR 32989295 OR 32991831 OR 32991838 OR 32997960 OR 33002411 OR 33007236 OR 33010822 OR 33020652 OR 33020653 OR 33020654 OR 33022226 OR 33022227 OR 33022228 OR 33027639 OR 33027640 OR 33049200 OR 33049201 OR 33049217 OR 33053374 OR 33068531 OR 33068532 OR 33077946 OR 33077947 OR 33077948 OR 33080226 OR 33080227 OR 33080228 OR 33080229 OR 33080230 OR 33086034 OR 33086038 OR 33086039 OR 33091338 OR 33091339 OR 33091368 OR 33096025 OR 33097921 OR 33098762 OR 33098807 OR 33108748 OR 33113347 OR 33113348 OR 33125872 OR 33125873 OR 33128895 OR 33139942 OR 33142113 OR 33142114 OR 33147442 OR 33147489 OR 33152265 OR 33152266 OR 33157003 OR 33159842 OR 33169029 OR 33169031 OR 33171117 OR 33176168 OR 33181065 OR 33181066 OR 33181078 OR 33186546 OR 33188733 OR 33199896 OR 33199898 OR 33202244 OR 33207217 OR 33207218 OR 33212012 OR 33217323 OR 33217328 OR 33220177 OR 33230320 OR 33230321 OR 33230322 OR 33230328 OR 33230329 OR 33232655 OR 33232662 OR 33232663 OR 33238137 OR 33242413 OR 33242421 OR 33242422 OR 33248017 OR 33257875 OR 33257876)</t>
+  </si>
+  <si>
+    <t>PMID=(33259798 OR 33259804 OR 33264592 OR 33264636 OR 33271069 OR 33271070 OR 33275875 OR 33275898 OR 33278341 OR 33278342 OR 33288907 OR 33288908 OR 33288909 OR 33288910 OR 33290731 OR 33290732 OR 33296670 OR 33301706 OR 33301712 OR 33318667 OR 33321071 OR 33321072 OR 33321074 OR 33326754 OR 33326755 OR 33328624 OR 33333001 OR 33338395 OR 33340448 OR 33340451 OR 33349709 OR 33349710 OR 33349711 OR 33349712 OR 33352111 OR 33352118 OR 33353966 OR 33357383 OR 33357384 OR 33357385 OR 33357405 OR 33357412 OR 33357413 OR 33357417 OR 33361822 OR 33373620 OR 33378647 OR 33406410 OR 33412101 OR 33417867 OR 33417871 OR 33432193 OR 33432194 OR 33432195 OR 33432196 OR 33450185 OR 33450186 OR 33450187 OR 33453151 OR 33462481 OR 33472037 OR 33472038 OR 33476548 OR 33476575 OR 33482086 OR 33482087 OR 33484641 OR 33495635 OR 33495636 OR 33495637 OR 33497602 OR 33503410 OR 33508244 OR 33510480 OR 33513358 OR 33513363 OR 33526922 OR 33526942 OR 33529599 OR 33529646 OR 33535028 OR 33539722 OR 33539723 OR 33539763 OR 33542524 OR 33545077 OR 33545078 OR 33545080 OR 33545081 OR 33548174 OR 33558694 OR 33558695 OR 33561398 OR 33561399 OR 33561425 OR 33567253 OR 33567267 OR 33571444 OR 33571445 OR 33577748 OR 33581058 OR 33589832 OR 33589833 OR 33589834 OR 33600762 OR 33600763 OR 33603228 OR 33603230 OR 33603231 OR 33606969 OR 33609440 OR 33609483 OR 33619403 OR 33619404 OR 33619405 OR 33621485 OR 33621486 OR 33626322 OR 33626327 OR 33631115 OR 33631116 OR 33631117 OR 33651975 OR 33657412 OR 33657413 OR 33667342 OR 33667343 OR 33667356 OR 33667358 OR 33675684 OR 33675685 OR 33675690 OR 33686297 OR 33686298 OR 33686299 OR 33707754 OR 33711258 OR 33711282 OR 33711283 OR 33723433 OR 33723434 OR 33723435 OR 33730554 OR 33730555 OR 33737752 OR 33740416 OR 33740417 OR 33743191 OR 33753944 OR 33753945 OR 33756103 OR 33756104 OR 33765445 OR 33770504 OR 33770505 OR 33782620 OR 33782621 OR 33782622 OR 33782623 OR 33784497 OR 33784498 OR 33789082 OR 33789083 OR 33795883 OR 33795885 OR 33798407 OR 33798421 OR 33820999 OR 33821000 OR 33821001 OR 33823137 OR 33823138 OR 33823144 OR 33826906 OR 33831348 OR 33831349 OR 33831364 OR 33831365 OR 33831366 OR 33838105 OR 33846625 OR 33846626 OR 33848469 OR 33848470 OR 33848471 OR 33848472 OR 33848473 OR 33848474 OR 33852896 OR 33852917 OR 33859437 OR 33859438 OR 33861941 OR 33861942 OR 33875891 OR 33875892 OR 33875893 OR 33878295 OR 33882290 OR 33882291 OR 33887179 OR 33887199 OR 33894142 OR 33903770 OR 33910058 OR 33915078 OR 33915079 OR 33915080 OR 33915081 OR 33915110 OR 33927400 OR 33930307 OR 33945793 OR 33945794 OR 33951478 OR 33951479 OR 33957065 OR 33957072 OR 33957073 OR 33957080 OR 33957081 OR 33958804 OR 33961761 OR 33961762 OR 33961763 OR 33961764 OR 33961765 OR 33961766 OR 33961767 OR 33961768 OR 33961804 OR 33972801 OR 33972802 OR 33974915 OR 33979633 OR 33979634 OR 33979635 OR 33984282 OR 33984283 OR 33986549 OR 33986551 OR 33991504 OR 34002087 OR 34004179 OR 34010627 OR 34010628 OR 34015253 OR 34017129 OR 34017130 OR 34017131 OR 34019810 OR 34022129 OR 34031600 OR 34033742 OR 34038708 OR 34038743 OR 34048697 OR 34051145 OR 34059832 OR 34077741 OR 34077742 OR 34081911 OR 34083786 OR 34083787 OR 34089643 OR 34099922 OR 34102111 OR 34102139 OR 34118190 OR 34129813 OR 34133944 OR 34133945 OR 34139149 OR 34140698 OR 34146468 OR 34146469 OR 34157306 OR 34166604 OR 34168338 OR 34168339 OR 34168340 OR 34171289 OR 34171290 OR 34171291 OR 34183865 OR 34183866 OR 34183867 OR 34183869 OR 34186026 OR 34186027 OR 34197732 OR 34197733 OR 34228959 OR 34228960 OR 34233151 OR 34239128 OR 34239129 OR 34242565 OR 34245686 OR 34253921 OR 34253922 OR 34265252 OR 34265253 OR 34267392 OR 34293291 OR 34293292 OR 34293295 OR 34293334 OR 34294918 OR 34294919 OR 34297916 OR 34314698 OR 34320411 OR 34341584 OR 34341585 OR 34341586 OR 34343491 OR 34343492 OR 34352213 OR 34352214 OR 34354282 OR 34358441 OR 34363751 OR 34363753 OR 34373644 OR 34380016 OR 34381241 OR 34384519 OR 34385700 OR 34388375 OR 34390650 OR 34390651 OR 34390652 OR 34400844 OR 34407389 OR 34407390 OR 34407456 OR 34411513 OR 34411514 OR 34413511 OR 34413512 OR 34413513 OR 34413514 OR 34413515 OR 34416169 OR 34426698 OR 34437845 OR 34450025 OR 34450026 OR 34450065 OR 34465915 OR 34469773 OR 34473944 OR 34473945 OR 34473953 OR 34473954 OR 34478630 OR 34478631 OR 34478642 OR 34480863 OR 34480866 OR 34496297 OR 34496298 OR 34499856 OR 34499868 OR 34506723 OR 34506724 OR 34506725 OR 34508666 OR 34508667 OR 34525346 OR 34525347 OR 34525348 OR 34529935 OR 34534453 OR 34534454 OR 34534455 OR 34534456 OR 34536352 OR 34536353 OR 34536354 OR 34545249 OR 34551362 OR 34555313 OR 34555314 OR 34555316 OR 34559981 OR 34582785 OR 34582804 OR 34592167 OR 34592168 OR 34608335 OR 34614419 OR 34614420 OR 34614421 OR 34619088 OR 34619093 OR 34624205 OR 34624206 OR 34624220 OR 34626537 OR 34637706 OR 34644545 OR 34644546 OR 34648750 OR 34655526 OR 34663956 OR 34663957 OR 34663958 OR 34663959 OR 34665999 OR 34672984 OR 34672985 OR 34675436 OR 34675437 OR 34678146 OR 34678147 OR 34678169 OR 34687663 OR 34687664 OR 34687665 OR 34697455 OR 34699777 OR 34699778 OR 34706218 OR 34706219 OR 34706220 OR 34706221 OR 34706256 OR 34710366 OR 34711960 OR 34711961 OR 34715026 OR 34717794 OR 34727519 OR 34727520 OR 34735779 OR 34737447 OR 34737448 OR 34739817 OR 34741806 OR 34752775 OR 34762860 OR 34764474 OR 34767769 OR 34767770 OR 34776042 OR 34782793 OR 34782794 OR 34788632)</t>
+  </si>
+  <si>
+    <t>PMID=(34793692 OR 34793693 OR 34793694 OR 34793707 OR 34795450 OR 34795451 OR 34798047 OR 34811521 OR 34847364 OR 34852235 OR 34856120 OR 34856121 OR 34857949 OR 34857950 OR 34861147 OR 34861149 OR 34861150 OR 34863366 OR 34863367 OR 34875233 OR 34879244 OR 34887588 OR 34887590 OR 34890566 OR 34903880 OR 34914919 OR 34916658 OR 34921780 OR 34921781 OR 34921782 OR 34931070 OR 34932940 OR 34932941 OR 34932942 OR 34932943 OR 34936886 OR 34942116 OR 34965381 OR 34980924 OR 34980925 OR 34982958 OR 34986325 OR 34990571 OR 34990576 OR 34990580 OR 34995486 OR 34995493 OR 34998469 OR 35027761 OR 35032430 OR 35041805 OR 35045331 OR 35045337 OR 35045338 OR 35045339 OR 35051374 OR 35051376 OR 35051377 OR 35065706 OR 35065714 OR 35065715 OR 35077667 OR 35085492 OR 35087246 OR 35090595 OR 35093191 OR 35102333 OR 35104442 OR 35104451 OR 35108498 OR 35108519 OR 35114101 OR 35114102 OR 35115729 OR 35115730 OR 35115731 OR 35120626 OR 35120627 OR 35120628 OR 35123654 OR 35123655 OR 35132236 OR 35139362 OR 35139363 OR 35139364 OR 35139365 OR 35143752 OR 35143761 OR 35165460 OR 35176221 OR 35176222 OR 35176223 OR 35180389 OR 35180390 OR 35180391 OR 35180398 OR 35210624 OR 35216662 OR 35216671 OR 35228700 OR 35241802 OR 35241804 OR 35245443 OR 35260862 OR 35260863 OR 35260864 OR 35260865 OR 35263617 OR 35263618 OR 35276083 OR 35276096 OR 35278361 OR 35278369 OR 35278370 OR 35288716 OR 35290791 OR 35290792 OR 35294899 OR 35294900 OR 35294901 OR 35301477 OR 35314823 OR 35325615 OR 35349784 OR 35349785 OR 35354062 OR 35358415 OR 35361972 OR 35361973 OR 35361974 OR 35364013 OR 35364014 OR 35379994 OR 35379995 OR 35381188 OR 35381189 OR 35383330 OR 35383331 OR 35383332 OR 35385698 OR 35390278 OR 35395180 OR 35395185 OR 35395187 OR 35395188 OR 35397211 OR 35413242 OR 35421327 OR 35421328 OR 35439430 OR 35443152 OR 35443153 OR 35443154 OR 35447088 OR 35447099 OR 35452598 OR 35452606 OR 35484406 OR 35489331 OR 35501379 OR 35501380 OR 35501382 OR 35501383 OR 35508174 OR 35508177 OR 35513515 OR 35513516 OR 35523139 OR 35523140 OR 35523141 OR 35523142 OR 35523143 OR 35524134 OR 35524136 OR 35524138 OR 35524139 OR 35524140 OR 35524141 OR 35525241 OR 35525242 OR 35525243 OR 35545090 OR 35550065 OR 35550066 OR 35561675 OR 35561677 OR 35578131 OR 35578132 OR 35584693 OR 35590075 OR 35597234 OR 35606419 OR 35606420 OR 35609615 OR 35613618 OR 35613619 OR 35618950 OR 35637368 OR 35637370 OR 35637371 OR 35637373 OR 35643078 OR 35649415 OR 35654036 OR 35654037 OR 35654956 OR 35654957 OR 35659876 OR 35659877 OR 35659878 OR 35659879 OR 35668173 OR 35668174 OR 35672490 OR 35672491 OR 35672492 OR 35679860 OR 35679861 OR 35690063 OR 35700735 OR 35700736 OR 35700737 OR 35705078 OR 35710983 OR 35710984 OR 35714610 OR 35726057 OR 35726058 OR 35726059 OR 35728595 OR 35728596 OR 35739273 OR 35750858 OR 35760863 OR 35760864 OR 35767994 OR 35767995 OR 35773543 OR 35773544 OR 35790859 OR 35790861 OR 35798979 OR 35798980 OR 35803225 OR 35803226 OR 35803227 OR 35803228 OR 35803229 OR 35803230 OR 35803269 OR 35803270 OR 35809573 OR 35809574 OR 35817847 OR 35856095 OR 35858618 OR 35858622 OR 35858623 OR 35879464 OR 35882228 OR 35896109 OR 35902648 OR 35915173 OR 35915174 OR 35915176 OR 35915177 OR 35915179 OR 35915180 OR 35917818 OR 35921846 OR 35931029 OR 35931030 OR 35931031 OR 35931032 OR 35931033 OR 35931034 OR 35931070 OR 35944526 OR 35952672 OR 35953545 OR 35961319 OR 35961320 OR 35963237 OR 35963238 OR 35982153 OR 35982154 OR 35987206 OR 35987207 OR 35995877 OR 35995878 OR 35998631 OR 35998632 OR 35998641 OR 35998642 OR 36002022 OR 36007521 OR 36041433 OR 36042306 OR 36042308 OR 36042309 OR 36042310 OR 36042311 OR 36042312 OR 36042313 OR 36042314 OR 36055191 OR 36055192 OR 36055193 OR 36055194 OR 36070748 OR 36070749 OR 36070750 OR 36070751 OR 36084654 OR 36084657 OR 36087581 OR 36087582 OR 36087583 OR 36087584 OR 36087585 OR 36099920 OR 36113462 OR 36113472 OR 36130594 OR 36130595 OR 36137550 OR 36150394 OR 36163283 OR 36170850 OR 36171426 OR 36171427 OR 36171428 OR 36171429 OR 36171430 OR 36171431 OR 36174572 OR 36175793 OR 36180790 OR 36180791 OR 36206730 OR 36206731 OR 36206732 OR 36206758 OR 36216998 OR 36216999 OR 36220098 OR 36240768 OR 36240770 OR 36243003 OR 36265442 OR 36265493 OR 36266470 OR 36266471 OR 36272401 OR 36280797 OR 36280798 OR 36303068 OR 36303069 OR 36303070 OR 36303071 OR 36319770 OR 36319771 OR 36327889 OR 36327892 OR 36327893 OR 36332570 OR 36332571 OR 36332572 OR 36344699 OR 36357811 OR 36376483 OR 36384141 OR 36396976 OR 36396977 OR 36424430 OR 36424431 OR 36424432 OR 36443609 OR 36443610 OR 36446381 OR 36446933 OR 36446934 OR 36459961 OR 36459962 OR 36459963 OR 36459965 OR 36459967 OR 36459968 OR 36459969 OR 36459970)</t>
   </si>
 </sst>
 </file>
@@ -67,7 +145,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B29"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -94,6 +172,214 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>